<commit_message>
Updated function distributing rewards with 2 variables (tokens and fees)
</commit_message>
<xml_diff>
--- a/20210921 - Staking Rewards.xlsx
+++ b/20210921 - Staking Rewards.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Documents\16slimchance16\token\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DCA4180-3F72-42D5-9E6C-41A2CAB370FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16455B87-3B48-4925-A208-F325ABB3D7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-90" windowWidth="16530" windowHeight="10980" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="840" yWindow="-90" windowWidth="16530" windowHeight="10980" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SNX" sheetId="1" r:id="rId1"/>
-    <sheet name="Rewards Score" sheetId="2" r:id="rId2"/>
-    <sheet name="KWENTA" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="SNX - Detail" sheetId="4" r:id="rId2"/>
+    <sheet name="Rewards Score" sheetId="2" r:id="rId3"/>
+    <sheet name="KWENTA" sheetId="3" r:id="rId4"/>
+    <sheet name="KWENTA - v2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="61">
   <si>
     <t>N stake 20</t>
   </si>
@@ -208,18 +209,33 @@
   </si>
   <si>
     <t>Notify (120)</t>
+  </si>
+  <si>
+    <t>rewardTokens</t>
+  </si>
+  <si>
+    <t>rewardFees</t>
+  </si>
+  <si>
+    <t>Token</t>
+  </si>
+  <si>
+    <t>Fee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
-    <numFmt numFmtId="165" formatCode="0.0000000"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="175" formatCode="0.0000000000000"/>
-    <numFmt numFmtId="191" formatCode="0.0000000%"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="8">
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="168" formatCode="0.0000000%"/>
+    <numFmt numFmtId="173" formatCode="0.0000000E+00"/>
+    <numFmt numFmtId="190" formatCode="#,##0.000000000000000000"/>
+    <numFmt numFmtId="191" formatCode="#,##0.0000000000000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -287,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -302,11 +318,14 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -621,7 +640,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -912,7 +931,438 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:O16"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2">
+        <v>8</v>
+      </c>
+      <c r="K2" s="2">
+        <v>9</v>
+      </c>
+      <c r="L2" s="2">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2">
+        <v>12</v>
+      </c>
+      <c r="O2" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>10</v>
+      </c>
+      <c r="N3">
+        <v>10</v>
+      </c>
+      <c r="O3">
+        <f>+N3</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f>+E5+4*F3/E10</f>
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <f>+F5</f>
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <f>+G5</f>
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <f>+H5</f>
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f>+I5</f>
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <f>+J5</f>
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <f>+K5+(L2-K4)*L3/K10</f>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="M5">
+        <f>+L5</f>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="N5">
+        <f>+M5+(N2-M4)*N3/M10</f>
+        <v>3.1428571428571428</v>
+      </c>
+      <c r="O5">
+        <f>+N5</f>
+        <v>3.1428571428571428</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f>+F5</f>
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:L8" si="0">+F7</f>
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <f>+N5</f>
+        <v>3.1428571428571428</v>
+      </c>
+      <c r="O7">
+        <f>+N7</f>
+        <v>3.1428571428571428</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f>+E10*(N5-E7)</f>
+        <v>62.857142857142854</v>
+      </c>
+      <c r="O8">
+        <f>+F11*(O5-F7)</f>
+        <v>457.14285714285711</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>420</v>
+      </c>
+      <c r="G10">
+        <v>420</v>
+      </c>
+      <c r="H10">
+        <v>420</v>
+      </c>
+      <c r="I10">
+        <v>420</v>
+      </c>
+      <c r="J10">
+        <v>420</v>
+      </c>
+      <c r="K10">
+        <v>420</v>
+      </c>
+      <c r="L10">
+        <v>20</v>
+      </c>
+      <c r="M10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>400</v>
+      </c>
+      <c r="N11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="C14">
+        <v>40</v>
+      </c>
+      <c r="K14">
+        <f>60*400/420</f>
+        <v>57.142857142857146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="C15">
+        <v>2.8</v>
+      </c>
+      <c r="G15">
+        <f>60/420*20</f>
+        <v>2.8571428571428568</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="C16">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1130,12 +1580,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1891,430 +2341,556 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O16"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DC2E69-E67B-45D9-BD33-D97282242B36}">
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="23.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.40625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.2265625" customWidth="1"/>
+    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.76953125" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.453125" customWidth="1"/>
+    <col min="12" max="12" width="23.90625" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+    <row r="1" spans="1:12" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="E1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>300</v>
+      </c>
+      <c r="F2">
+        <v>300</v>
+      </c>
+      <c r="G2">
+        <f>+E2/F2</f>
         <v>1</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2">
-        <v>5</v>
-      </c>
-      <c r="H2" s="2">
+      <c r="H2">
+        <f>+G2*0.7</f>
+        <v>0.7</v>
+      </c>
+      <c r="I2">
+        <f>+G2*0.3</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="18">
+        <v>2.5E+19</v>
+      </c>
+      <c r="H6">
+        <f>+G6*70%</f>
+        <v>1.7499999999999998E+19</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="9">
+        <f>+$I$2*G6/SUM($G$6:$G$7)*60</f>
         <v>6</v>
       </c>
-      <c r="I2" s="2">
-        <v>7</v>
-      </c>
-      <c r="J2" s="2">
-        <v>8</v>
-      </c>
-      <c r="K2" s="2">
-        <v>9</v>
-      </c>
-      <c r="L2" s="2">
-        <v>10</v>
-      </c>
-      <c r="M2" s="2">
-        <v>11</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="K6" s="9">
+        <f>+J6+I6</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="18">
+        <v>5E+19</v>
+      </c>
+      <c r="H7">
+        <f>+G7*70%</f>
+        <v>3.4999999999999996E+19</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="9">
+        <f>+$I$2*G7/SUM($G$6:$G$7)*60</f>
         <v>12</v>
       </c>
-      <c r="O2" s="2">
+      <c r="K7" s="9">
+        <f>+J7+I7</f>
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>10</v>
-      </c>
-      <c r="K3">
-        <v>10</v>
-      </c>
-      <c r="L3">
-        <v>10</v>
-      </c>
-      <c r="M3">
-        <v>10</v>
-      </c>
-      <c r="N3">
-        <v>10</v>
-      </c>
-      <c r="O3">
-        <f>+N3</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>4</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>4</v>
-      </c>
-      <c r="K4">
-        <v>4</v>
-      </c>
-      <c r="L4">
-        <v>10</v>
-      </c>
-      <c r="M4">
-        <v>10</v>
-      </c>
-      <c r="N4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A8">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9">
+        <v>40</v>
+      </c>
+      <c r="G9" s="18">
+        <v>2.5E+19</v>
+      </c>
+      <c r="H9">
+        <f>+G9*70%</f>
+        <v>1.7499999999999998E+19</v>
+      </c>
+      <c r="I9">
+        <f>+E9/SUM(E9:E10)*$H$2*60</f>
+        <v>42</v>
+      </c>
+      <c r="J9" s="9">
+        <f>+$I$2*G9/SUM(G9:G10)*60</f>
+        <v>6</v>
+      </c>
+      <c r="K9" s="9">
+        <f>+J9+I9</f>
+        <v>48</v>
+      </c>
+      <c r="L9" s="22">
+        <f>+K9+K6</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="18">
+        <v>5E+19</v>
+      </c>
+      <c r="H10">
+        <f>+G10*70%</f>
+        <v>3.4999999999999996E+19</v>
+      </c>
+      <c r="I10">
+        <f>+E10/SUM(E9:E10)*$H$3*60</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="9">
+        <f>+$I$2*G10/SUM(G9:G10)*60</f>
         <v>12</v>
       </c>
-      <c r="O4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <f>+E5+4*F3/E10</f>
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <f>+F5</f>
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <f>+G5</f>
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <f>+H5</f>
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <f>+I5</f>
-        <v>2</v>
-      </c>
-      <c r="K5">
-        <f>+J5</f>
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <f>+K5+(L2-K4)*L3/K10</f>
-        <v>2.1428571428571428</v>
-      </c>
-      <c r="M5">
-        <f>+L5</f>
-        <v>2.1428571428571428</v>
-      </c>
-      <c r="N5">
-        <f>+M5+(N2-M4)*N3/M10</f>
-        <v>3.1428571428571428</v>
-      </c>
-      <c r="O5">
-        <f>+N5</f>
-        <v>3.1428571428571428</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <f>+F5</f>
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <f>+F7</f>
-        <v>2</v>
-      </c>
-      <c r="H7">
-        <f>+G7</f>
-        <v>2</v>
-      </c>
-      <c r="I7">
-        <f>+H7</f>
-        <v>2</v>
-      </c>
-      <c r="J7">
-        <f>+I7</f>
-        <v>2</v>
-      </c>
-      <c r="K7">
-        <f>+J7</f>
-        <v>2</v>
-      </c>
-      <c r="L7">
-        <f>+K7</f>
-        <v>2</v>
-      </c>
-      <c r="N7">
-        <f>+N5</f>
-        <v>3.1428571428571428</v>
-      </c>
-      <c r="O7">
-        <f>+N7</f>
-        <v>3.1428571428571428</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <f>+F8</f>
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <f>+G8</f>
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <f>+H8</f>
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <f>+I8</f>
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <f>+J8</f>
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <f>+K8</f>
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <f>+E10*(N5-E7)</f>
-        <v>62.857142857142854</v>
-      </c>
-      <c r="O8">
-        <f>+F11*(O5-F7)</f>
-        <v>457.14285714285711</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
+      <c r="K10" s="9">
+        <f>+J10+I10</f>
+        <v>12</v>
+      </c>
+      <c r="L10" s="22">
+        <f>+K10+K7</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A11">
+        <v>120</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12">
+        <v>40</v>
+      </c>
+      <c r="G12" s="18">
+        <v>2.5E+19</v>
+      </c>
+      <c r="H12">
+        <f>+G12*70%</f>
+        <v>1.7499999999999998E+19</v>
+      </c>
+      <c r="I12">
+        <f>+E12/SUM(E12:E13)*$H$2*30</f>
+        <v>21</v>
+      </c>
+      <c r="J12" s="21">
+        <f>+$I$2*G12/SUM(G12:G13)*30</f>
+        <v>2.3684210526315788</v>
+      </c>
+      <c r="K12" s="9">
+        <f>+J12+I12</f>
+        <v>23.368421052631579</v>
+      </c>
+      <c r="L12" s="22">
+        <f>+L9+K12</f>
+        <v>77.368421052631575</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="18">
+        <v>7E+19</v>
+      </c>
+      <c r="H13">
+        <f>+G13*70%</f>
+        <v>4.9E+19</v>
+      </c>
+      <c r="I13">
+        <f>+E13/SUM(E12:E13)*$H$3*30</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="9">
+        <f>+$I$2*G13/SUM(G12:G13)*30</f>
+        <v>6.6315789473684212</v>
+      </c>
+      <c r="K13" s="9">
+        <f>+J13+I13</f>
+        <v>6.6315789473684212</v>
+      </c>
+      <c r="L13" s="22">
+        <f>+L10+K13</f>
+        <v>30.631578947368421</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A14">
+        <v>150</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14">
+        <v>40</v>
+      </c>
+      <c r="G14">
+        <v>25</v>
+      </c>
+      <c r="H14">
+        <f>+G14*70%</f>
+        <v>17.5</v>
+      </c>
+      <c r="I14">
+        <f>+E14/SUM(E14:E15)*$H$2*70</f>
+        <v>32.666666666666664</v>
+      </c>
+      <c r="J14" s="9">
+        <f>+$I$2*G14/SUM(G14:G15)*70</f>
+        <v>5.5263157894736841</v>
+      </c>
+      <c r="K14" s="9">
+        <f>+J14+I14</f>
+        <v>38.192982456140349</v>
+      </c>
+      <c r="L14" s="22">
+        <f>+L12+K14</f>
+        <v>115.56140350877192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15">
         <v>20</v>
       </c>
-      <c r="D10">
+      <c r="G15">
+        <v>70</v>
+      </c>
+      <c r="H15">
+        <f>+G15*70%</f>
+        <v>49</v>
+      </c>
+      <c r="I15">
+        <f>+E15/SUM(E14:E15)*$H$2*70</f>
+        <v>16.333333333333332</v>
+      </c>
+      <c r="J15" s="9">
+        <f>+$I$2*G15/SUM(G14:G15)*70</f>
+        <v>15.473684210526315</v>
+      </c>
+      <c r="K15" s="9">
+        <f>+J15+I15</f>
+        <v>31.807017543859647</v>
+      </c>
+      <c r="L15" s="22">
+        <f>+L13+K15</f>
+        <v>62.438596491228068</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A16">
+        <v>220</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17">
+        <v>30</v>
+      </c>
+      <c r="G17">
+        <v>25</v>
+      </c>
+      <c r="H17">
+        <f>+G17*70%</f>
+        <v>17.5</v>
+      </c>
+      <c r="I17">
+        <f>+E17/SUM(E17:E18)*$H$2*30</f>
+        <v>12.6</v>
+      </c>
+      <c r="J17" s="9">
+        <f>+$I$2*G17/SUM(G17:G18)*30</f>
+        <v>2.3684210526315788</v>
+      </c>
+      <c r="K17" s="9">
+        <f>+J17+I17</f>
+        <v>14.968421052631578</v>
+      </c>
+      <c r="L17" s="22">
+        <f>+L14+K17</f>
+        <v>130.5298245614035</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18">
         <v>20</v>
       </c>
-      <c r="E10">
+      <c r="G18">
+        <v>70</v>
+      </c>
+      <c r="H18">
+        <f>+G18*70%</f>
+        <v>49</v>
+      </c>
+      <c r="I18">
+        <f>+E18/SUM(E17:E18)*$H$2*30</f>
+        <v>8.3999999999999986</v>
+      </c>
+      <c r="J18" s="9">
+        <f>+$I$2*G18/SUM(G17:G18)*30</f>
+        <v>6.6315789473684212</v>
+      </c>
+      <c r="K18" s="9">
+        <f>+J18+I18</f>
+        <v>15.03157894736842</v>
+      </c>
+      <c r="L18" s="22">
+        <f>+L15+K18</f>
+        <v>77.470175438596485</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A19">
+        <v>250</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20">
+        <v>30</v>
+      </c>
+      <c r="G20">
+        <v>125</v>
+      </c>
+      <c r="H20">
+        <f>+G20*70%</f>
+        <v>87.5</v>
+      </c>
+      <c r="I20">
+        <f>+E20/SUM(E20:E21)*$H$2*50</f>
+        <v>21</v>
+      </c>
+      <c r="J20" s="9">
+        <f>+$I$2*G20/SUM(G20:G21)*50</f>
+        <v>9.6153846153846168</v>
+      </c>
+      <c r="K20" s="9">
+        <f>+J20+I20</f>
+        <v>30.615384615384617</v>
+      </c>
+      <c r="L20" s="22">
+        <f>+L17+K20</f>
+        <v>161.14520917678811</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="A21">
+        <v>300</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21">
         <v>20</v>
       </c>
-      <c r="F10">
-        <v>420</v>
-      </c>
-      <c r="G10">
-        <v>420</v>
-      </c>
-      <c r="H10">
-        <v>420</v>
-      </c>
-      <c r="I10">
-        <v>420</v>
-      </c>
-      <c r="J10">
-        <v>420</v>
-      </c>
-      <c r="K10">
-        <v>420</v>
-      </c>
-      <c r="L10">
-        <v>20</v>
-      </c>
-      <c r="M10">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>20</v>
-      </c>
-      <c r="F11">
-        <v>400</v>
-      </c>
-      <c r="N11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
-      <c r="C14">
-        <v>40</v>
-      </c>
-      <c r="K14">
-        <f>60*400/420</f>
-        <v>57.142857142857146</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
-      <c r="C15">
-        <v>2.8</v>
-      </c>
-      <c r="G15">
-        <f>60/420*20</f>
-        <v>2.8571428571428568</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
-      <c r="C16">
-        <v>20</v>
+      <c r="G21">
+        <v>70</v>
+      </c>
+      <c r="H21">
+        <f>+G21*70%</f>
+        <v>49</v>
+      </c>
+      <c r="I21">
+        <f>+E21/SUM(E20:E21)*$H$2*50</f>
+        <v>13.999999999999998</v>
+      </c>
+      <c r="J21" s="9">
+        <f>+$I$2*G21/SUM(G20:G21)*50</f>
+        <v>5.384615384615385</v>
+      </c>
+      <c r="K21" s="9">
+        <f>+J21+I21</f>
+        <v>19.384615384615383</v>
+      </c>
+      <c r="L21" s="22">
+        <f>+L18+K21</f>
+        <v>96.854790823211871</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="16">
+        <f>+SUM(K6,K9,K12,K14,K17,K20)</f>
+        <v>161.14520917678811</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="16">
+        <f>+SUM(K7,K10,K13,K15,K18,K21)</f>
+        <v>96.854790823211871</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="E26">
+        <f>+SUM(E24:E25)</f>
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final implementation test includes token interactions and final balance checks
</commit_message>
<xml_diff>
--- a/20210921 - Staking Rewards.xlsx
+++ b/20210921 - Staking Rewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Documents\16slimchance16\token\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16455B87-3B48-4925-A208-F325ABB3D7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F25D1A3-3E7E-4D1A-9652-2ADB2D4EF8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-90" windowWidth="16530" windowHeight="10980" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -227,15 +227,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0000000000000"/>
     <numFmt numFmtId="168" formatCode="0.0000000%"/>
-    <numFmt numFmtId="173" formatCode="0.0000000E+00"/>
-    <numFmt numFmtId="190" formatCode="#,##0.000000000000000000"/>
-    <numFmt numFmtId="191" formatCode="#,##0.0000000000000000000"/>
+    <numFmt numFmtId="169" formatCode="0.0000000E+00"/>
+    <numFmt numFmtId="170" formatCode="#,##0.000000000000000000"/>
+    <numFmt numFmtId="171" formatCode="#,##0.0000000000000000000"/>
+    <numFmt numFmtId="190" formatCode="0.E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -303,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -324,9 +325,10 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2343,10 +2345,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DC2E69-E67B-45D9-BD33-D97282242B36}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2362,7 +2364,7 @@
     <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.76953125" style="20" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.453125" customWidth="1"/>
-    <col min="12" max="12" width="23.90625" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -2877,6 +2879,9 @@
         <f>+SUM(K6,K9,K12,K14,K17,K20)</f>
         <v>161.14520917678811</v>
       </c>
+      <c r="L24" s="23">
+        <v>1E+16</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.75">
       <c r="D25" t="s">
@@ -2892,8 +2897,17 @@
         <f>+SUM(E24:E25)</f>
         <v>258</v>
       </c>
+      <c r="L26" s="22">
+        <v>77.368421052631604</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="L27" s="22">
+        <v>30.6315789473684</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Included stakeEscrow functions in staking rewards
</commit_message>
<xml_diff>
--- a/20210921 - Staking Rewards.xlsx
+++ b/20210921 - Staking Rewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Documents\16slimchance16\token\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA63F86-B5C4-439E-9C84-3C6E9B1363D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416C1A72-B310-419F-BBDB-D31F6E0D8222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-90" windowWidth="16530" windowHeight="10980" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -236,13 +236,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0000000000000"/>
     <numFmt numFmtId="168" formatCode="0.0000000%"/>
     <numFmt numFmtId="169" formatCode="0.0000000E+00"/>
+    <numFmt numFmtId="171" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -413,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -450,11 +451,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2474,7 +2478,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2490,7 +2494,7 @@
     <col min="9" max="9" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.453125" style="20" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.04296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.31640625" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -2561,9 +2565,9 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="40"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="10"/>
+      <c r="L4" s="40"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A6" s="29" t="s">
@@ -2594,7 +2598,7 @@
       <c r="K6" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="32" t="s">
+      <c r="L6" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2602,7 +2606,7 @@
       <c r="A7" s="23">
         <v>0</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="36" t="s">
         <v>46</v>
       </c>
       <c r="C7" s="3"/>
@@ -2632,11 +2636,11 @@
         <f>+J7+I7</f>
         <v>6</v>
       </c>
-      <c r="L7" s="36"/>
+      <c r="L7" s="42"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A8" s="23"/>
-      <c r="B8" s="38"/>
+      <c r="B8" s="36"/>
       <c r="D8" s="23" t="s">
         <v>35</v>
       </c>
@@ -2663,13 +2667,13 @@
         <f>+J8+I8</f>
         <v>12</v>
       </c>
-      <c r="L8" s="36"/>
+      <c r="L8" s="42"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A9" s="23">
         <v>60</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="36" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="23"/>
@@ -2680,11 +2684,11 @@
       <c r="I9" s="35"/>
       <c r="J9" s="35"/>
       <c r="K9" s="35"/>
-      <c r="L9" s="36"/>
+      <c r="L9" s="42"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A10" s="23"/>
-      <c r="B10" s="38"/>
+      <c r="B10" s="36"/>
       <c r="D10" s="23" t="s">
         <v>34</v>
       </c>
@@ -2712,14 +2716,14 @@
         <f>+J10+I10</f>
         <v>48</v>
       </c>
-      <c r="L10" s="36">
+      <c r="L10" s="42">
         <f>+K10+K7</f>
         <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A11" s="23"/>
-      <c r="B11" s="38"/>
+      <c r="B11" s="36"/>
       <c r="D11" s="23" t="s">
         <v>35</v>
       </c>
@@ -2746,7 +2750,7 @@
         <f>+J11+I11</f>
         <v>12</v>
       </c>
-      <c r="L11" s="36">
+      <c r="L11" s="42">
         <f>+K11+K8</f>
         <v>24</v>
       </c>
@@ -2755,7 +2759,7 @@
       <c r="A12" s="23">
         <v>120</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="36" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="23"/>
@@ -2766,11 +2770,11 @@
       <c r="I12" s="35"/>
       <c r="J12" s="35"/>
       <c r="K12" s="35"/>
-      <c r="L12" s="36"/>
+      <c r="L12" s="42"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A13" s="23"/>
-      <c r="B13" s="38"/>
+      <c r="B13" s="36"/>
       <c r="D13" s="23" t="s">
         <v>34</v>
       </c>
@@ -2798,14 +2802,14 @@
         <f>+J13+I13</f>
         <v>23.368421052631579</v>
       </c>
-      <c r="L13" s="36">
+      <c r="L13" s="42">
         <f>+L10+K13</f>
         <v>77.368421052631575</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A14" s="23"/>
-      <c r="B14" s="38"/>
+      <c r="B14" s="36"/>
       <c r="D14" s="23" t="s">
         <v>35</v>
       </c>
@@ -2832,7 +2836,7 @@
         <f>+J14+I14</f>
         <v>6.6315789473684212</v>
       </c>
-      <c r="L14" s="36">
+      <c r="L14" s="42">
         <f>+L11+K14</f>
         <v>30.631578947368421</v>
       </c>
@@ -2841,7 +2845,7 @@
       <c r="A15" s="23">
         <v>150</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="36" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="23" t="s">
@@ -2871,14 +2875,14 @@
         <f>+J15+I15</f>
         <v>38.192982456140349</v>
       </c>
-      <c r="L15" s="36">
+      <c r="L15" s="42">
         <f>+L13+K15</f>
         <v>115.56140350877192</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A16" s="23"/>
-      <c r="B16" s="38"/>
+      <c r="B16" s="36"/>
       <c r="D16" s="23" t="s">
         <v>35</v>
       </c>
@@ -2905,7 +2909,7 @@
         <f>+J16+I16</f>
         <v>31.807017543859647</v>
       </c>
-      <c r="L16" s="36">
+      <c r="L16" s="42">
         <f>+L14+K16</f>
         <v>62.438596491228068</v>
       </c>
@@ -2914,7 +2918,7 @@
       <c r="A17" s="23">
         <v>220</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="36" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="23"/>
@@ -2925,11 +2929,11 @@
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
-      <c r="L17" s="36"/>
+      <c r="L17" s="42"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A18" s="23"/>
-      <c r="B18" s="38"/>
+      <c r="B18" s="36"/>
       <c r="D18" s="23" t="s">
         <v>34</v>
       </c>
@@ -2957,14 +2961,14 @@
         <f>+J18+I18</f>
         <v>14.968421052631578</v>
       </c>
-      <c r="L18" s="36">
+      <c r="L18" s="42">
         <f>+L15+K18</f>
         <v>130.5298245614035</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A19" s="23"/>
-      <c r="B19" s="38"/>
+      <c r="B19" s="36"/>
       <c r="D19" s="23" t="s">
         <v>35</v>
       </c>
@@ -2991,7 +2995,7 @@
         <f>+J19+I19</f>
         <v>15.03157894736842</v>
       </c>
-      <c r="L19" s="36">
+      <c r="L19" s="42">
         <f>+L16+K19</f>
         <v>77.470175438596485</v>
       </c>
@@ -3000,7 +3004,7 @@
       <c r="A20" s="23">
         <v>250</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="36" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="23"/>
@@ -3011,11 +3015,11 @@
       <c r="I20" s="35"/>
       <c r="J20" s="35"/>
       <c r="K20" s="35"/>
-      <c r="L20" s="36"/>
+      <c r="L20" s="42"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A21" s="23"/>
-      <c r="B21" s="38"/>
+      <c r="B21" s="36"/>
       <c r="D21" s="23" t="s">
         <v>34</v>
       </c>
@@ -3043,7 +3047,7 @@
         <f>+J21+I21</f>
         <v>30.615384615384617</v>
       </c>
-      <c r="L21" s="36">
+      <c r="L21" s="42">
         <f>+L18+K21</f>
         <v>161.14520917678811</v>
       </c>
@@ -3052,7 +3056,7 @@
       <c r="A22" s="25">
         <v>300</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="37" t="s">
         <v>25</v>
       </c>
       <c r="D22" s="25" t="s">
@@ -3081,7 +3085,7 @@
         <f>+J22+I22</f>
         <v>19.384615384615383</v>
       </c>
-      <c r="L22" s="37">
+      <c r="L22" s="43">
         <f>+L19+K22</f>
         <v>96.854790823211871</v>
       </c>

</xml_diff>

<commit_message>
Tests with exit() function
</commit_message>
<xml_diff>
--- a/20210921 - Staking Rewards.xlsx
+++ b/20210921 - Staking Rewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Documents\16slimchance16\token\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00C8562-5620-44CB-9B2B-1C9336197E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1470B85-1A93-4A29-88A7-82D1B27EA324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-90" windowWidth="16530" windowHeight="10980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,9 +169,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.0000000E+00"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0000000E+00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -352,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -361,19 +361,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1417,7 +1417,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1719,15 +1719,15 @@
       </c>
       <c r="J13" s="22">
         <f>+$I$2*G13/SUM(G13:G14)*30</f>
-        <v>2.3684210526315788</v>
+        <v>3.2142855994898003E-7</v>
       </c>
       <c r="K13" s="22">
         <f>+J13+I13</f>
-        <v>19.868421052631579</v>
+        <v>17.500000321428558</v>
       </c>
       <c r="L13" s="31">
         <f>+L10+K13</f>
-        <v>87.868421052631575</v>
+        <v>85.500000321428558</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.75">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="21">
-        <v>7E+19</v>
+        <v>6.9999999999999998E+26</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="22">
@@ -1750,15 +1750,15 @@
       </c>
       <c r="J14" s="22">
         <f>+$I$2*G14/SUM(G13:G14)*30</f>
-        <v>6.6315789473684212</v>
+        <v>8.9999996785714398</v>
       </c>
       <c r="K14" s="22">
         <f>+J14+I14</f>
-        <v>10.131578947368421</v>
+        <v>12.49999967857144</v>
       </c>
       <c r="L14" s="31">
         <f>+L11+K14</f>
-        <v>62.131578947368425</v>
+        <v>64.499999678571442</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.75">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="L15" s="31">
         <f>+L13+K15</f>
-        <v>124.01973684210526</v>
+        <v>121.65131611090224</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.75">
@@ -1824,7 +1824,7 @@
       </c>
       <c r="L16" s="31">
         <f>+L14+K16</f>
-        <v>95.98026315789474</v>
+        <v>98.348683889097757</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.75">
@@ -1872,7 +1872,7 @@
       </c>
       <c r="L18" s="31">
         <f>+L15+K18</f>
-        <v>138.38815789473685</v>
+        <v>136.01973716353382</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.75">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="L19" s="31">
         <f>+L16+K19</f>
-        <v>111.61184210526316</v>
+        <v>113.98026283646618</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.75">
@@ -1951,7 +1951,7 @@
       </c>
       <c r="L21" s="31">
         <f>+L18+K21</f>
-        <v>168.00354251012146</v>
+        <v>165.63512177891843</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.75">
@@ -1986,7 +1986,7 @@
       </c>
       <c r="L22" s="32">
         <f>+L19+K22</f>
-        <v>131.99645748987854</v>
+        <v>134.36487822108157</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -2001,7 +2001,7 @@
       </c>
       <c r="E25" s="33">
         <f>+SUM(K7,K10,K13,K15,K18,K21)</f>
-        <v>168.00354251012146</v>
+        <v>165.63512177891843</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.75">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="E26" s="34">
         <f>+SUM(K8,K11,K14,K16,K19,K22)</f>
-        <v>131.99645748987854</v>
+        <v>134.36487822108157</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
Added power formula in excel
</commit_message>
<xml_diff>
--- a/20210921 - Staking Rewards.xlsx
+++ b/20210921 - Staking Rewards.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Documents\16slimchance16\token\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1470B85-1A93-4A29-88A7-82D1B27EA324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DC6639-44DE-4582-B168-FCC9BCC97F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-90" windowWidth="16530" windowHeight="10980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-90" windowWidth="16530" windowHeight="10980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SNX" sheetId="1" r:id="rId1"/>
     <sheet name="SNX - Detail" sheetId="4" r:id="rId2"/>
     <sheet name="KWENTA" sheetId="5" r:id="rId3"/>
+    <sheet name="KWENTA - power" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="50">
   <si>
     <t>N stake 20</t>
   </si>
@@ -162,6 +163,30 @@
   </si>
   <si>
     <t>Account</t>
+  </si>
+  <si>
+    <t>stakerScore</t>
+  </si>
+  <si>
+    <t>traderScore</t>
+  </si>
+  <si>
+    <t>weight stake</t>
+  </si>
+  <si>
+    <t>weight trade</t>
+  </si>
+  <si>
+    <t>stakingPart</t>
+  </si>
+  <si>
+    <t>tradingPart</t>
+  </si>
+  <si>
+    <t>rewScore</t>
+  </si>
+  <si>
+    <t>%rewards</t>
   </si>
 </sst>
 </file>
@@ -342,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -378,6 +403,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1416,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DC2E69-E67B-45D9-BD33-D97282242B36}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2026,4 +2054,755 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486B17B1-BE12-4310-9A3F-24B7422EA458}">
+  <dimension ref="A1:N27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:R1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.40625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.31640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.54296875" style="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.04296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="E1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>300</v>
+      </c>
+      <c r="F2">
+        <v>300</v>
+      </c>
+      <c r="G2">
+        <f>+E2/F2</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="30"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A4" s="8"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="27"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A6" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A7" s="12">
+        <v>0</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="20">
+        <v>10</v>
+      </c>
+      <c r="F7" s="21">
+        <v>2.5E+19</v>
+      </c>
+      <c r="G7" s="22">
+        <f>+E7/SUM(E7:E8)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="22">
+        <f>+F7/SUM(F7:F8)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I7" s="22">
+        <f>+G7^$H$2</f>
+        <v>0.125</v>
+      </c>
+      <c r="J7" s="22">
+        <f>+H7^$I$2</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K7" s="22">
+        <f>+J7*I7</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="L7" s="37">
+        <f>+K7/SUM(K7:K8)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M7" s="35">
+        <f>+$G$2*60*L7</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A8" s="12"/>
+      <c r="B8" s="23"/>
+      <c r="D8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="20">
+        <v>10</v>
+      </c>
+      <c r="F8" s="21">
+        <v>5E+19</v>
+      </c>
+      <c r="G8" s="22">
+        <f>+E8/SUM(E7:E8)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="22">
+        <f>+F8/SUM(F7:F8)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I8" s="22">
+        <f>+G8^$H$2</f>
+        <v>0.125</v>
+      </c>
+      <c r="J8" s="22">
+        <f>+H8^$I$2</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K8" s="22">
+        <f>+J8*I8</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="L8" s="37">
+        <f>+K8/SUM(K7:K8)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M8" s="35">
+        <f>+$G$2*60*L8</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A9" s="12">
+        <v>60</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="35"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A10" s="12"/>
+      <c r="B10" s="23"/>
+      <c r="D10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="20">
+        <v>50</v>
+      </c>
+      <c r="F10" s="21">
+        <v>2.5E+19</v>
+      </c>
+      <c r="G10" s="22">
+        <f>+E10/SUM(E10:E11)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H10" s="22">
+        <f>+F10/SUM(F10:F11)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I10" s="22">
+        <f>+G10^$H$2</f>
+        <v>0.57870370370370383</v>
+      </c>
+      <c r="J10" s="22">
+        <f>+H10^$I$2</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K10" s="22">
+        <f>+J10*I10</f>
+        <v>0.19290123456790126</v>
+      </c>
+      <c r="L10" s="22">
+        <f>+K10/SUM(K10:K11)</f>
+        <v>0.98425196850393692</v>
+      </c>
+      <c r="M10" s="35">
+        <f>+$G$2*60*L10</f>
+        <v>59.055118110236215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A11" s="12"/>
+      <c r="B11" s="23"/>
+      <c r="D11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="20">
+        <v>10</v>
+      </c>
+      <c r="F11" s="21">
+        <v>5E+19</v>
+      </c>
+      <c r="G11" s="22">
+        <f>+E11/SUM(E10:E11)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H11" s="22">
+        <f>+F11/SUM(F10:F11)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I11" s="22">
+        <f>+G11^$H$2</f>
+        <v>4.6296296296296294E-3</v>
+      </c>
+      <c r="J11" s="22">
+        <f>+H11^$I$2</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K11" s="22">
+        <f>+J11*I11</f>
+        <v>3.0864197530864196E-3</v>
+      </c>
+      <c r="L11" s="22">
+        <f>+K11/SUM(K10:K11)</f>
+        <v>1.5748031496062988E-2</v>
+      </c>
+      <c r="M11" s="35">
+        <f>+$G$2*60*L11</f>
+        <v>0.94488188976377929</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A12" s="12">
+        <v>120</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="35"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A13" s="12"/>
+      <c r="B13" s="23"/>
+      <c r="D13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="20">
+        <v>50</v>
+      </c>
+      <c r="F13" s="21">
+        <v>2.5E+19</v>
+      </c>
+      <c r="G13" s="22">
+        <f>+E13/SUM(E13:E14)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H13" s="22">
+        <f>+F13/SUM(F13:F14)</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="I13" s="22">
+        <f>+G13^$H$2</f>
+        <v>0.57870370370370383</v>
+      </c>
+      <c r="J13" s="22">
+        <f>+H13^$I$2</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="K13" s="22">
+        <f>+J13*I13</f>
+        <v>0.15229044834307995</v>
+      </c>
+      <c r="L13" s="22">
+        <f>+K13/SUM(K13:K14)</f>
+        <v>0.9780907668231611</v>
+      </c>
+      <c r="M13" s="35">
+        <f>+$G$2*30*L13</f>
+        <v>29.342723004694832</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A14" s="12"/>
+      <c r="B14" s="23"/>
+      <c r="D14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="20">
+        <v>10</v>
+      </c>
+      <c r="F14" s="21">
+        <v>7E+19</v>
+      </c>
+      <c r="G14" s="22">
+        <f>+E14/SUM(E13:E14)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H14" s="22">
+        <f>+F14/SUM(F13:F14)</f>
+        <v>0.73684210526315785</v>
+      </c>
+      <c r="I14" s="22">
+        <f>+G14^$H$2</f>
+        <v>4.6296296296296294E-3</v>
+      </c>
+      <c r="J14" s="22">
+        <f>+H14^$I$2</f>
+        <v>0.73684210526315785</v>
+      </c>
+      <c r="K14" s="22">
+        <f>+J14*I14</f>
+        <v>3.4113060428849901E-3</v>
+      </c>
+      <c r="L14" s="22">
+        <f>+K14/SUM(K13:K14)</f>
+        <v>2.1909233176838804E-2</v>
+      </c>
+      <c r="M14" s="35">
+        <f>+$G$2*30*L14</f>
+        <v>0.65727699530516415</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A15" s="12">
+        <v>150</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="20">
+        <v>50</v>
+      </c>
+      <c r="F15" s="20">
+        <v>2.5E+19</v>
+      </c>
+      <c r="G15" s="22">
+        <f>+E15/SUM(E15:E16)</f>
+        <v>0.625</v>
+      </c>
+      <c r="H15" s="22">
+        <f>+F15/SUM(F15:F16)</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="I15" s="22">
+        <f>+G15^$H$2</f>
+        <v>0.244140625</v>
+      </c>
+      <c r="J15" s="22">
+        <f>+H15^$I$2</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="K15" s="22">
+        <f>+J15*I15</f>
+        <v>6.4247532894736836E-2</v>
+      </c>
+      <c r="L15" s="22">
+        <f>+K15/SUM(K15:K16)</f>
+        <v>0.62313060817547361</v>
+      </c>
+      <c r="M15" s="35">
+        <f>+$G$2*70*L15</f>
+        <v>43.619142572283153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.75">
+      <c r="A16" s="12"/>
+      <c r="B16" s="23"/>
+      <c r="D16" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="20">
+        <v>30</v>
+      </c>
+      <c r="F16" s="20">
+        <v>7E+19</v>
+      </c>
+      <c r="G16" s="22">
+        <f>+E16/SUM(E15:E16)</f>
+        <v>0.375</v>
+      </c>
+      <c r="H16" s="22">
+        <f>+F16/SUM(F15:F16)</f>
+        <v>0.73684210526315785</v>
+      </c>
+      <c r="I16" s="22">
+        <f>+G16^$H$2</f>
+        <v>5.2734375E-2</v>
+      </c>
+      <c r="J16" s="22">
+        <f>+H16^$I$2</f>
+        <v>0.73684210526315785</v>
+      </c>
+      <c r="K16" s="22">
+        <f>+J16*I16</f>
+        <v>3.8856907894736843E-2</v>
+      </c>
+      <c r="L16" s="22">
+        <f>+K16/SUM(K15:K16)</f>
+        <v>0.3768693918245265</v>
+      </c>
+      <c r="M16" s="35">
+        <f>+$G$2*70*L16</f>
+        <v>26.380857427716855</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.75">
+      <c r="A17" s="12">
+        <v>220</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="35"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.75">
+      <c r="A18" s="12"/>
+      <c r="B18" s="23"/>
+      <c r="D18" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="20">
+        <v>40</v>
+      </c>
+      <c r="F18" s="20">
+        <v>2.5E+19</v>
+      </c>
+      <c r="G18" s="22">
+        <f>+E18/SUM(E18:E19)</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="H18" s="22">
+        <f>+F18/SUM(F18:F19)</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="I18" s="22">
+        <f>+G18^$H$2</f>
+        <v>0.1865889212827988</v>
+      </c>
+      <c r="J18" s="22">
+        <f>+H18^$I$2</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="K18" s="22">
+        <f>+J18*I18</f>
+        <v>4.910234770599968E-2</v>
+      </c>
+      <c r="L18" s="22">
+        <f>+K18/SUM(K18:K19)</f>
+        <v>0.45845272206303722</v>
+      </c>
+      <c r="M18" s="35">
+        <f>+$G$2*30*L18</f>
+        <v>13.753581661891117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.75">
+      <c r="A19" s="12"/>
+      <c r="B19" s="23"/>
+      <c r="D19" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="20">
+        <v>30</v>
+      </c>
+      <c r="F19" s="20">
+        <v>7E+19</v>
+      </c>
+      <c r="G19" s="22">
+        <f>+E19/SUM(E18:E19)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="H19" s="22">
+        <f>+F19/SUM(F18:F19)</f>
+        <v>0.73684210526315785</v>
+      </c>
+      <c r="I19" s="22">
+        <f>+G19^$H$2</f>
+        <v>7.871720116618075E-2</v>
+      </c>
+      <c r="J19" s="22">
+        <f>+H19^$I$2</f>
+        <v>0.73684210526315785</v>
+      </c>
+      <c r="K19" s="22">
+        <f>+J19*I19</f>
+        <v>5.800214822771213E-2</v>
+      </c>
+      <c r="L19" s="22">
+        <f>+K19/SUM(K18:K19)</f>
+        <v>0.54154727793696278</v>
+      </c>
+      <c r="M19" s="35">
+        <f>+$G$2*30*L19</f>
+        <v>16.246418338108882</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.75">
+      <c r="A20" s="12">
+        <v>250</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="35"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.75">
+      <c r="A21" s="12"/>
+      <c r="B21" s="23"/>
+      <c r="D21" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="20">
+        <v>40</v>
+      </c>
+      <c r="F21" s="20">
+        <v>1.25E+20</v>
+      </c>
+      <c r="G21" s="22">
+        <f>+E21/SUM(E21:E22)</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="H21" s="22">
+        <f>+F21/SUM(F21:F22)</f>
+        <v>0.64102564102564108</v>
+      </c>
+      <c r="I21" s="22">
+        <f>+G21^$H$2</f>
+        <v>0.1865889212827988</v>
+      </c>
+      <c r="J21" s="22">
+        <f>+H21^$I$2</f>
+        <v>0.64102564102564108</v>
+      </c>
+      <c r="K21" s="22">
+        <f>+J21*I21</f>
+        <v>0.11960828287358899</v>
+      </c>
+      <c r="L21" s="22">
+        <f>+K21/SUM(K21:K22)</f>
+        <v>0.80889787664307389</v>
+      </c>
+      <c r="M21" s="35">
+        <f>+$G$2*50*L21</f>
+        <v>40.444893832153696</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.75">
+      <c r="A22" s="13">
+        <v>300</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="6">
+        <v>30</v>
+      </c>
+      <c r="F22" s="6">
+        <v>7E+19</v>
+      </c>
+      <c r="G22" s="7">
+        <f>+E22/SUM(E21:E22)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="H22" s="7">
+        <f>+F22/SUM(F21:F22)</f>
+        <v>0.35897435897435898</v>
+      </c>
+      <c r="I22" s="7">
+        <f>+G22^$H$2</f>
+        <v>7.871720116618075E-2</v>
+      </c>
+      <c r="J22" s="22">
+        <f>+H22^$I$2</f>
+        <v>0.35897435897435898</v>
+      </c>
+      <c r="K22" s="7">
+        <f>+J22*I22</f>
+        <v>2.8257456828885398E-2</v>
+      </c>
+      <c r="L22" s="7">
+        <f>+K22/SUM(K21:K22)</f>
+        <v>0.1911021233569262</v>
+      </c>
+      <c r="M22" s="36">
+        <f>+$G$2*50*L22</f>
+        <v>9.5551061678463096</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="D24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="D25" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="33">
+        <f>+SUM(M7,M10,M13,M15,M18,M21)</f>
+        <v>206.21545918125898</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.75">
+      <c r="D26" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="34">
+        <f>+SUM(M8,M11,M14,M16,M19,M22)</f>
+        <v>93.784540818740979</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.75">
+      <c r="D27" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="15">
+        <f>+SUM(E25:E26)</f>
+        <v>299.99999999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor code to use power formula in reward score calculations
</commit_message>
<xml_diff>
--- a/20210921 - Staking Rewards.xlsx
+++ b/20210921 - Staking Rewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Documents\16slimchance16\token\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DC6639-44DE-4582-B168-FCC9BCC97F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7000EF3C-7087-4169-96B0-DBBBB1BBF4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-90" windowWidth="16530" windowHeight="10980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
   <si>
     <t>N stake 20</t>
   </si>
@@ -193,10 +193,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000000E+00"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -367,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -404,8 +405,11 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2060,8 +2064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486B17B1-BE12-4310-9A3F-24B7422EA458}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:R1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2074,11 +2078,11 @@
     <col min="6" max="6" width="8.86328125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12.1328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.31640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.26953125" style="9" customWidth="1"/>
     <col min="11" max="11" width="8.6328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.54296875" style="26" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.04296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
@@ -2123,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -2153,6 +2157,7 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A6" s="16" t="s">
@@ -2188,8 +2193,11 @@
       <c r="L6" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="39" t="s">
         <v>6</v>
+      </c>
+      <c r="N6" s="40" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.75">
@@ -2219,7 +2227,7 @@
       </c>
       <c r="I7" s="22">
         <f>+G7^$H$2</f>
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="J7" s="22">
         <f>+H7^$I$2</f>
@@ -2227,14 +2235,18 @@
       </c>
       <c r="K7" s="22">
         <f>+J7*I7</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L7" s="37">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="L7" s="36">
         <f>+K7/SUM(K7:K8)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="M7" s="35">
+      <c r="M7" s="22">
         <f>+$G$2*60*L7</f>
+        <v>20</v>
+      </c>
+      <c r="N7" s="35">
+        <f>+M7</f>
         <v>20</v>
       </c>
     </row>
@@ -2260,7 +2272,7 @@
       </c>
       <c r="I8" s="22">
         <f>+G8^$H$2</f>
-        <v>0.125</v>
+        <v>0.5</v>
       </c>
       <c r="J8" s="22">
         <f>+H8^$I$2</f>
@@ -2268,14 +2280,18 @@
       </c>
       <c r="K8" s="22">
         <f>+J8*I8</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="L8" s="37">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L8" s="36">
         <f>+K8/SUM(K7:K8)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="M8" s="35">
+      <c r="M8" s="22">
         <f>+$G$2*60*L8</f>
+        <v>40</v>
+      </c>
+      <c r="N8" s="35">
+        <f>+M8</f>
         <v>40</v>
       </c>
     </row>
@@ -2295,7 +2311,8 @@
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
       <c r="L9" s="22"/>
-      <c r="M9" s="35"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="23"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A10" s="12"/>
@@ -2319,7 +2336,7 @@
       </c>
       <c r="I10" s="22">
         <f>+G10^$H$2</f>
-        <v>0.57870370370370383</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="J10" s="22">
         <f>+H10^$I$2</f>
@@ -2327,15 +2344,19 @@
       </c>
       <c r="K10" s="22">
         <f>+J10*I10</f>
-        <v>0.19290123456790126</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="L10" s="22">
         <f>+K10/SUM(K10:K11)</f>
-        <v>0.98425196850393692</v>
-      </c>
-      <c r="M10" s="35">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="M10" s="22">
         <f>+$G$2*60*L10</f>
-        <v>59.055118110236215</v>
+        <v>42.857142857142861</v>
+      </c>
+      <c r="N10" s="37">
+        <f>+M10+M7</f>
+        <v>62.857142857142861</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.75">
@@ -2360,7 +2381,7 @@
       </c>
       <c r="I11" s="22">
         <f>+G11^$H$2</f>
-        <v>4.6296296296296294E-3</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="J11" s="22">
         <f>+H11^$I$2</f>
@@ -2368,15 +2389,19 @@
       </c>
       <c r="K11" s="22">
         <f>+J11*I11</f>
-        <v>3.0864197530864196E-3</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="L11" s="22">
         <f>+K11/SUM(K10:K11)</f>
-        <v>1.5748031496062988E-2</v>
-      </c>
-      <c r="M11" s="35">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="M11" s="22">
         <f>+$G$2*60*L11</f>
-        <v>0.94488188976377929</v>
+        <v>17.142857142857142</v>
+      </c>
+      <c r="N11" s="37">
+        <f>+M11+M8</f>
+        <v>57.142857142857139</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.75">
@@ -2395,7 +2420,8 @@
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22"/>
-      <c r="M12" s="35"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="23"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A13" s="12"/>
@@ -2419,7 +2445,7 @@
       </c>
       <c r="I13" s="22">
         <f>+G13^$H$2</f>
-        <v>0.57870370370370383</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="J13" s="22">
         <f>+H13^$I$2</f>
@@ -2427,15 +2453,19 @@
       </c>
       <c r="K13" s="22">
         <f>+J13*I13</f>
-        <v>0.15229044834307995</v>
+        <v>0.21929824561403508</v>
       </c>
       <c r="L13" s="22">
         <f>+K13/SUM(K13:K14)</f>
-        <v>0.9780907668231611</v>
-      </c>
-      <c r="M13" s="35">
+        <v>0.64102564102564108</v>
+      </c>
+      <c r="M13" s="22">
         <f>+$G$2*30*L13</f>
-        <v>29.342723004694832</v>
+        <v>19.230769230769234</v>
+      </c>
+      <c r="N13" s="37">
+        <f>+N10+M13</f>
+        <v>82.087912087912088</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.75">
@@ -2460,7 +2490,7 @@
       </c>
       <c r="I14" s="22">
         <f>+G14^$H$2</f>
-        <v>4.6296296296296294E-3</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="J14" s="22">
         <f>+H14^$I$2</f>
@@ -2468,15 +2498,19 @@
       </c>
       <c r="K14" s="22">
         <f>+J14*I14</f>
-        <v>3.4113060428849901E-3</v>
+        <v>0.12280701754385964</v>
       </c>
       <c r="L14" s="22">
         <f>+K14/SUM(K13:K14)</f>
-        <v>2.1909233176838804E-2</v>
-      </c>
-      <c r="M14" s="35">
+        <v>0.35897435897435898</v>
+      </c>
+      <c r="M14" s="22">
         <f>+$G$2*30*L14</f>
-        <v>0.65727699530516415</v>
+        <v>10.76923076923077</v>
+      </c>
+      <c r="N14" s="37">
+        <f>+N11+M14</f>
+        <v>67.912087912087912</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.75">
@@ -2505,7 +2539,7 @@
       </c>
       <c r="I15" s="22">
         <f>+G15^$H$2</f>
-        <v>0.244140625</v>
+        <v>0.625</v>
       </c>
       <c r="J15" s="22">
         <f>+H15^$I$2</f>
@@ -2513,15 +2547,19 @@
       </c>
       <c r="K15" s="22">
         <f>+J15*I15</f>
-        <v>6.4247532894736836E-2</v>
+        <v>0.1644736842105263</v>
       </c>
       <c r="L15" s="22">
         <f>+K15/SUM(K15:K16)</f>
-        <v>0.62313060817547361</v>
-      </c>
-      <c r="M15" s="35">
+        <v>0.37313432835820892</v>
+      </c>
+      <c r="M15" s="22">
         <f>+$G$2*70*L15</f>
-        <v>43.619142572283153</v>
+        <v>26.119402985074625</v>
+      </c>
+      <c r="N15" s="37">
+        <f>+N13+M15</f>
+        <v>108.20731507298672</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.75">
@@ -2546,7 +2584,7 @@
       </c>
       <c r="I16" s="22">
         <f>+G16^$H$2</f>
-        <v>5.2734375E-2</v>
+        <v>0.375</v>
       </c>
       <c r="J16" s="22">
         <f>+H16^$I$2</f>
@@ -2554,18 +2592,22 @@
       </c>
       <c r="K16" s="22">
         <f>+J16*I16</f>
-        <v>3.8856907894736843E-2</v>
+        <v>0.27631578947368418</v>
       </c>
       <c r="L16" s="22">
         <f>+K16/SUM(K15:K16)</f>
-        <v>0.3768693918245265</v>
-      </c>
-      <c r="M16" s="35">
+        <v>0.62686567164179097</v>
+      </c>
+      <c r="M16" s="22">
         <f>+$G$2*70*L16</f>
-        <v>26.380857427716855</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.75">
+        <v>43.880597014925371</v>
+      </c>
+      <c r="N16" s="37">
+        <f>+N14+M16</f>
+        <v>111.79268492701328</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A17" s="12">
         <v>220</v>
       </c>
@@ -2581,9 +2623,10 @@
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
       <c r="L17" s="22"/>
-      <c r="M17" s="35"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.75">
+      <c r="M17" s="22"/>
+      <c r="N17" s="37"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A18" s="12"/>
       <c r="B18" s="23"/>
       <c r="D18" s="12" t="s">
@@ -2605,7 +2648,7 @@
       </c>
       <c r="I18" s="22">
         <f>+G18^$H$2</f>
-        <v>0.1865889212827988</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="J18" s="22">
         <f>+H18^$I$2</f>
@@ -2613,18 +2656,22 @@
       </c>
       <c r="K18" s="22">
         <f>+J18*I18</f>
-        <v>4.910234770599968E-2</v>
+        <v>0.15037593984962405</v>
       </c>
       <c r="L18" s="22">
         <f>+K18/SUM(K18:K19)</f>
-        <v>0.45845272206303722</v>
-      </c>
-      <c r="M18" s="35">
+        <v>0.32258064516129031</v>
+      </c>
+      <c r="M18" s="22">
         <f>+$G$2*30*L18</f>
-        <v>13.753581661891117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.75">
+        <v>9.67741935483871</v>
+      </c>
+      <c r="N18" s="37">
+        <f>+N15+M18</f>
+        <v>117.88473442782542</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A19" s="12"/>
       <c r="B19" s="23"/>
       <c r="D19" s="12" t="s">
@@ -2646,7 +2693,7 @@
       </c>
       <c r="I19" s="22">
         <f>+G19^$H$2</f>
-        <v>7.871720116618075E-2</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="J19" s="22">
         <f>+H19^$I$2</f>
@@ -2654,18 +2701,22 @@
       </c>
       <c r="K19" s="22">
         <f>+J19*I19</f>
-        <v>5.800214822771213E-2</v>
+        <v>0.31578947368421051</v>
       </c>
       <c r="L19" s="22">
         <f>+K19/SUM(K18:K19)</f>
-        <v>0.54154727793696278</v>
-      </c>
-      <c r="M19" s="35">
+        <v>0.67741935483870963</v>
+      </c>
+      <c r="M19" s="22">
         <f>+$G$2*30*L19</f>
-        <v>16.246418338108882</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.75">
+        <v>20.322580645161288</v>
+      </c>
+      <c r="N19" s="37">
+        <f>+N16+M19</f>
+        <v>132.11526557217456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A20" s="12">
         <v>250</v>
       </c>
@@ -2681,9 +2732,10 @@
       <c r="J20" s="22"/>
       <c r="K20" s="22"/>
       <c r="L20" s="22"/>
-      <c r="M20" s="35"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.75">
+      <c r="M20" s="22"/>
+      <c r="N20" s="37"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A21" s="12"/>
       <c r="B21" s="23"/>
       <c r="D21" s="12" t="s">
@@ -2705,7 +2757,7 @@
       </c>
       <c r="I21" s="22">
         <f>+G21^$H$2</f>
-        <v>0.1865889212827988</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="J21" s="22">
         <f>+H21^$I$2</f>
@@ -2713,18 +2765,22 @@
       </c>
       <c r="K21" s="22">
         <f>+J21*I21</f>
-        <v>0.11960828287358899</v>
+        <v>0.36630036630036633</v>
       </c>
       <c r="L21" s="22">
         <f>+K21/SUM(K21:K22)</f>
-        <v>0.80889787664307389</v>
-      </c>
-      <c r="M21" s="35">
+        <v>0.70422535211267612</v>
+      </c>
+      <c r="M21" s="22">
         <f>+$G$2*50*L21</f>
-        <v>40.444893832153696</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.75">
+        <v>35.211267605633807</v>
+      </c>
+      <c r="N21" s="37">
+        <f>+N18+M21</f>
+        <v>153.09600203345923</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A22" s="13">
         <v>300</v>
       </c>
@@ -2750,56 +2806,60 @@
       </c>
       <c r="I22" s="7">
         <f>+G22^$H$2</f>
-        <v>7.871720116618075E-2</v>
-      </c>
-      <c r="J22" s="22">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="J22" s="7">
         <f>+H22^$I$2</f>
         <v>0.35897435897435898</v>
       </c>
       <c r="K22" s="7">
         <f>+J22*I22</f>
-        <v>2.8257456828885398E-2</v>
+        <v>0.15384615384615383</v>
       </c>
       <c r="L22" s="7">
         <f>+K22/SUM(K21:K22)</f>
-        <v>0.1911021233569262</v>
-      </c>
-      <c r="M22" s="36">
+        <v>0.29577464788732388</v>
+      </c>
+      <c r="M22" s="7">
         <f>+$G$2*50*L22</f>
-        <v>9.5551061678463096</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+        <v>14.788732394366194</v>
+      </c>
+      <c r="N22" s="38">
+        <f>+N19+M22</f>
+        <v>146.90399796654077</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="D24" s="10" t="s">
         <v>31</v>
       </c>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:13" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:14" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
       <c r="D25" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E25" s="33">
         <f>+SUM(M7,M10,M13,M15,M18,M21)</f>
-        <v>206.21545918125898</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.75">
+        <v>153.09600203345923</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.75">
       <c r="D26" s="13" t="s">
         <v>25</v>
       </c>
       <c r="E26" s="34">
         <f>+SUM(M8,M11,M14,M16,M19,M22)</f>
-        <v>93.784540818740979</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.75">
+        <v>146.90399796654077</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.75">
       <c r="D27" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="15">
         <f>+SUM(E25:E26)</f>
-        <v>299.99999999999994</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added PR changes and checked escrow state after 1 year and vesting
</commit_message>
<xml_diff>
--- a/20210921 - Staking Rewards.xlsx
+++ b/20210921 - Staking Rewards.xlsx
@@ -8,16 +8,100 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Documents\16slimchance16\token\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7000EF3C-7087-4169-96B0-DBBBB1BBF4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEC6D9B-B17A-40CD-85FC-1287CBCA26DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-90" windowWidth="16530" windowHeight="10980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="875" yWindow="-90" windowWidth="16495" windowHeight="10980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SNX" sheetId="1" r:id="rId1"/>
     <sheet name="SNX - Detail" sheetId="4" r:id="rId2"/>
     <sheet name="KWENTA" sheetId="5" r:id="rId3"/>
     <sheet name="KWENTA - power" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">Sheet1!$L$2:$L$138</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">Sheet1!$L$2:$L$138</definedName>
+    <definedName name="solver_lhs10" localSheetId="4" hidden="1">Sheet1!$L$19</definedName>
+    <definedName name="solver_lhs11" localSheetId="4" hidden="1">Sheet1!$L$2</definedName>
+    <definedName name="solver_lhs12" localSheetId="4" hidden="1">Sheet1!$L$3</definedName>
+    <definedName name="solver_lhs13" localSheetId="4" hidden="1">Sheet1!$L$4</definedName>
+    <definedName name="solver_lhs14" localSheetId="4" hidden="1">Sheet1!$L$5</definedName>
+    <definedName name="solver_lhs15" localSheetId="4" hidden="1">Sheet1!$L$6</definedName>
+    <definedName name="solver_lhs16" localSheetId="4" hidden="1">Sheet1!$L$7</definedName>
+    <definedName name="solver_lhs17" localSheetId="4" hidden="1">Sheet1!$L$8</definedName>
+    <definedName name="solver_lhs18" localSheetId="4" hidden="1">Sheet1!$L$9</definedName>
+    <definedName name="solver_lhs2" localSheetId="4" hidden="1">Sheet1!$L$11</definedName>
+    <definedName name="solver_lhs3" localSheetId="4" hidden="1">Sheet1!$L$12</definedName>
+    <definedName name="solver_lhs4" localSheetId="4" hidden="1">Sheet1!$L$13</definedName>
+    <definedName name="solver_lhs5" localSheetId="4" hidden="1">Sheet1!$L$14</definedName>
+    <definedName name="solver_lhs6" localSheetId="4" hidden="1">Sheet1!$L$15</definedName>
+    <definedName name="solver_lhs7" localSheetId="4" hidden="1">Sheet1!$L$16</definedName>
+    <definedName name="solver_lhs8" localSheetId="4" hidden="1">Sheet1!$L$17</definedName>
+    <definedName name="solver_lhs9" localSheetId="4" hidden="1">Sheet1!$L$18</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">Sheet1!$F$13</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel10" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel11" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel12" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel13" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel14" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel15" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel16" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel17" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel18" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel2" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel3" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel4" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel5" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel6" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel7" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel8" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rel9" localSheetId="4" hidden="1">5</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs10" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs11" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs12" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs13" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs14" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs15" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs16" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs17" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs18" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs2" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs3" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs4" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs5" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs6" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs7" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs8" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rhs9" localSheetId="4" hidden="1">"binary"</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="58">
   <si>
     <t>N stake 20</t>
   </si>
@@ -188,16 +272,42 @@
   <si>
     <t>%rewards</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>2^I</t>
+  </si>
+  <si>
+    <t>ki</t>
+  </si>
+  <si>
+    <t>fi</t>
+  </si>
+  <si>
+    <t>term</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.0000000E+00"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0000E+00"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0000000000"/>
+    <numFmt numFmtId="169" formatCode="0.0000000000000000000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -368,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -406,10 +516,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2064,8 +2177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486B17B1-BE12-4310-9A3F-24B7422EA458}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2865,4 +2978,3411 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9234254F-409F-4009-B91D-1C1F86884B03}">
+  <dimension ref="A1:O138"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="13" max="13" width="27.36328125" style="42" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1796875" style="41" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1">
+        <f>+D18</f>
+        <v>1.6253496664211535</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1">
+        <f>+INT(B1)</f>
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <f>+B2^E1</f>
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2">
+        <f>+B1-E1</f>
+        <v>0.62534966642115353</v>
+      </c>
+      <c r="G2">
+        <f>+G1*O138</f>
+        <v>3.1011697553699999</v>
+      </c>
+      <c r="J2">
+        <v>-1</v>
+      </c>
+      <c r="K2">
+        <f>2^J2</f>
+        <v>0.5</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="42">
+        <f>2^K2</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="N2">
+        <f>+IF(L2,M2,1)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="O2" s="41">
+        <f>+N2</f>
+        <v>1.4142135623730951</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="J3">
+        <v>-2</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K66" si="0">2^J3</f>
+        <v>0.25</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="42">
+        <f>2^K3</f>
+        <v>1.189207115002721</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N19" si="1">+IF(L3,M3,1)</f>
+        <v>1</v>
+      </c>
+      <c r="O3" s="41">
+        <f>+O2*N3</f>
+        <v>1.4142135623730951</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="B4">
+        <f>+B2^B1</f>
+        <v>3.0851693136000478</v>
+      </c>
+      <c r="G4" s="43">
+        <f>+G2/B4-1</f>
+        <v>5.186244300894316E-3</v>
+      </c>
+      <c r="J4">
+        <v>-3</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="42">
+        <f>2^K4</f>
+        <v>1.0905077326652577</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>1.0905077326652577</v>
+      </c>
+      <c r="O4" s="41">
+        <f t="shared" ref="O4:O19" si="2">+O3*N4</f>
+        <v>1.542210825407941</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="J5">
+        <v>-4</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="42">
+        <f>2^K5</f>
+        <v>1.0442737824274138</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O5" s="41">
+        <f t="shared" si="2"/>
+        <v>1.542210825407941</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="J6">
+        <v>-5</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="42">
+        <f t="shared" ref="M6:M19" si="3">2^K6</f>
+        <v>1.0218971486541166</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O6" s="41">
+        <f>+O5*N6</f>
+        <v>1.542210825407941</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="J7">
+        <v>-6</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="42">
+        <f t="shared" si="3"/>
+        <v>1.0108892860517005</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O7" s="41">
+        <f t="shared" si="2"/>
+        <v>1.542210825407941</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="J8">
+        <v>-7</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8" s="42">
+        <f t="shared" si="3"/>
+        <v>1.0054299011128027</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>1.0054299011128027</v>
+      </c>
+      <c r="O8" s="41">
+        <f t="shared" si="2"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="J9">
+        <v>-8</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>3.90625E-3</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="42">
+        <f t="shared" si="3"/>
+        <v>1.0027112750502025</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O9" s="41">
+        <f t="shared" si="2"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="J10">
+        <v>-9</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10" s="42">
+        <f t="shared" si="3"/>
+        <v>1.0013547198921082</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O10" s="41">
+        <f t="shared" si="2"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="J11">
+        <v>-10</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>9.765625E-4</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="42">
+        <f t="shared" si="3"/>
+        <v>1.0006771306930664</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O11" s="41">
+        <f t="shared" si="2"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12">
+        <f>+SUMPRODUCT(L2:L138,K2:K138)</f>
+        <v>0.6328125</v>
+      </c>
+      <c r="J12">
+        <v>-11</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>4.8828125E-4</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="42">
+        <f t="shared" si="3"/>
+        <v>1.0003385080526823</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O12" s="41">
+        <f t="shared" si="2"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="F13">
+        <f>+ABS(F12-E2)</f>
+        <v>7.4628335788464728E-3</v>
+      </c>
+      <c r="J13">
+        <v>-12</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>2.44140625E-4</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="42">
+        <f t="shared" si="3"/>
+        <v>1.0001692397053021</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O13" s="41">
+        <f t="shared" si="2"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="J14">
+        <v>-13</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>1.220703125E-4</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14" s="42">
+        <f t="shared" si="3"/>
+        <v>1.0000846162726944</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O14" s="41">
+        <f t="shared" si="2"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="B15">
+        <f>5^2.3</f>
+        <v>40.516414917319047</v>
+      </c>
+      <c r="D15">
+        <f>5^0.7</f>
+        <v>3.0851693136000478</v>
+      </c>
+      <c r="J15">
+        <v>-14</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>6.103515625E-5</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15" s="42">
+        <f t="shared" si="3"/>
+        <v>1.0000423072413958</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O15" s="41">
+        <f t="shared" si="2"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
+      <c r="J16">
+        <v>-15</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>3.0517578125E-5</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16" s="42">
+        <f t="shared" si="3"/>
+        <v>1.0000211533969647</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O16" s="41">
+        <f t="shared" si="2"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B17">
+        <f>+LOG(5, 2)</f>
+        <v>2.3219280948873622</v>
+      </c>
+      <c r="D17">
+        <f>+LOG(5, 2)</f>
+        <v>2.3219280948873622</v>
+      </c>
+      <c r="J17">
+        <v>-16</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17" s="42">
+        <f t="shared" si="3"/>
+        <v>1.0000105766425498</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O17" s="41">
+        <f t="shared" si="2"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B18">
+        <f>+B17*2.3</f>
+        <v>5.3404346182409324</v>
+      </c>
+      <c r="D18">
+        <f>+D17*0.7</f>
+        <v>1.6253496664211535</v>
+      </c>
+      <c r="J18">
+        <v>-17</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>7.62939453125E-6</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18" s="42">
+        <f t="shared" si="3"/>
+        <v>1.0000052883072919</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O18" s="41">
+        <f t="shared" si="2"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B19">
+        <f>2^B18</f>
+        <v>40.516414917319025</v>
+      </c>
+      <c r="D19">
+        <f>2^D18</f>
+        <v>3.0851693136000478</v>
+      </c>
+      <c r="J19">
+        <v>-18</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>3.814697265625E-6</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19" s="42">
+        <f t="shared" si="3"/>
+        <v>1.0000026441501502</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O19" s="41">
+        <f t="shared" si="2"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="J20">
+        <v>-19</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>1.9073486328125E-6</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20" s="42">
+        <f t="shared" ref="M20:M83" si="4">2^K20</f>
+        <v>1.0000013220742012</v>
+      </c>
+      <c r="N20">
+        <f t="shared" ref="N20:N83" si="5">+IF(L20,M20,1)</f>
+        <v>1</v>
+      </c>
+      <c r="O20" s="41">
+        <f t="shared" ref="O20:O83" si="6">+O19*N20</f>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="J21">
+        <v>-20</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000006610368821</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O21" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="J22">
+        <v>-21</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>4.76837158203125E-7</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000003305183864</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O22" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="J23">
+        <v>-22</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>2.384185791015625E-7</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000001652591795</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O23" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="J24">
+        <v>-23</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>1.1920928955078125E-7</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000826295863</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O24" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="J25">
+        <v>-24</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>5.9604644775390625E-8</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000413147923</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O25" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="J26">
+        <v>-25</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>2.9802322387695313E-8</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26" s="42">
+        <f t="shared" si="4"/>
+        <v>1.000000020657396</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O26" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="J27">
+        <v>-26</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>1.4901161193847656E-8</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000103286979</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O27" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="J28">
+        <v>-27</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>7.4505805969238281E-9</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000051643489</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O28" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="J29">
+        <v>-28</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>3.7252902984619141E-9</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000025821745</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O29" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="J30">
+        <v>-29</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>1.862645149230957E-9</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000012910872</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O30" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="J31">
+        <v>-30</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>9.3132257461547852E-10</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000006455436</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O31" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="J32">
+        <v>-31</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>4.6566128730773926E-10</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000003227718</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O32" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="33" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J33">
+        <v>-32</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>2.3283064365386963E-10</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000001613858</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O33" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="34" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J34">
+        <v>-33</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="0"/>
+        <v>1.1641532182693481E-10</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34" s="42">
+        <f t="shared" si="4"/>
+        <v>1.000000000080693</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O34" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="35" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J35">
+        <v>-34</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>5.8207660913467407E-11</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000403464</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O35" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="36" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J36">
+        <v>-35</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="0"/>
+        <v>2.9103830456733704E-11</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000201732</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O36" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="37" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J37">
+        <v>-36</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="0"/>
+        <v>1.4551915228366852E-11</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000100866</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O37" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="38" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J38">
+        <v>-37</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="0"/>
+        <v>7.2759576141834259E-12</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000050433</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O38" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="39" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J39">
+        <v>-38</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>3.637978807091713E-12</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000025218</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O39" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="40" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J40">
+        <v>-39</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="0"/>
+        <v>1.8189894035458565E-12</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000012608</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O40" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="41" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J41">
+        <v>-40</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="0"/>
+        <v>9.0949470177292824E-13</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000006304</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O41" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="42" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J42">
+        <v>-41</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="0"/>
+        <v>4.5474735088646412E-13</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000003153</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O42" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="43" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J43">
+        <v>-42</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="0"/>
+        <v>2.2737367544323206E-13</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000001577</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O43" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="44" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J44">
+        <v>-43</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="0"/>
+        <v>1.1368683772161603E-13</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000788</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O44" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="45" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J45">
+        <v>-44</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="0"/>
+        <v>5.6843418860808015E-14</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000393</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O45" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="46" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J46">
+        <v>-45</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="0"/>
+        <v>2.8421709430404007E-14</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000198</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O46" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="47" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J47">
+        <v>-46</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="0"/>
+        <v>1.4210854715202004E-14</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000098</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O47" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="48" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J48">
+        <v>-47</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="0"/>
+        <v>7.1054273576010019E-15</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000049</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O48" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="49" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J49">
+        <v>-48</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="0"/>
+        <v>3.5527136788005009E-15</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000024</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O49" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="50" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J50">
+        <v>-49</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="0"/>
+        <v>1.7763568394002505E-15</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000013</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O50" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="51" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J51">
+        <v>-50</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="0"/>
+        <v>8.8817841970012523E-16</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000007</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O51" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="52" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J52">
+        <v>-51</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="0"/>
+        <v>4.4408920985006262E-16</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O52" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="53" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J53">
+        <v>-52</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="0"/>
+        <v>2.2204460492503131E-16</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53" s="42">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O53" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="54" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J54">
+        <v>-53</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="0"/>
+        <v>1.1102230246251565E-16</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O54" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="55" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J55">
+        <v>-54</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="0"/>
+        <v>5.5511151231257827E-17</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O55" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="56" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J56">
+        <v>-55</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="0"/>
+        <v>2.7755575615628914E-17</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O56" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="57" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J57">
+        <v>-56</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="0"/>
+        <v>1.3877787807814457E-17</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O57" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="58" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J58">
+        <v>-57</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="0"/>
+        <v>6.9388939039072284E-18</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O58" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="59" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J59">
+        <v>-58</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="0"/>
+        <v>3.4694469519536142E-18</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O59" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="60" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J60">
+        <v>-59</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="0"/>
+        <v>1.7347234759768071E-18</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O60" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="61" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J61">
+        <v>-60</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="0"/>
+        <v>8.6736173798840355E-19</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O61" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="62" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J62">
+        <v>-61</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="0"/>
+        <v>4.3368086899420177E-19</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O62" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="63" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J63">
+        <v>-62</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="0"/>
+        <v>2.1684043449710089E-19</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O63" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="64" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J64">
+        <v>-63</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="0"/>
+        <v>1.0842021724855044E-19</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O64" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="65" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J65">
+        <v>-64</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="0"/>
+        <v>5.4210108624275222E-20</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O65" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="66" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J66">
+        <v>-65</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="0"/>
+        <v>2.7105054312137611E-20</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O66" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="67" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J67">
+        <v>-66</v>
+      </c>
+      <c r="K67">
+        <f t="shared" ref="K67:K130" si="7">2^J67</f>
+        <v>1.3552527156068805E-20</v>
+      </c>
+      <c r="L67">
+        <v>0</v>
+      </c>
+      <c r="M67" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O67" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="68" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J68">
+        <v>-67</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="7"/>
+        <v>6.7762635780344027E-21</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O68" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="69" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J69">
+        <v>-68</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="7"/>
+        <v>3.3881317890172014E-21</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O69" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="70" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J70">
+        <v>-69</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="7"/>
+        <v>1.6940658945086007E-21</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O70" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="71" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J71">
+        <v>-70</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="7"/>
+        <v>8.4703294725430034E-22</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O71" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="72" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J72">
+        <v>-71</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="7"/>
+        <v>4.2351647362715017E-22</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O72" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="73" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J73">
+        <v>-72</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="7"/>
+        <v>2.1175823681357508E-22</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O73" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="74" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J74">
+        <v>-73</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="7"/>
+        <v>1.0587911840678754E-22</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O74" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="75" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J75">
+        <v>-74</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="7"/>
+        <v>5.2939559203393771E-23</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N75">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O75" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="76" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J76">
+        <v>-75</v>
+      </c>
+      <c r="K76">
+        <f t="shared" si="7"/>
+        <v>2.6469779601696886E-23</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N76">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O76" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="77" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J77">
+        <v>-76</v>
+      </c>
+      <c r="K77">
+        <f t="shared" si="7"/>
+        <v>1.3234889800848443E-23</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N77">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O77" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="78" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J78">
+        <v>-77</v>
+      </c>
+      <c r="K78">
+        <f t="shared" si="7"/>
+        <v>6.6174449004242214E-24</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N78">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O78" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="79" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J79">
+        <v>-78</v>
+      </c>
+      <c r="K79">
+        <f t="shared" si="7"/>
+        <v>3.3087224502121107E-24</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N79">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O79" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="80" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J80">
+        <v>-79</v>
+      </c>
+      <c r="K80">
+        <f t="shared" si="7"/>
+        <v>1.6543612251060553E-24</v>
+      </c>
+      <c r="L80">
+        <v>0</v>
+      </c>
+      <c r="M80" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N80">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O80" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="81" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J81">
+        <v>-80</v>
+      </c>
+      <c r="K81">
+        <f t="shared" si="7"/>
+        <v>8.2718061255302767E-25</v>
+      </c>
+      <c r="L81">
+        <v>0</v>
+      </c>
+      <c r="M81" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N81">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O81" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="82" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J82">
+        <v>-81</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="7"/>
+        <v>4.1359030627651384E-25</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N82">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O82" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="83" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J83">
+        <v>-82</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="7"/>
+        <v>2.0679515313825692E-25</v>
+      </c>
+      <c r="L83">
+        <v>0</v>
+      </c>
+      <c r="M83" s="42">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N83">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O83" s="41">
+        <f t="shared" si="6"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="84" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J84">
+        <v>-83</v>
+      </c>
+      <c r="K84">
+        <f t="shared" si="7"/>
+        <v>1.0339757656912846E-25</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84" s="42">
+        <f t="shared" ref="M84:M138" si="8">2^K84</f>
+        <v>1</v>
+      </c>
+      <c r="N84">
+        <f t="shared" ref="N84:N138" si="9">+IF(L84,M84,1)</f>
+        <v>1</v>
+      </c>
+      <c r="O84" s="41">
+        <f t="shared" ref="O84:O138" si="10">+O83*N84</f>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="85" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J85">
+        <v>-84</v>
+      </c>
+      <c r="K85">
+        <f t="shared" si="7"/>
+        <v>5.169878828456423E-26</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N85">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O85" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="86" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J86">
+        <v>-85</v>
+      </c>
+      <c r="K86">
+        <f t="shared" si="7"/>
+        <v>2.5849394142282115E-26</v>
+      </c>
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N86">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O86" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="87" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J87">
+        <v>-86</v>
+      </c>
+      <c r="K87">
+        <f t="shared" si="7"/>
+        <v>1.2924697071141057E-26</v>
+      </c>
+      <c r="L87">
+        <v>0</v>
+      </c>
+      <c r="M87" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N87">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O87" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="88" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J88">
+        <v>-87</v>
+      </c>
+      <c r="K88">
+        <f t="shared" si="7"/>
+        <v>6.4623485355705287E-27</v>
+      </c>
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N88">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O88" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="89" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J89">
+        <v>-88</v>
+      </c>
+      <c r="K89">
+        <f t="shared" si="7"/>
+        <v>3.2311742677852644E-27</v>
+      </c>
+      <c r="L89">
+        <v>0</v>
+      </c>
+      <c r="M89" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N89">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O89" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="90" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J90">
+        <v>-89</v>
+      </c>
+      <c r="K90">
+        <f t="shared" si="7"/>
+        <v>1.6155871338926322E-27</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N90">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O90" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="91" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J91">
+        <v>-90</v>
+      </c>
+      <c r="K91">
+        <f t="shared" si="7"/>
+        <v>8.0779356694631609E-28</v>
+      </c>
+      <c r="L91">
+        <v>0</v>
+      </c>
+      <c r="M91" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N91">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O91" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="92" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J92">
+        <v>-91</v>
+      </c>
+      <c r="K92">
+        <f t="shared" si="7"/>
+        <v>4.0389678347315804E-28</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+      <c r="M92" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N92">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O92" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="93" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J93">
+        <v>-92</v>
+      </c>
+      <c r="K93">
+        <f t="shared" si="7"/>
+        <v>2.0194839173657902E-28</v>
+      </c>
+      <c r="L93">
+        <v>0</v>
+      </c>
+      <c r="M93" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N93">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O93" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="94" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J94">
+        <v>-93</v>
+      </c>
+      <c r="K94">
+        <f t="shared" si="7"/>
+        <v>1.0097419586828951E-28</v>
+      </c>
+      <c r="L94">
+        <v>0</v>
+      </c>
+      <c r="M94" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N94">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O94" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="95" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J95">
+        <v>-94</v>
+      </c>
+      <c r="K95">
+        <f t="shared" si="7"/>
+        <v>5.0487097934144756E-29</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+      <c r="M95" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N95">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O95" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="96" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J96">
+        <v>-95</v>
+      </c>
+      <c r="K96">
+        <f t="shared" si="7"/>
+        <v>2.5243548967072378E-29</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N96">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O96" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="97" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J97">
+        <v>-96</v>
+      </c>
+      <c r="K97">
+        <f t="shared" si="7"/>
+        <v>1.2621774483536189E-29</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+      <c r="M97" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N97">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O97" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="98" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J98">
+        <v>-97</v>
+      </c>
+      <c r="K98">
+        <f t="shared" si="7"/>
+        <v>6.3108872417680944E-30</v>
+      </c>
+      <c r="L98">
+        <v>0</v>
+      </c>
+      <c r="M98" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N98">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O98" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="99" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J99">
+        <v>-98</v>
+      </c>
+      <c r="K99">
+        <f t="shared" si="7"/>
+        <v>3.1554436208840472E-30</v>
+      </c>
+      <c r="L99">
+        <v>0</v>
+      </c>
+      <c r="M99" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N99">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O99" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="100" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J100">
+        <v>-99</v>
+      </c>
+      <c r="K100">
+        <f t="shared" si="7"/>
+        <v>1.5777218104420236E-30</v>
+      </c>
+      <c r="L100">
+        <v>0</v>
+      </c>
+      <c r="M100" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N100">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O100" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="101" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J101">
+        <v>-100</v>
+      </c>
+      <c r="K101">
+        <f t="shared" si="7"/>
+        <v>7.8886090522101181E-31</v>
+      </c>
+      <c r="L101">
+        <v>0</v>
+      </c>
+      <c r="M101" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N101">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O101" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="102" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J102">
+        <v>-101</v>
+      </c>
+      <c r="K102">
+        <f t="shared" si="7"/>
+        <v>3.944304526105059E-31</v>
+      </c>
+      <c r="L102">
+        <v>0</v>
+      </c>
+      <c r="M102" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N102">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O102" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="103" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J103">
+        <v>-102</v>
+      </c>
+      <c r="K103">
+        <f t="shared" si="7"/>
+        <v>1.9721522630525295E-31</v>
+      </c>
+      <c r="L103">
+        <v>0</v>
+      </c>
+      <c r="M103" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N103">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O103" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="104" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J104">
+        <v>-103</v>
+      </c>
+      <c r="K104">
+        <f t="shared" si="7"/>
+        <v>9.8607613152626476E-32</v>
+      </c>
+      <c r="L104">
+        <v>0</v>
+      </c>
+      <c r="M104" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N104">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O104" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="105" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J105">
+        <v>-104</v>
+      </c>
+      <c r="K105">
+        <f t="shared" si="7"/>
+        <v>4.9303806576313238E-32</v>
+      </c>
+      <c r="L105">
+        <v>0</v>
+      </c>
+      <c r="M105" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N105">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O105" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="106" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J106">
+        <v>-105</v>
+      </c>
+      <c r="K106">
+        <f t="shared" si="7"/>
+        <v>2.4651903288156619E-32</v>
+      </c>
+      <c r="L106">
+        <v>0</v>
+      </c>
+      <c r="M106" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N106">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O106" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="107" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J107">
+        <v>-106</v>
+      </c>
+      <c r="K107">
+        <f t="shared" si="7"/>
+        <v>1.2325951644078309E-32</v>
+      </c>
+      <c r="L107">
+        <v>0</v>
+      </c>
+      <c r="M107" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N107">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O107" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="108" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J108">
+        <v>-107</v>
+      </c>
+      <c r="K108">
+        <f t="shared" si="7"/>
+        <v>6.1629758220391547E-33</v>
+      </c>
+      <c r="L108">
+        <v>0</v>
+      </c>
+      <c r="M108" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N108">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O108" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="109" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J109">
+        <v>-108</v>
+      </c>
+      <c r="K109">
+        <f t="shared" si="7"/>
+        <v>3.0814879110195774E-33</v>
+      </c>
+      <c r="L109">
+        <v>0</v>
+      </c>
+      <c r="M109" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N109">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O109" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="110" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J110">
+        <v>-109</v>
+      </c>
+      <c r="K110">
+        <f t="shared" si="7"/>
+        <v>1.5407439555097887E-33</v>
+      </c>
+      <c r="L110">
+        <v>0</v>
+      </c>
+      <c r="M110" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N110">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O110" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="111" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J111">
+        <v>-110</v>
+      </c>
+      <c r="K111">
+        <f t="shared" si="7"/>
+        <v>7.7037197775489434E-34</v>
+      </c>
+      <c r="L111">
+        <v>0</v>
+      </c>
+      <c r="M111" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N111">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O111" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="112" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J112">
+        <v>-111</v>
+      </c>
+      <c r="K112">
+        <f t="shared" si="7"/>
+        <v>3.8518598887744717E-34</v>
+      </c>
+      <c r="L112">
+        <v>0</v>
+      </c>
+      <c r="M112" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N112">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O112" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="113" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J113">
+        <v>-112</v>
+      </c>
+      <c r="K113">
+        <f t="shared" si="7"/>
+        <v>1.9259299443872359E-34</v>
+      </c>
+      <c r="L113">
+        <v>0</v>
+      </c>
+      <c r="M113" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N113">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O113" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="114" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J114">
+        <v>-113</v>
+      </c>
+      <c r="K114">
+        <f t="shared" si="7"/>
+        <v>9.6296497219361793E-35</v>
+      </c>
+      <c r="L114">
+        <v>0</v>
+      </c>
+      <c r="M114" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N114">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O114" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="115" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J115">
+        <v>-114</v>
+      </c>
+      <c r="K115">
+        <f t="shared" si="7"/>
+        <v>4.8148248609680896E-35</v>
+      </c>
+      <c r="L115">
+        <v>0</v>
+      </c>
+      <c r="M115" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N115">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O115" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="116" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J116">
+        <v>-115</v>
+      </c>
+      <c r="K116">
+        <f t="shared" si="7"/>
+        <v>2.4074124304840448E-35</v>
+      </c>
+      <c r="L116">
+        <v>0</v>
+      </c>
+      <c r="M116" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N116">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O116" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="117" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J117">
+        <v>-116</v>
+      </c>
+      <c r="K117">
+        <f t="shared" si="7"/>
+        <v>1.2037062152420224E-35</v>
+      </c>
+      <c r="L117">
+        <v>0</v>
+      </c>
+      <c r="M117" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N117">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O117" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="118" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J118">
+        <v>-117</v>
+      </c>
+      <c r="K118">
+        <f t="shared" si="7"/>
+        <v>6.018531076210112E-36</v>
+      </c>
+      <c r="L118">
+        <v>0</v>
+      </c>
+      <c r="M118" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N118">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O118" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="119" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J119">
+        <v>-118</v>
+      </c>
+      <c r="K119">
+        <f t="shared" si="7"/>
+        <v>3.009265538105056E-36</v>
+      </c>
+      <c r="L119">
+        <v>0</v>
+      </c>
+      <c r="M119" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N119">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O119" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="120" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J120">
+        <v>-119</v>
+      </c>
+      <c r="K120">
+        <f t="shared" si="7"/>
+        <v>1.504632769052528E-36</v>
+      </c>
+      <c r="L120">
+        <v>0</v>
+      </c>
+      <c r="M120" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N120">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O120" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="121" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J121">
+        <v>-120</v>
+      </c>
+      <c r="K121">
+        <f t="shared" si="7"/>
+        <v>7.5231638452626401E-37</v>
+      </c>
+      <c r="L121">
+        <v>0</v>
+      </c>
+      <c r="M121" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N121">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O121" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="122" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J122">
+        <v>-121</v>
+      </c>
+      <c r="K122">
+        <f t="shared" si="7"/>
+        <v>3.76158192263132E-37</v>
+      </c>
+      <c r="L122">
+        <v>0</v>
+      </c>
+      <c r="M122" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N122">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O122" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="123" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J123">
+        <v>-122</v>
+      </c>
+      <c r="K123">
+        <f t="shared" si="7"/>
+        <v>1.88079096131566E-37</v>
+      </c>
+      <c r="L123">
+        <v>0</v>
+      </c>
+      <c r="M123" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N123">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O123" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="124" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J124">
+        <v>-123</v>
+      </c>
+      <c r="K124">
+        <f t="shared" si="7"/>
+        <v>9.4039548065783001E-38</v>
+      </c>
+      <c r="L124">
+        <v>0</v>
+      </c>
+      <c r="M124" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N124">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O124" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="125" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J125">
+        <v>-124</v>
+      </c>
+      <c r="K125">
+        <f t="shared" si="7"/>
+        <v>4.70197740328915E-38</v>
+      </c>
+      <c r="L125">
+        <v>0</v>
+      </c>
+      <c r="M125" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N125">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O125" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="126" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J126">
+        <v>-125</v>
+      </c>
+      <c r="K126">
+        <f t="shared" si="7"/>
+        <v>2.350988701644575E-38</v>
+      </c>
+      <c r="L126">
+        <v>0</v>
+      </c>
+      <c r="M126" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N126">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O126" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="127" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J127">
+        <v>-126</v>
+      </c>
+      <c r="K127">
+        <f t="shared" si="7"/>
+        <v>1.1754943508222875E-38</v>
+      </c>
+      <c r="L127">
+        <v>0</v>
+      </c>
+      <c r="M127" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N127">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O127" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="128" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J128">
+        <v>-127</v>
+      </c>
+      <c r="K128">
+        <f t="shared" si="7"/>
+        <v>5.8774717541114375E-39</v>
+      </c>
+      <c r="L128">
+        <v>0</v>
+      </c>
+      <c r="M128" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N128">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O128" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="129" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J129">
+        <v>-128</v>
+      </c>
+      <c r="K129">
+        <f t="shared" si="7"/>
+        <v>2.9387358770557188E-39</v>
+      </c>
+      <c r="L129">
+        <v>0</v>
+      </c>
+      <c r="M129" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N129">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O129" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="130" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J130">
+        <v>-129</v>
+      </c>
+      <c r="K130">
+        <f t="shared" si="7"/>
+        <v>1.4693679385278594E-39</v>
+      </c>
+      <c r="L130">
+        <v>0</v>
+      </c>
+      <c r="M130" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N130">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O130" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="131" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J131">
+        <v>-130</v>
+      </c>
+      <c r="K131">
+        <f t="shared" ref="K131:K138" si="11">2^J131</f>
+        <v>7.3468396926392969E-40</v>
+      </c>
+      <c r="L131">
+        <v>0</v>
+      </c>
+      <c r="M131" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N131">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O131" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="132" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J132">
+        <v>-131</v>
+      </c>
+      <c r="K132">
+        <f t="shared" si="11"/>
+        <v>3.6734198463196485E-40</v>
+      </c>
+      <c r="L132">
+        <v>0</v>
+      </c>
+      <c r="M132" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N132">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O132" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="133" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J133">
+        <v>-132</v>
+      </c>
+      <c r="K133">
+        <f t="shared" si="11"/>
+        <v>1.8367099231598242E-40</v>
+      </c>
+      <c r="L133">
+        <v>0</v>
+      </c>
+      <c r="M133" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N133">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O133" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="134" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J134">
+        <v>-133</v>
+      </c>
+      <c r="K134">
+        <f t="shared" si="11"/>
+        <v>9.1835496157991212E-41</v>
+      </c>
+      <c r="L134">
+        <v>0</v>
+      </c>
+      <c r="M134" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N134">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O134" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="135" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J135">
+        <v>-134</v>
+      </c>
+      <c r="K135">
+        <f t="shared" si="11"/>
+        <v>4.5917748078995606E-41</v>
+      </c>
+      <c r="L135">
+        <v>0</v>
+      </c>
+      <c r="M135" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N135">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O135" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="136" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J136">
+        <v>-135</v>
+      </c>
+      <c r="K136">
+        <f t="shared" si="11"/>
+        <v>2.2958874039497803E-41</v>
+      </c>
+      <c r="L136">
+        <v>0</v>
+      </c>
+      <c r="M136" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N136">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O136" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="137" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J137">
+        <v>-136</v>
+      </c>
+      <c r="K137">
+        <f t="shared" si="11"/>
+        <v>1.1479437019748901E-41</v>
+      </c>
+      <c r="L137">
+        <v>0</v>
+      </c>
+      <c r="M137" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N137">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O137" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+    <row r="138" spans="10:15" x14ac:dyDescent="0.75">
+      <c r="J138">
+        <v>-137</v>
+      </c>
+      <c r="K138">
+        <f t="shared" si="11"/>
+        <v>5.7397185098744507E-42</v>
+      </c>
+      <c r="L138">
+        <v>0</v>
+      </c>
+      <c r="M138" s="42">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N138">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O138" s="41">
+        <f t="shared" si="10"/>
+        <v>1.550584877685</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes from jmonteer PR3
</commit_message>
<xml_diff>
--- a/20210921 - Staking Rewards.xlsx
+++ b/20210921 - Staking Rewards.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Documents\16slimchance16\token\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90476539-49F8-415F-88C1-9FB7CF0D1F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71580DC1-7491-4FF4-B0A5-8708B1AA2928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-90" windowWidth="16530" windowHeight="10980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-90" windowWidth="16530" windowHeight="10980" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SNX" sheetId="1" r:id="rId1"/>
-    <sheet name="SNX - Detail" sheetId="4" r:id="rId2"/>
-    <sheet name="KWENTA" sheetId="5" r:id="rId3"/>
+    <sheet name="SNX" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="SNX - Detail" sheetId="4" state="hidden" r:id="rId2"/>
+    <sheet name="KWENTA" sheetId="5" state="hidden" r:id="rId3"/>
     <sheet name="KWENTA - power" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -193,11 +193,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000000E+00"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0000E+00"/>
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -368,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -410,6 +411,11 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1449,7 +1455,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C10" sqref="A1:XFD1048576"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2062,802 +2068,819 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486B17B1-BE12-4310-9A3F-24B7422EA458}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="B2:O28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.40625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.26953125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.54296875" style="26" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.1328125" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.58984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.31640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.54296875" style="26" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A1" s="4" t="s">
+    <row r="2" spans="2:15" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="E1" s="5" t="s">
+      <c r="D2" s="4"/>
+      <c r="F2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="2:15" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2">
+      <c r="C3">
         <v>25</v>
       </c>
-      <c r="E2">
+      <c r="F3">
         <v>300</v>
       </c>
-      <c r="F2">
+      <c r="G3">
         <v>300</v>
       </c>
-      <c r="G2">
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="I3">
         <v>0.7</v>
       </c>
-      <c r="I2">
+      <c r="J3">
         <v>0.3</v>
       </c>
-      <c r="M2" s="30"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A3" s="3" t="s">
+      <c r="N3" s="30"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3">
+      <c r="C4">
         <v>50</v>
       </c>
-      <c r="N3" s="9"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A4" s="8"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A6" s="16" t="s">
+      <c r="O4" s="9"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B5" s="8"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B7" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="C7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D7" s="17"/>
+      <c r="E7" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="F7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="G7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="H7" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="I7" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="J7" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="K7" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="L7" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="M7" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="39" t="s">
+      <c r="N7" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="40" t="s">
+      <c r="O7" s="40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A7" s="12">
-        <v>0</v>
-      </c>
-      <c r="B7" s="23" t="s">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B8" s="44">
+        <v>0</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="12" t="s">
+      <c r="D8" s="20"/>
+      <c r="E8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="20">
-        <v>10</v>
-      </c>
-      <c r="F7" s="21">
+      <c r="F8" s="20">
+        <v>1E+19</v>
+      </c>
+      <c r="G8" s="21">
         <v>2.5E+19</v>
       </c>
-      <c r="G7" s="22">
-        <f>+E7/SUM(E7:E8)</f>
+      <c r="H8" s="22">
+        <f>+F8/SUM(F8:F9)</f>
         <v>0.5</v>
       </c>
-      <c r="H7" s="22">
-        <f>+F7/SUM(F7:F8)</f>
+      <c r="I8" s="22">
+        <f>+G8/SUM(G8:G9)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I7" s="22">
-        <f>+G7^$H$2</f>
+      <c r="J8" s="22">
+        <f>+H8^$I$3</f>
         <v>0.61557220667245816</v>
       </c>
-      <c r="J7" s="22">
-        <f>+H7^$I$2</f>
+      <c r="K8" s="22">
+        <f>+I8^$J$3</f>
         <v>0.71922309332486434</v>
       </c>
-      <c r="K7" s="22">
-        <f>+J7*I7</f>
+      <c r="L8" s="22">
+        <f>+K8*J8</f>
         <v>0.44273374664777804</v>
       </c>
-      <c r="L7" s="36">
-        <f>+K7/SUM(K7:K8)</f>
+      <c r="M8" s="36">
+        <f>+L8/SUM(L8:L9)</f>
         <v>0.44820048133989088</v>
       </c>
-      <c r="M7" s="22">
-        <f>+$G$2*60*L7</f>
+      <c r="N8" s="22">
+        <f>+$H$3*60*M8</f>
         <v>26.892028880393454</v>
       </c>
-      <c r="N7" s="35">
-        <f>+M7</f>
+      <c r="O8" s="35">
+        <f>+N8</f>
         <v>26.892028880393454</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A8" s="12"/>
-      <c r="B8" s="23"/>
-      <c r="D8" s="12" t="s">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B9" s="44"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="20">
-        <v>10</v>
-      </c>
-      <c r="F8" s="21">
+      <c r="F9" s="20">
+        <v>1E+19</v>
+      </c>
+      <c r="G9" s="21">
         <v>5E+19</v>
       </c>
-      <c r="G8" s="22">
-        <f>+E8/SUM(E7:E8)</f>
+      <c r="H9" s="22">
+        <f>+F9/SUM(F8:F9)</f>
         <v>0.5</v>
       </c>
-      <c r="H8" s="22">
-        <f>+F8/SUM(F7:F8)</f>
+      <c r="I9" s="22">
+        <f>+G9/SUM(G8:G9)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="I8" s="22">
-        <f>+G8^$H$2</f>
+      <c r="J9" s="22">
+        <f>+H9^$I$3</f>
         <v>0.61557220667245816</v>
       </c>
-      <c r="J8" s="22">
-        <f>+H8^$I$2</f>
+      <c r="K9" s="22">
+        <f>+I9^$J$3</f>
         <v>0.88546749329555607</v>
       </c>
-      <c r="K8" s="22">
-        <f>+J8*I8</f>
+      <c r="L9" s="22">
+        <f>+K9*J9</f>
         <v>0.54506917878467553</v>
       </c>
-      <c r="L8" s="36">
-        <f>+K8/SUM(K7:K8)</f>
+      <c r="M9" s="36">
+        <f>+L9/SUM(L8:L9)</f>
         <v>0.55179951866010912</v>
       </c>
-      <c r="M8" s="22">
-        <f>+$G$2*60*L8</f>
+      <c r="N9" s="22">
+        <f>+$H$3*60*M9</f>
         <v>33.107971119606546</v>
       </c>
-      <c r="N8" s="35">
-        <f>+M8</f>
+      <c r="O9" s="35">
+        <f>+N9</f>
         <v>33.107971119606546</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A9" s="12">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B10" s="44">
         <v>60</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="C10" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="23"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A10" s="12"/>
-      <c r="B10" s="23"/>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="20"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="23"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B11" s="44"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="20">
-        <v>50</v>
-      </c>
-      <c r="F10" s="21">
+      <c r="F11" s="20">
+        <v>5E+19</v>
+      </c>
+      <c r="G11" s="21">
         <v>2.5E+19</v>
       </c>
-      <c r="G10" s="22">
-        <f>+E10/SUM(E10:E11)</f>
+      <c r="H11" s="22">
+        <f>+F11/SUM(F11:F12)</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="H10" s="22">
-        <f>+F10/SUM(F10:F11)</f>
+      <c r="I11" s="22">
+        <f>+G11/SUM(G11:G12)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I10" s="22">
-        <f>+G10^$H$2</f>
+      <c r="J11" s="22">
+        <f>+H11^$I$3</f>
         <v>0.88018330703271519</v>
       </c>
-      <c r="J10" s="22">
-        <f>+H10^$I$2</f>
+      <c r="K11" s="22">
+        <f>+I11^$J$3</f>
         <v>0.71922309332486434</v>
       </c>
-      <c r="K10" s="22">
-        <f>+J10*I10</f>
+      <c r="L11" s="22">
+        <f>+K11*J11</f>
         <v>0.63304816077697823</v>
       </c>
-      <c r="L10" s="22">
-        <f>+K10/SUM(K10:K11)</f>
+      <c r="M11" s="22">
+        <f>+L11/SUM(L11:L12)</f>
         <v>0.71476947895159004</v>
       </c>
-      <c r="M10" s="22">
-        <f>+$G$2*60*L10</f>
+      <c r="N11" s="22">
+        <f>+$H$3*60*M11</f>
         <v>42.886168737095403</v>
       </c>
-      <c r="N10" s="37">
-        <f>+M10+M7</f>
+      <c r="O11" s="37">
+        <f>+N11+N8</f>
         <v>69.778197617488857</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A11" s="12"/>
-      <c r="B11" s="23"/>
-      <c r="D11" s="12" t="s">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B12" s="44"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="20">
-        <v>10</v>
-      </c>
-      <c r="F11" s="21">
+      <c r="F12" s="20">
+        <v>1E+19</v>
+      </c>
+      <c r="G12" s="21">
         <v>5E+19</v>
       </c>
-      <c r="G11" s="22">
-        <f>+E11/SUM(E10:E11)</f>
+      <c r="H12" s="22">
+        <f>+F12/SUM(F11:F12)</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="H11" s="22">
-        <f>+F11/SUM(F10:F11)</f>
+      <c r="I12" s="22">
+        <f>+G12/SUM(G11:G12)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="I11" s="22">
-        <f>+G11^$H$2</f>
+      <c r="J12" s="22">
+        <f>+H12^$I$3</f>
         <v>0.28529497656828423</v>
       </c>
-      <c r="J11" s="22">
-        <f>+H11^$I$2</f>
+      <c r="K12" s="22">
+        <f>+I12^$J$3</f>
         <v>0.88546749329555607</v>
       </c>
-      <c r="K11" s="22">
-        <f>+J11*I11</f>
+      <c r="L12" s="22">
+        <f>+K12*J12</f>
         <v>0.25261942775173307</v>
       </c>
-      <c r="L11" s="22">
-        <f>+K11/SUM(K10:K11)</f>
+      <c r="M12" s="22">
+        <f>+L12/SUM(L11:L12)</f>
         <v>0.28523052104840996</v>
       </c>
-      <c r="M11" s="22">
-        <f>+$G$2*60*L11</f>
+      <c r="N12" s="22">
+        <f>+$H$3*60*M12</f>
         <v>17.113831262904597</v>
       </c>
-      <c r="N11" s="37">
-        <f>+M11+M8</f>
+      <c r="O12" s="37">
+        <f>+N12+N9</f>
         <v>50.221802382511143</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A12" s="12">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B13" s="44">
         <v>120</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="C13" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="23"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A13" s="12"/>
-      <c r="B13" s="23"/>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="20"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="23"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B14" s="44"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="20">
-        <v>50</v>
-      </c>
-      <c r="F13" s="21">
+      <c r="F14" s="20">
+        <v>5E+19</v>
+      </c>
+      <c r="G14" s="21">
         <v>2.5E+19</v>
       </c>
-      <c r="G13" s="22">
-        <f>+E13/SUM(E13:E14)</f>
+      <c r="H14" s="22">
+        <f>+F14/SUM(F14:F15)</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="H13" s="22">
-        <f>+F13/SUM(F13:F14)</f>
+      <c r="I14" s="22">
+        <f>+G14/SUM(G14:G15)</f>
         <v>0.26315789473684209</v>
       </c>
-      <c r="I13" s="22">
-        <f>+G13^$H$2</f>
+      <c r="J14" s="22">
+        <f>+H14^$I$3</f>
         <v>0.88018330703271519</v>
       </c>
-      <c r="J13" s="22">
-        <f>+H13^$I$2</f>
+      <c r="K14" s="22">
+        <f>+I14^$J$3</f>
         <v>0.66998475538030788</v>
       </c>
-      <c r="K13" s="22">
-        <f>+J13*I13</f>
+      <c r="L14" s="22">
+        <f>+K14*J14</f>
         <v>0.58970939765214414</v>
       </c>
-      <c r="L13" s="22">
-        <f>+K13/SUM(K13:K14)</f>
+      <c r="M14" s="22">
+        <f>+L14/SUM(L14:L15)</f>
         <v>0.69375229677182093</v>
       </c>
-      <c r="M13" s="22">
-        <f>+$G$2*30*L13</f>
+      <c r="N14" s="22">
+        <f>+$H$3*30*M14</f>
         <v>20.812568903154627</v>
       </c>
-      <c r="N13" s="37">
-        <f>+N10+M13</f>
+      <c r="O14" s="37">
+        <f>+O11+N14</f>
         <v>90.590766520643484</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A14" s="12"/>
-      <c r="B14" s="23"/>
-      <c r="D14" s="12" t="s">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B15" s="44"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="20">
-        <v>10</v>
-      </c>
-      <c r="F14" s="21">
+      <c r="F15" s="20">
+        <v>1E+19</v>
+      </c>
+      <c r="G15" s="21">
         <v>7E+19</v>
       </c>
-      <c r="G14" s="22">
-        <f>+E14/SUM(E13:E14)</f>
+      <c r="H15" s="22">
+        <f>+F15/SUM(F14:F15)</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="H14" s="22">
-        <f>+F14/SUM(F13:F14)</f>
+      <c r="I15" s="22">
+        <f>+G15/SUM(G14:G15)</f>
         <v>0.73684210526315785</v>
       </c>
-      <c r="I14" s="22">
-        <f>+G14^$H$2</f>
+      <c r="J15" s="22">
+        <f>+H15^$I$3</f>
         <v>0.28529497656828423</v>
       </c>
-      <c r="J14" s="22">
-        <f>+H14^$I$2</f>
+      <c r="K15" s="22">
+        <f>+I15^$J$3</f>
         <v>0.91245683854817927</v>
       </c>
-      <c r="K14" s="22">
-        <f>+J14*I14</f>
+      <c r="L15" s="22">
+        <f>+K15*J15</f>
         <v>0.2603193523731735</v>
       </c>
-      <c r="L14" s="22">
-        <f>+K14/SUM(K13:K14)</f>
+      <c r="M15" s="22">
+        <f>+L15/SUM(L14:L15)</f>
         <v>0.30624770322817907</v>
       </c>
-      <c r="M14" s="22">
-        <f>+$G$2*30*L14</f>
+      <c r="N15" s="22">
+        <f>+$H$3*30*M15</f>
         <v>9.1874310968453727</v>
       </c>
-      <c r="N14" s="37">
-        <f>+N11+M14</f>
+      <c r="O15" s="37">
+        <f>+O12+N15</f>
         <v>59.409233479356516</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A15" s="12">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B16" s="44">
         <v>150</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="C16" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D16" s="20"/>
+      <c r="E16" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="20">
-        <v>50</v>
-      </c>
-      <c r="F15" s="20">
+      <c r="F16" s="20">
+        <v>5E+19</v>
+      </c>
+      <c r="G16" s="20">
         <v>2.5E+19</v>
       </c>
-      <c r="G15" s="22">
-        <f>+E15/SUM(E15:E16)</f>
+      <c r="H16" s="22">
+        <f>+F16/SUM(F16:F17)</f>
         <v>0.625</v>
       </c>
-      <c r="H15" s="22">
-        <f>+F15/SUM(F15:F16)</f>
+      <c r="I16" s="22">
+        <f>+G16/SUM(G16:G17)</f>
         <v>0.26315789473684209</v>
       </c>
-      <c r="I15" s="22">
-        <f>+G15^$H$2</f>
+      <c r="J16" s="22">
+        <f>+H16^$I$3</f>
         <v>0.71964118851645298</v>
       </c>
-      <c r="J15" s="22">
-        <f>+H15^$I$2</f>
+      <c r="K16" s="22">
+        <f>+I16^$J$3</f>
         <v>0.66998475538030788</v>
       </c>
-      <c r="K15" s="22">
-        <f>+J15*I15</f>
+      <c r="L16" s="22">
+        <f>+K16*J16</f>
         <v>0.48214862564978977</v>
       </c>
-      <c r="L15" s="22">
-        <f>+K15/SUM(K15:K16)</f>
+      <c r="M16" s="22">
+        <f>+L16/SUM(L16:L17)</f>
         <v>0.51217062333254171</v>
       </c>
-      <c r="M15" s="22">
-        <f>+$G$2*70*L15</f>
+      <c r="N16" s="22">
+        <f>+$H$3*70*M16</f>
         <v>35.851943633277919</v>
       </c>
-      <c r="N15" s="37">
-        <f>+N13+M15</f>
+      <c r="O16" s="37">
+        <f>+O14+N16</f>
         <v>126.44271015392141</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A16" s="12"/>
-      <c r="B16" s="23"/>
-      <c r="D16" s="12" t="s">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B17" s="44"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="20">
-        <v>30</v>
-      </c>
-      <c r="F16" s="20">
+      <c r="F17" s="20">
+        <v>3E+19</v>
+      </c>
+      <c r="G17" s="20">
         <v>7E+19</v>
       </c>
-      <c r="G16" s="22">
-        <f>+E16/SUM(E15:E16)</f>
+      <c r="H17" s="22">
+        <f>+F17/SUM(F16:F17)</f>
         <v>0.375</v>
       </c>
-      <c r="H16" s="22">
-        <f>+F16/SUM(F15:F16)</f>
+      <c r="I17" s="22">
+        <f>+G17/SUM(G16:G17)</f>
         <v>0.73684210526315785</v>
       </c>
-      <c r="I16" s="22">
-        <f>+G16^$H$2</f>
+      <c r="J17" s="22">
+        <f>+H17^$I$3</f>
         <v>0.50329415576044101</v>
       </c>
-      <c r="J16" s="22">
-        <f>+H16^$I$2</f>
+      <c r="K17" s="22">
+        <f>+I17^$J$3</f>
         <v>0.91245683854817927</v>
       </c>
-      <c r="K16" s="22">
-        <f>+J16*I16</f>
+      <c r="L17" s="22">
+        <f>+K17*J17</f>
         <v>0.45923419422494693</v>
       </c>
-      <c r="L16" s="22">
-        <f>+K16/SUM(K15:K16)</f>
+      <c r="M17" s="22">
+        <f>+L17/SUM(L16:L17)</f>
         <v>0.48782937666745824</v>
       </c>
-      <c r="M16" s="22">
-        <f>+$G$2*70*L16</f>
+      <c r="N17" s="22">
+        <f>+$H$3*70*M17</f>
         <v>34.148056366722074</v>
       </c>
-      <c r="N16" s="37">
-        <f>+N14+M16</f>
+      <c r="O17" s="37">
+        <f>+O15+N17</f>
         <v>93.557289846078589</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A17" s="12">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B18" s="44">
         <v>220</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="C18" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="37"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A18" s="12"/>
-      <c r="B18" s="23"/>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="20"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="37"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B19" s="44"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="20">
-        <v>40</v>
-      </c>
-      <c r="F18" s="20">
+      <c r="F19" s="20">
+        <v>4E+19</v>
+      </c>
+      <c r="G19" s="20">
         <v>2.5E+19</v>
       </c>
-      <c r="G18" s="22">
-        <f>+E18/SUM(E18:E19)</f>
+      <c r="H19" s="22">
+        <f>+F19/SUM(F19:F20)</f>
         <v>0.5714285714285714</v>
       </c>
-      <c r="H18" s="22">
-        <f>+F18/SUM(F18:F19)</f>
+      <c r="I19" s="22">
+        <f>+G19/SUM(G19:G20)</f>
         <v>0.26315789473684209</v>
       </c>
-      <c r="I18" s="22">
-        <f>+G18^$H$2</f>
+      <c r="J19" s="22">
+        <f>+H19^$I$3</f>
         <v>0.67588586797162753</v>
       </c>
-      <c r="J18" s="22">
-        <f>+H18^$I$2</f>
+      <c r="K19" s="22">
+        <f>+I19^$J$3</f>
         <v>0.66998475538030788</v>
       </c>
-      <c r="K18" s="22">
-        <f>+J18*I18</f>
+      <c r="L19" s="22">
+        <f>+K19*J19</f>
         <v>0.45283322791797792</v>
       </c>
-      <c r="L18" s="22">
-        <f>+K18/SUM(K18:K19)</f>
+      <c r="M19" s="22">
+        <f>+L19/SUM(L19:L20)</f>
         <v>0.4731487637387678</v>
       </c>
-      <c r="M18" s="22">
-        <f>+$G$2*30*L18</f>
+      <c r="N19" s="22">
+        <f>+$H$3*30*M19</f>
         <v>14.194462912163035</v>
       </c>
-      <c r="N18" s="37">
-        <f>+N15+M18</f>
+      <c r="O19" s="37">
+        <f>+O16+N19</f>
         <v>140.63717306608444</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A19" s="12"/>
-      <c r="B19" s="23"/>
-      <c r="D19" s="12" t="s">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B20" s="44"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="20">
-        <v>30</v>
-      </c>
-      <c r="F19" s="20">
+      <c r="F20" s="20">
+        <v>3E+19</v>
+      </c>
+      <c r="G20" s="20">
         <v>7E+19</v>
       </c>
-      <c r="G19" s="22">
-        <f>+E19/SUM(E18:E19)</f>
+      <c r="H20" s="22">
+        <f>+F20/SUM(F19:F20)</f>
         <v>0.42857142857142855</v>
       </c>
-      <c r="H19" s="22">
-        <f>+F19/SUM(F18:F19)</f>
+      <c r="I20" s="22">
+        <f>+G20/SUM(G19:G20)</f>
         <v>0.73684210526315785</v>
       </c>
-      <c r="I19" s="22">
-        <f>+G19^$H$2</f>
+      <c r="J20" s="22">
+        <f>+H20^$I$3</f>
         <v>0.55260683251119402</v>
       </c>
-      <c r="J19" s="22">
-        <f>+H19^$I$2</f>
+      <c r="K20" s="22">
+        <f>+I20^$J$3</f>
         <v>0.91245683854817927</v>
       </c>
-      <c r="K19" s="22">
-        <f>+J19*I19</f>
+      <c r="L20" s="22">
+        <f>+K20*J20</f>
         <v>0.50422988335328733</v>
       </c>
-      <c r="L19" s="22">
-        <f>+K19/SUM(K18:K19)</f>
+      <c r="M20" s="22">
+        <f>+L20/SUM(L19:L20)</f>
         <v>0.5268512362612322</v>
       </c>
-      <c r="M19" s="22">
-        <f>+$G$2*30*L19</f>
+      <c r="N20" s="22">
+        <f>+$H$3*30*M20</f>
         <v>15.805537087836965</v>
       </c>
-      <c r="N19" s="37">
-        <f>+N16+M19</f>
+      <c r="O20" s="37">
+        <f>+O17+N20</f>
         <v>109.36282693391556</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A20" s="12">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B21" s="44">
         <v>250</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="C21" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="37"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A21" s="12"/>
-      <c r="B21" s="23"/>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="20"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="37"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B22" s="44"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="20">
-        <v>40</v>
-      </c>
-      <c r="F21" s="20">
+      <c r="F22" s="20">
+        <v>4E+19</v>
+      </c>
+      <c r="G22" s="20">
         <v>1.25E+20</v>
       </c>
-      <c r="G21" s="22">
-        <f>+E21/SUM(E21:E22)</f>
+      <c r="H22" s="22">
+        <f>+F22/SUM(F22:F23)</f>
         <v>0.5714285714285714</v>
       </c>
-      <c r="H21" s="22">
-        <f>+F21/SUM(F21:F22)</f>
+      <c r="I22" s="22">
+        <f>+G22/SUM(G22:G23)</f>
         <v>0.64102564102564108</v>
       </c>
-      <c r="I21" s="22">
-        <f>+G21^$H$2</f>
+      <c r="J22" s="22">
+        <f>+H22^$I$3</f>
         <v>0.67588586797162753</v>
       </c>
-      <c r="J21" s="22">
-        <f>+H21^$I$2</f>
+      <c r="K22" s="22">
+        <f>+I22^$J$3</f>
         <v>0.87510994737242054</v>
       </c>
-      <c r="K21" s="22">
-        <f>+J21*I21</f>
+      <c r="L22" s="22">
+        <f>+K22*J22</f>
         <v>0.5914744463504138</v>
       </c>
-      <c r="L21" s="22">
-        <f>+K21/SUM(K21:K22)</f>
+      <c r="M22" s="22">
+        <f>+L22/SUM(L22:L23)</f>
         <v>0.59274457381575263</v>
       </c>
-      <c r="M21" s="22">
-        <f>+$G$2*50*L21</f>
+      <c r="N22" s="22">
+        <f>+$H$3*50*M22</f>
         <v>29.63722869078763</v>
       </c>
-      <c r="N21" s="37">
-        <f>+N18+M21</f>
+      <c r="O22" s="37">
+        <f>+O19+N22</f>
         <v>170.27440175687207</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="A22" s="13">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="B23" s="45">
         <v>300</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="C23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D23" s="6"/>
+      <c r="E23" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="6">
-        <v>30</v>
-      </c>
-      <c r="F22" s="6">
+      <c r="F23" s="6">
+        <v>3E+19</v>
+      </c>
+      <c r="G23" s="6">
         <v>7E+19</v>
       </c>
-      <c r="G22" s="7">
-        <f>+E22/SUM(E21:E22)</f>
+      <c r="H23" s="7">
+        <f>+F23/SUM(F22:F23)</f>
         <v>0.42857142857142855</v>
       </c>
-      <c r="H22" s="7">
-        <f>+F22/SUM(F21:F22)</f>
+      <c r="I23" s="7">
+        <f>+G23/SUM(G22:G23)</f>
         <v>0.35897435897435898</v>
       </c>
-      <c r="I22" s="7">
-        <f>+G22^$H$2</f>
+      <c r="J23" s="7">
+        <f>+H23^$I$3</f>
         <v>0.55260683251119402</v>
       </c>
-      <c r="J22" s="7">
-        <f>+H22^$I$2</f>
+      <c r="K23" s="7">
+        <f>+I23^$J$3</f>
         <v>0.73539221595033788</v>
       </c>
-      <c r="K22" s="7">
-        <f>+J22*I22</f>
+      <c r="L23" s="7">
+        <f>+K23*J23</f>
         <v>0.40638276310970417</v>
       </c>
-      <c r="L22" s="7">
-        <f>+K22/SUM(K21:K22)</f>
+      <c r="M23" s="7">
+        <f>+L23/SUM(L22:L23)</f>
         <v>0.40725542618424743</v>
       </c>
-      <c r="M22" s="7">
-        <f>+$G$2*50*L22</f>
+      <c r="N23" s="7">
+        <f>+$H$3*50*M23</f>
         <v>20.36277130921237</v>
       </c>
-      <c r="N22" s="38">
-        <f>+N19+M22</f>
+      <c r="O23" s="38">
+        <f>+O20+N23</f>
         <v>129.72559824312793</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="D24" s="10" t="s">
+    <row r="25" spans="2:15" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="E25" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="11"/>
-    </row>
-    <row r="25" spans="1:14" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
-      <c r="D25" s="12" t="s">
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="2:15" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="E26" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="33">
-        <f>+SUM(M7,M10,M13,M15,M18,M21)</f>
+      <c r="F26" s="41">
+        <f>+SUM(N8,N11,N14,N16,N19,N22)</f>
         <v>170.27440175687207</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="D26" s="13" t="s">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="E27" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="34">
-        <f>+SUM(M8,M11,M14,M16,M19,M22)</f>
+      <c r="F27" s="42">
+        <f>+SUM(N9,N12,N15,N17,N20,N23)</f>
         <v>129.72559824312793</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.75">
-      <c r="D27" s="14" t="s">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="E28" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="15">
-        <f>+SUM(E25:E26)</f>
+      <c r="F28" s="43">
+        <f>+SUM(F26:F27)</f>
         <v>300</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: included decay rate in rewardPerRewardScore()
</commit_message>
<xml_diff>
--- a/20210921 - Staking Rewards.xlsx
+++ b/20210921 - Staking Rewards.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Documents\16slimchance16\token\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71580DC1-7491-4FF4-B0A5-8708B1AA2928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3359C63-0188-4F6B-9F87-084DF9F462FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-90" windowWidth="16530" windowHeight="10980" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="-90" windowWidth="16490" windowHeight="10980" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SNX" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="SNX - Detail" sheetId="4" state="hidden" r:id="rId2"/>
     <sheet name="KWENTA" sheetId="5" state="hidden" r:id="rId3"/>
     <sheet name="KWENTA - power" sheetId="6" r:id="rId4"/>
+    <sheet name="KWENTA - Decay" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="52">
   <si>
     <t>N stake 20</t>
   </si>
@@ -187,20 +188,31 @@
   </si>
   <si>
     <t>%rewards</t>
+  </si>
+  <si>
+    <t>Decay rate</t>
+  </si>
+  <si>
+    <t>decayedFees</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="10">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000000E+00"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0000E+00"/>
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0%"/>
+    <numFmt numFmtId="172" formatCode="0.000000"/>
+    <numFmt numFmtId="174" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="175" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,13 +228,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -366,10 +391,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -411,13 +437,53 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="174" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="175" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2068,10 +2134,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486B17B1-BE12-4310-9A3F-24B7422EA458}">
-  <dimension ref="B2:O28"/>
+  <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2085,14 +2151,1277 @@
     <col min="8" max="8" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.31640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.54296875" style="26" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.2265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+    </row>
+    <row r="2" spans="1:20" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A2" s="49"/>
+      <c r="B2" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="52"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="50"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+    </row>
+    <row r="3" spans="1:20" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="A3" s="49"/>
+      <c r="B3" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="49">
+        <v>25</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49">
+        <v>300</v>
+      </c>
+      <c r="G3" s="49">
+        <v>300</v>
+      </c>
+      <c r="H3" s="49">
+        <v>1</v>
+      </c>
+      <c r="I3" s="49">
+        <v>0.7</v>
+      </c>
+      <c r="J3" s="49">
+        <v>0.3</v>
+      </c>
+      <c r="K3" s="50"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A4" s="49"/>
+      <c r="B4" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="49">
+        <v>50</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A5" s="49"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A6" s="49"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A7" s="49"/>
+      <c r="B7" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="60"/>
+      <c r="E7" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="49"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A8" s="49"/>
+      <c r="B8" s="64">
+        <v>0</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="65"/>
+      <c r="E8" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="65">
+        <v>1E+19</v>
+      </c>
+      <c r="G8" s="67">
+        <v>2.5E+19</v>
+      </c>
+      <c r="H8" s="68">
+        <f>+F8/SUM(F8:F9)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="68">
+        <f>+G8/SUM(G8:G9)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J8" s="68">
+        <f>+H8^$I$3</f>
+        <v>0.61557220667245816</v>
+      </c>
+      <c r="K8" s="68">
+        <f>+I8^$J$3</f>
+        <v>0.71922309332486434</v>
+      </c>
+      <c r="L8" s="68">
+        <f>+K8*J8</f>
+        <v>0.44273374664777804</v>
+      </c>
+      <c r="M8" s="69">
+        <f>+L8/SUM(L8:L9)</f>
+        <v>0.44820048133989088</v>
+      </c>
+      <c r="N8" s="68">
+        <f>+$H$3*60*M8</f>
+        <v>26.892028880393454</v>
+      </c>
+      <c r="O8" s="70">
+        <f>+N8</f>
+        <v>26.892028880393454</v>
+      </c>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49">
+        <f>10^0.7</f>
+        <v>5.0118723362727229</v>
+      </c>
+      <c r="S8" s="49">
+        <f>10^0.7</f>
+        <v>5.0118723362727229</v>
+      </c>
+      <c r="T8" s="49"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A9" s="49"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="65">
+        <v>1E+19</v>
+      </c>
+      <c r="G9" s="67">
+        <v>5E+19</v>
+      </c>
+      <c r="H9" s="68">
+        <f>+F9/SUM(F8:F9)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="68">
+        <f>+G9/SUM(G8:G9)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J9" s="68">
+        <f>+H9^$I$3</f>
+        <v>0.61557220667245816</v>
+      </c>
+      <c r="K9" s="68">
+        <f>+I9^$J$3</f>
+        <v>0.88546749329555607</v>
+      </c>
+      <c r="L9" s="68">
+        <f>+K9*J9</f>
+        <v>0.54506917878467553</v>
+      </c>
+      <c r="M9" s="69">
+        <f>+L9/SUM(L8:L9)</f>
+        <v>0.55179951866010912</v>
+      </c>
+      <c r="N9" s="68">
+        <f>+$H$3*60*M9</f>
+        <v>33.107971119606546</v>
+      </c>
+      <c r="O9" s="70">
+        <f>+N9</f>
+        <v>33.107971119606546</v>
+      </c>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49">
+        <f>25^0.3</f>
+        <v>2.626527804403767</v>
+      </c>
+      <c r="S9" s="49">
+        <f>50^0.3</f>
+        <v>3.2336350328867871</v>
+      </c>
+      <c r="T9" s="49"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A10" s="49"/>
+      <c r="B10" s="64">
+        <v>60</v>
+      </c>
+      <c r="C10" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="65"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49">
+        <f>+R9*R8</f>
+        <v>13.163822043342373</v>
+      </c>
+      <c r="S10" s="49">
+        <f>+S9*S8</f>
+        <v>16.206565966927624</v>
+      </c>
+      <c r="T10" s="49"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A11" s="49"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="65">
+        <v>5E+19</v>
+      </c>
+      <c r="G11" s="67">
+        <v>2.5E+19</v>
+      </c>
+      <c r="H11" s="68">
+        <f>+F11/SUM(F11:F12)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I11" s="68">
+        <f>+G11/SUM(G11:G12)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J11" s="68">
+        <f>+H11^$I$3</f>
+        <v>0.88018330703271519</v>
+      </c>
+      <c r="K11" s="68">
+        <f>+I11^$J$3</f>
+        <v>0.71922309332486434</v>
+      </c>
+      <c r="L11" s="68">
+        <f>+K11*J11</f>
+        <v>0.63304816077697823</v>
+      </c>
+      <c r="M11" s="68">
+        <f>+L11/SUM(L11:L12)</f>
+        <v>0.71476947895159004</v>
+      </c>
+      <c r="N11" s="68">
+        <f>+$H$3*60*M11</f>
+        <v>42.886168737095403</v>
+      </c>
+      <c r="O11" s="72">
+        <f>+N11+N8</f>
+        <v>69.778197617488857</v>
+      </c>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A12" s="49"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="65">
+        <v>1E+19</v>
+      </c>
+      <c r="G12" s="67">
+        <v>5E+19</v>
+      </c>
+      <c r="H12" s="68">
+        <f>+F12/SUM(F11:F12)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I12" s="68">
+        <f>+G12/SUM(G11:G12)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J12" s="68">
+        <f>+H12^$I$3</f>
+        <v>0.28529497656828423</v>
+      </c>
+      <c r="K12" s="68">
+        <f>+I12^$J$3</f>
+        <v>0.88546749329555607</v>
+      </c>
+      <c r="L12" s="68">
+        <f>+K12*J12</f>
+        <v>0.25261942775173307</v>
+      </c>
+      <c r="M12" s="68">
+        <f>+L12/SUM(L11:L12)</f>
+        <v>0.28523052104840996</v>
+      </c>
+      <c r="N12" s="68">
+        <f>+$H$3*60*M12</f>
+        <v>17.113831262904597</v>
+      </c>
+      <c r="O12" s="72">
+        <f>+N12+N9</f>
+        <v>50.221802382511143</v>
+      </c>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49">
+        <f>+R10+S10</f>
+        <v>29.370388010269998</v>
+      </c>
+      <c r="S12" s="49"/>
+      <c r="T12" s="49"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A13" s="49"/>
+      <c r="B13" s="64">
+        <v>120</v>
+      </c>
+      <c r="C13" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="65"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="71"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49">
+        <f>1/R12/60</f>
+        <v>5.6746498074314853E-4</v>
+      </c>
+      <c r="S13" s="49"/>
+      <c r="T13" s="49"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A14" s="49"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="65">
+        <v>5E+19</v>
+      </c>
+      <c r="G14" s="67">
+        <v>2.5E+19</v>
+      </c>
+      <c r="H14" s="68">
+        <f>+F14/SUM(F14:F15)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I14" s="68">
+        <f>+G14/SUM(G14:G15)</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="J14" s="68">
+        <f>+H14^$I$3</f>
+        <v>0.88018330703271519</v>
+      </c>
+      <c r="K14" s="68">
+        <f>+I14^$J$3</f>
+        <v>0.66998475538030788</v>
+      </c>
+      <c r="L14" s="68">
+        <f>+K14*J14</f>
+        <v>0.58970939765214414</v>
+      </c>
+      <c r="M14" s="68">
+        <f>+L14/SUM(L14:L15)</f>
+        <v>0.69375229677182093</v>
+      </c>
+      <c r="N14" s="68">
+        <f>+$H$3*30*M14</f>
+        <v>20.812568903154627</v>
+      </c>
+      <c r="O14" s="72">
+        <f>+O11+N14</f>
+        <v>90.590766520643484</v>
+      </c>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="49"/>
+      <c r="T14" s="49"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A15" s="49"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="65">
+        <v>1E+19</v>
+      </c>
+      <c r="G15" s="67">
+        <v>7E+19</v>
+      </c>
+      <c r="H15" s="68">
+        <f>+F15/SUM(F14:F15)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I15" s="68">
+        <f>+G15/SUM(G14:G15)</f>
+        <v>0.73684210526315785</v>
+      </c>
+      <c r="J15" s="68">
+        <f>+H15^$I$3</f>
+        <v>0.28529497656828423</v>
+      </c>
+      <c r="K15" s="68">
+        <f>+I15^$J$3</f>
+        <v>0.91245683854817927</v>
+      </c>
+      <c r="L15" s="68">
+        <f>+K15*J15</f>
+        <v>0.2603193523731735</v>
+      </c>
+      <c r="M15" s="68">
+        <f>+L15/SUM(L14:L15)</f>
+        <v>0.30624770322817907</v>
+      </c>
+      <c r="N15" s="68">
+        <f>+$H$3*30*M15</f>
+        <v>9.1874310968453727</v>
+      </c>
+      <c r="O15" s="72">
+        <f>+O12+N15</f>
+        <v>59.409233479356516</v>
+      </c>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="49"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A16" s="49"/>
+      <c r="B16" s="64">
+        <v>150</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="65"/>
+      <c r="E16" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="65">
+        <v>5E+19</v>
+      </c>
+      <c r="G16" s="65">
+        <v>2.5E+19</v>
+      </c>
+      <c r="H16" s="68">
+        <f>+F16/SUM(F16:F17)</f>
+        <v>0.625</v>
+      </c>
+      <c r="I16" s="68">
+        <f>+G16/SUM(G16:G17)</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="J16" s="68">
+        <f>+H16^$I$3</f>
+        <v>0.71964118851645298</v>
+      </c>
+      <c r="K16" s="68">
+        <f>+I16^$J$3</f>
+        <v>0.66998475538030788</v>
+      </c>
+      <c r="L16" s="68">
+        <f>+K16*J16</f>
+        <v>0.48214862564978977</v>
+      </c>
+      <c r="M16" s="68">
+        <f>+L16/SUM(L16:L17)</f>
+        <v>0.51217062333254171</v>
+      </c>
+      <c r="N16" s="68">
+        <f>+$H$3*70*M16</f>
+        <v>35.851943633277919</v>
+      </c>
+      <c r="O16" s="72">
+        <f>+O14+N16</f>
+        <v>126.44271015392141</v>
+      </c>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="49"/>
+      <c r="S16" s="49"/>
+      <c r="T16" s="49"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A17" s="49"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="65">
+        <v>3E+19</v>
+      </c>
+      <c r="G17" s="65">
+        <v>7E+19</v>
+      </c>
+      <c r="H17" s="68">
+        <f>+F17/SUM(F16:F17)</f>
+        <v>0.375</v>
+      </c>
+      <c r="I17" s="68">
+        <f>+G17/SUM(G16:G17)</f>
+        <v>0.73684210526315785</v>
+      </c>
+      <c r="J17" s="68">
+        <f>+H17^$I$3</f>
+        <v>0.50329415576044101</v>
+      </c>
+      <c r="K17" s="68">
+        <f>+I17^$J$3</f>
+        <v>0.91245683854817927</v>
+      </c>
+      <c r="L17" s="68">
+        <f>+K17*J17</f>
+        <v>0.45923419422494693</v>
+      </c>
+      <c r="M17" s="68">
+        <f>+L17/SUM(L16:L17)</f>
+        <v>0.48782937666745824</v>
+      </c>
+      <c r="N17" s="68">
+        <f>+$H$3*70*M17</f>
+        <v>34.148056366722074</v>
+      </c>
+      <c r="O17" s="72">
+        <f>+O15+N17</f>
+        <v>93.557289846078589</v>
+      </c>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49">
+        <f>60*1000000000000000000</f>
+        <v>6E+19</v>
+      </c>
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A18" s="49"/>
+      <c r="B18" s="64">
+        <v>220</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="65"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="68"/>
+      <c r="O18" s="72"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="49">
+        <f>+R17*10000</f>
+        <v>6.0000000000000002E+23</v>
+      </c>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A19" s="49"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="65">
+        <v>4E+19</v>
+      </c>
+      <c r="G19" s="65">
+        <v>2.5E+19</v>
+      </c>
+      <c r="H19" s="68">
+        <f>+F19/SUM(F19:F20)</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="I19" s="68">
+        <f>+G19/SUM(G19:G20)</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="J19" s="68">
+        <f>+H19^$I$3</f>
+        <v>0.67588586797162753</v>
+      </c>
+      <c r="K19" s="68">
+        <f>+I19^$J$3</f>
+        <v>0.66998475538030788</v>
+      </c>
+      <c r="L19" s="68">
+        <f>+K19*J19</f>
+        <v>0.45283322791797792</v>
+      </c>
+      <c r="M19" s="68">
+        <f>+L19/SUM(L19:L20)</f>
+        <v>0.4731487637387678</v>
+      </c>
+      <c r="N19" s="68">
+        <f>+$H$3*30*M19</f>
+        <v>14.194462912163035</v>
+      </c>
+      <c r="O19" s="72">
+        <f>+O16+N19</f>
+        <v>140.63717306608444</v>
+      </c>
+      <c r="P19" s="49"/>
+      <c r="Q19" s="49"/>
+      <c r="R19" s="49">
+        <f>+R18*1E+50</f>
+        <v>6.0000000000000002E+73</v>
+      </c>
+      <c r="S19" s="49"/>
+      <c r="T19" s="49"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A20" s="49"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="65">
+        <v>3E+19</v>
+      </c>
+      <c r="G20" s="65">
+        <v>7E+19</v>
+      </c>
+      <c r="H20" s="68">
+        <f>+F20/SUM(F19:F20)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="I20" s="68">
+        <f>+G20/SUM(G19:G20)</f>
+        <v>0.73684210526315785</v>
+      </c>
+      <c r="J20" s="68">
+        <f>+H20^$I$3</f>
+        <v>0.55260683251119402</v>
+      </c>
+      <c r="K20" s="68">
+        <f>+I20^$J$3</f>
+        <v>0.91245683854817927</v>
+      </c>
+      <c r="L20" s="68">
+        <f>+K20*J20</f>
+        <v>0.50422988335328733</v>
+      </c>
+      <c r="M20" s="68">
+        <f>+L20/SUM(L19:L20)</f>
+        <v>0.5268512362612322</v>
+      </c>
+      <c r="N20" s="68">
+        <f>+$H$3*30*M20</f>
+        <v>15.805537087836965</v>
+      </c>
+      <c r="O20" s="72">
+        <f>+O17+N20</f>
+        <v>109.36282693391556</v>
+      </c>
+      <c r="P20" s="49"/>
+      <c r="Q20" s="50">
+        <f>+K27</f>
+        <v>0.999</v>
+      </c>
+      <c r="R20" s="49">
+        <f>+R19/2.93703880102699E+37</f>
+        <v>2.0428739306753418E+36</v>
+      </c>
+      <c r="S20" s="49"/>
+      <c r="T20" s="49"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A21" s="49"/>
+      <c r="B21" s="64">
+        <v>250</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="65"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="68"/>
+      <c r="K21" s="68"/>
+      <c r="L21" s="68"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="68"/>
+      <c r="O21" s="72"/>
+      <c r="P21" s="49"/>
+      <c r="Q21" s="49">
+        <f>+Q20^(0.3*60)</f>
+        <v>0.98215218705145069</v>
+      </c>
+      <c r="R21" s="84">
+        <f>+R20/(Q21*1000000000000000000)</f>
+        <v>2.0799973340265288E+18</v>
+      </c>
+      <c r="S21" s="49"/>
+      <c r="T21" s="49"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A22" s="49"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="65">
+        <v>4E+19</v>
+      </c>
+      <c r="G22" s="65">
+        <v>1.25E+20</v>
+      </c>
+      <c r="H22" s="68">
+        <f>+F22/SUM(F22:F23)</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="I22" s="68">
+        <f>+G22/SUM(G22:G23)</f>
+        <v>0.64102564102564108</v>
+      </c>
+      <c r="J22" s="68">
+        <f>+H22^$I$3</f>
+        <v>0.67588586797162753</v>
+      </c>
+      <c r="K22" s="68">
+        <f>+I22^$J$3</f>
+        <v>0.87510994737242054</v>
+      </c>
+      <c r="L22" s="68">
+        <f>+K22*J22</f>
+        <v>0.5914744463504138</v>
+      </c>
+      <c r="M22" s="68">
+        <f>+L22/SUM(L22:L23)</f>
+        <v>0.59274457381575263</v>
+      </c>
+      <c r="N22" s="68">
+        <f>+$H$3*50*M22</f>
+        <v>29.63722869078763</v>
+      </c>
+      <c r="O22" s="72">
+        <f>+O19+N22</f>
+        <v>170.27440175687207</v>
+      </c>
+      <c r="P22" s="49"/>
+      <c r="Q22" s="49"/>
+      <c r="R22" s="49"/>
+      <c r="S22" s="49"/>
+      <c r="T22" s="49"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A23" s="49"/>
+      <c r="B23" s="73">
+        <v>300</v>
+      </c>
+      <c r="C23" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="56"/>
+      <c r="E23" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="56">
+        <v>3E+19</v>
+      </c>
+      <c r="G23" s="56">
+        <v>7E+19</v>
+      </c>
+      <c r="H23" s="75">
+        <f>+F23/SUM(F22:F23)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="I23" s="75">
+        <f>+G23/SUM(G22:G23)</f>
+        <v>0.35897435897435898</v>
+      </c>
+      <c r="J23" s="75">
+        <f>+H23^$I$3</f>
+        <v>0.55260683251119402</v>
+      </c>
+      <c r="K23" s="75">
+        <f>+I23^$J$3</f>
+        <v>0.73539221595033788</v>
+      </c>
+      <c r="L23" s="75">
+        <f>+K23*J23</f>
+        <v>0.40638276310970417</v>
+      </c>
+      <c r="M23" s="75">
+        <f>+L23/SUM(L22:L23)</f>
+        <v>0.40725542618424743</v>
+      </c>
+      <c r="N23" s="75">
+        <f>+$H$3*50*M23</f>
+        <v>20.36277130921237</v>
+      </c>
+      <c r="O23" s="76">
+        <f>+O20+N23</f>
+        <v>129.72559824312793</v>
+      </c>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="49"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="49"/>
+      <c r="T23" s="49"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A24" s="49"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="49"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="49"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="49"/>
+      <c r="T24" s="49"/>
+    </row>
+    <row r="25" spans="1:20" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A25" s="49"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="77" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="78"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="49"/>
+      <c r="P25" s="49"/>
+      <c r="Q25" s="49"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="49"/>
+      <c r="T25" s="49"/>
+    </row>
+    <row r="26" spans="1:20" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="79">
+        <f>+SUM(N8,N11,N14,N16,N19,N22)</f>
+        <v>170.27440175687207</v>
+      </c>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="82"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="49"/>
+      <c r="P26" s="49"/>
+      <c r="Q26" s="49"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="49"/>
+      <c r="T26" s="49"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A27" s="49"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="80">
+        <f>+SUM(N9,N12,N15,N17,N20,N23)</f>
+        <v>129.72559824312793</v>
+      </c>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="50">
+        <v>0.999</v>
+      </c>
+      <c r="L27" s="83">
+        <f>+K27*1000000000000000000</f>
+        <v>9.99E+17</v>
+      </c>
+      <c r="M27" s="49"/>
+      <c r="N27" s="51"/>
+      <c r="O27" s="49"/>
+      <c r="P27" s="49"/>
+      <c r="Q27" s="49"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="49"/>
+      <c r="T27" s="49"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A28" s="49"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="81">
+        <f>+SUM(F26:F27)</f>
+        <v>300</v>
+      </c>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="50">
+        <f>+K27^(0.3*60)</f>
+        <v>0.98215218705145069</v>
+      </c>
+      <c r="L28" s="49">
+        <f>60*0.3</f>
+        <v>18</v>
+      </c>
+      <c r="M28" s="49"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="49"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A29" s="49"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="51"/>
+      <c r="O29" s="49"/>
+      <c r="P29" s="49"/>
+      <c r="Q29" s="49"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="49"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A30" s="49"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49">
+        <f>2^256-1</f>
+        <v>1.157920892373162E+77</v>
+      </c>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="49"/>
+      <c r="P30" s="49"/>
+      <c r="Q30" s="49"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="49"/>
+      <c r="T30" s="49"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A31" s="49"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49">
+        <f>2^255-1</f>
+        <v>5.7896044618658098E+76</v>
+      </c>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="51"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
+      <c r="T31" s="49"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A32" s="49"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="50"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="51"/>
+      <c r="O32" s="49"/>
+      <c r="P32" s="49"/>
+      <c r="Q32" s="49"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="49"/>
+      <c r="T32" s="49"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9645F85E-96B2-448C-B0D9-612FF5920724}">
+  <dimension ref="B2:P28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="2" max="2" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.1328125" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.58984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.31640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.90625" customWidth="1"/>
+    <col min="15" max="15" width="7.54296875" style="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
@@ -2106,17 +3435,24 @@
       <c r="G2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="M2" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="47">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
       <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
@@ -2129,27 +3465,27 @@
       <c r="G3">
         <v>300</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.7</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.3</v>
       </c>
-      <c r="N3" s="30"/>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="O3" s="30"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C4">
         <v>50</v>
       </c>
-      <c r="O4" s="9"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="P4" s="9"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B5" s="8"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -2159,13 +3495,14 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="25"/>
       <c r="M5" s="6"/>
-      <c r="N5" s="27"/>
+      <c r="N5" s="6"/>
       <c r="O5" s="27"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="P5" s="27"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B7" s="16" t="s">
         <v>39</v>
       </c>
@@ -2183,31 +3520,34 @@
         <v>13</v>
       </c>
       <c r="H7" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="J7" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="K7" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="L7" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="M7" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="M7" s="17" t="s">
+      <c r="N7" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="N7" s="39" t="s">
+      <c r="O7" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="40" t="s">
+      <c r="P7" s="40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.75">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B8" s="44">
         <v>0</v>
       </c>
@@ -2224,40 +3564,44 @@
       <c r="G8" s="21">
         <v>2.5E+19</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="21">
+        <f>+((G8/1000000000000000000)*$N$2^60)*1000000000000000000</f>
+        <v>2.3543406555579216E+19</v>
+      </c>
+      <c r="I8" s="22">
         <f>+F8/SUM(F8:F9)</f>
         <v>0.5</v>
       </c>
-      <c r="I8" s="22">
-        <f>+G8/SUM(G8:G9)</f>
-        <v>0.33333333333333331</v>
-      </c>
       <c r="J8" s="22">
-        <f>+H8^$I$3</f>
-        <v>0.61557220667245816</v>
+        <f>+H8/SUM(H8:H9)</f>
+        <v>0.33333333333333337</v>
       </c>
       <c r="K8" s="22">
         <f>+I8^$J$3</f>
-        <v>0.71922309332486434</v>
+        <v>0.61557220667245816</v>
       </c>
       <c r="L8" s="22">
-        <f>+K8*J8</f>
-        <v>0.44273374664777804</v>
-      </c>
-      <c r="M8" s="36">
-        <f>+L8/SUM(L8:L9)</f>
-        <v>0.44820048133989088</v>
-      </c>
-      <c r="N8" s="22">
-        <f>+$H$3*60*M8</f>
-        <v>26.892028880393454</v>
-      </c>
-      <c r="O8" s="35">
-        <f>+N8</f>
-        <v>26.892028880393454</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.75">
+        <f>+J8^$K$3</f>
+        <v>0.71922309332486445</v>
+      </c>
+      <c r="M8" s="22">
+        <f>+L8*K8</f>
+        <v>0.44273374664777809</v>
+      </c>
+      <c r="N8" s="36">
+        <f>+M8/SUM(M8:M9)</f>
+        <v>0.44820048133989093</v>
+      </c>
+      <c r="O8" s="22">
+        <f>+$I$3*60*N8</f>
+        <v>26.892028880393458</v>
+      </c>
+      <c r="P8" s="35">
+        <f>+O8</f>
+        <v>26.892028880393458</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B9" s="44"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
@@ -2270,40 +3614,44 @@
       <c r="G9" s="21">
         <v>5E+19</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="21">
+        <f>+((G9/1000000000000000000)*$N$2^60)*1000000000000000000</f>
+        <v>4.7086813111158432E+19</v>
+      </c>
+      <c r="I9" s="22">
         <f>+F9/SUM(F8:F9)</f>
         <v>0.5</v>
       </c>
-      <c r="I9" s="22">
-        <f>+G9/SUM(G8:G9)</f>
-        <v>0.66666666666666663</v>
-      </c>
       <c r="J9" s="22">
-        <f>+H9^$I$3</f>
-        <v>0.61557220667245816</v>
+        <f>+H9/SUM(H8:H9)</f>
+        <v>0.66666666666666674</v>
       </c>
       <c r="K9" s="22">
         <f>+I9^$J$3</f>
-        <v>0.88546749329555607</v>
+        <v>0.61557220667245816</v>
       </c>
       <c r="L9" s="22">
-        <f>+K9*J9</f>
+        <f>+J9^$K$3</f>
+        <v>0.88546749329555619</v>
+      </c>
+      <c r="M9" s="22">
+        <f>+L9*K9</f>
         <v>0.54506917878467553</v>
       </c>
-      <c r="M9" s="36">
-        <f>+L9/SUM(L8:L9)</f>
+      <c r="N9" s="36">
+        <f>+M9/SUM(M8:M9)</f>
         <v>0.55179951866010912</v>
       </c>
-      <c r="N9" s="22">
-        <f>+$H$3*60*M9</f>
+      <c r="O9" s="22">
+        <f>+$I$3*60*N9</f>
         <v>33.107971119606546</v>
       </c>
-      <c r="O9" s="35">
-        <f>+N9</f>
+      <c r="P9" s="35">
+        <f>+O9</f>
         <v>33.107971119606546</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.75">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B10" s="44">
         <v>60</v>
       </c>
@@ -2314,16 +3662,17 @@
       <c r="E10" s="12"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="22"/>
+      <c r="H10" s="20"/>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
       <c r="L10" s="22"/>
       <c r="M10" s="22"/>
       <c r="N10" s="22"/>
-      <c r="O10" s="23"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="O10" s="22"/>
+      <c r="P10" s="23"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B11" s="44"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
@@ -2336,40 +3685,44 @@
       <c r="G11" s="21">
         <v>2.5E+19</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="21">
+        <f>+((G11/1000000000000000000)*$N$2^120)*1000000000000000000</f>
+        <v>2.2171679689651618E+19</v>
+      </c>
+      <c r="I11" s="22">
         <f>+F11/SUM(F11:F12)</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="I11" s="22">
-        <f>+G11/SUM(G11:G12)</f>
+      <c r="J11" s="22">
+        <f>+H11/SUM(H11:H12)</f>
         <v>0.33333333333333331</v>
-      </c>
-      <c r="J11" s="22">
-        <f>+H11^$I$3</f>
-        <v>0.88018330703271519</v>
       </c>
       <c r="K11" s="22">
         <f>+I11^$J$3</f>
+        <v>0.88018330703271519</v>
+      </c>
+      <c r="L11" s="22">
+        <f>+J11^$K$3</f>
         <v>0.71922309332486434</v>
       </c>
-      <c r="L11" s="22">
-        <f>+K11*J11</f>
+      <c r="M11" s="22">
+        <f>+L11*K11</f>
         <v>0.63304816077697823</v>
       </c>
-      <c r="M11" s="22">
-        <f>+L11/SUM(L11:L12)</f>
+      <c r="N11" s="22">
+        <f>+M11/SUM(M11:M12)</f>
         <v>0.71476947895159004</v>
       </c>
-      <c r="N11" s="22">
-        <f>+$H$3*60*M11</f>
+      <c r="O11" s="22">
+        <f>+$I$3*60*N11</f>
         <v>42.886168737095403</v>
       </c>
-      <c r="O11" s="37">
-        <f>+N11+N8</f>
+      <c r="P11" s="37">
+        <f>+O11+O8</f>
         <v>69.778197617488857</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.75">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B12" s="44"/>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
@@ -2382,40 +3735,44 @@
       <c r="G12" s="21">
         <v>5E+19</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="21">
+        <f>+((G12/1000000000000000000)*$N$2^120)*1000000000000000000</f>
+        <v>4.4343359379303236E+19</v>
+      </c>
+      <c r="I12" s="22">
         <f>+F12/SUM(F11:F12)</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="I12" s="22">
-        <f>+G12/SUM(G11:G12)</f>
+      <c r="J12" s="22">
+        <f>+H12/SUM(H11:H12)</f>
         <v>0.66666666666666663</v>
-      </c>
-      <c r="J12" s="22">
-        <f>+H12^$I$3</f>
-        <v>0.28529497656828423</v>
       </c>
       <c r="K12" s="22">
         <f>+I12^$J$3</f>
+        <v>0.28529497656828423</v>
+      </c>
+      <c r="L12" s="22">
+        <f>+J12^$K$3</f>
         <v>0.88546749329555607</v>
       </c>
-      <c r="L12" s="22">
-        <f>+K12*J12</f>
+      <c r="M12" s="22">
+        <f>+L12*K12</f>
         <v>0.25261942775173307</v>
       </c>
-      <c r="M12" s="22">
-        <f>+L12/SUM(L11:L12)</f>
+      <c r="N12" s="22">
+        <f>+M12/SUM(M11:M12)</f>
         <v>0.28523052104840996</v>
       </c>
-      <c r="N12" s="22">
-        <f>+$H$3*60*M12</f>
+      <c r="O12" s="22">
+        <f>+$I$3*60*N12</f>
         <v>17.113831262904597</v>
       </c>
-      <c r="O12" s="37">
-        <f>+N12+N9</f>
+      <c r="P12" s="37">
+        <f>+O12+O9</f>
         <v>50.221802382511143</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.75">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B13" s="44">
         <v>120</v>
       </c>
@@ -2426,16 +3783,17 @@
       <c r="E13" s="12"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
-      <c r="H13" s="22"/>
+      <c r="H13" s="20"/>
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22"/>
       <c r="M13" s="22"/>
       <c r="N13" s="22"/>
-      <c r="O13" s="23"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="O13" s="22"/>
+      <c r="P13" s="23"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B14" s="44"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
@@ -2448,40 +3806,44 @@
       <c r="G14" s="21">
         <v>2.5E+19</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="21">
+        <f>+((G14/1000000000000000000)*$N$2^150)*1000000000000000000</f>
+        <v>2.1516084567075938E+19</v>
+      </c>
+      <c r="I14" s="22">
         <f>+F14/SUM(F14:F15)</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="I14" s="22">
-        <f>+G14/SUM(G14:G15)</f>
-        <v>0.26315789473684209</v>
-      </c>
       <c r="J14" s="22">
-        <f>+H14^$I$3</f>
-        <v>0.88018330703271519</v>
+        <f>+H14/SUM(H14:H15)</f>
+        <v>0.25448289734177543</v>
       </c>
       <c r="K14" s="22">
         <f>+I14^$J$3</f>
-        <v>0.66998475538030788</v>
+        <v>0.88018330703271519</v>
       </c>
       <c r="L14" s="22">
-        <f>+K14*J14</f>
-        <v>0.58970939765214414</v>
+        <f>+J14^$K$3</f>
+        <v>0.66328103557648221</v>
       </c>
       <c r="M14" s="22">
-        <f>+L14/SUM(L14:L15)</f>
-        <v>0.69375229677182093</v>
+        <f>+L14*K14</f>
+        <v>0.58380889538579217</v>
       </c>
       <c r="N14" s="22">
-        <f>+$H$3*30*M14</f>
-        <v>20.812568903154627</v>
-      </c>
-      <c r="O14" s="37">
-        <f>+O11+N14</f>
-        <v>90.590766520643484</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.75">
+        <f>+M14/SUM(M14:M15)</f>
+        <v>0.69086219047673991</v>
+      </c>
+      <c r="O14" s="22">
+        <f>+$I$3*30*N14</f>
+        <v>20.725865714302198</v>
+      </c>
+      <c r="P14" s="37">
+        <f>+P11+O14</f>
+        <v>90.504063331791059</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B15" s="44"/>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
@@ -2494,40 +3856,44 @@
       <c r="G15" s="21">
         <v>7E+19</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="21">
+        <f>+((G12/1000000000000000000)*$N$2^150)*1000000000000000000+20000000000000000000</f>
+        <v>6.3032169134151877E+19</v>
+      </c>
+      <c r="I15" s="22">
         <f>+F15/SUM(F14:F15)</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="I15" s="22">
-        <f>+G15/SUM(G14:G15)</f>
-        <v>0.73684210526315785</v>
-      </c>
       <c r="J15" s="22">
-        <f>+H15^$I$3</f>
-        <v>0.28529497656828423</v>
+        <f>+H15/SUM(H14:H15)</f>
+        <v>0.74551710265822468</v>
       </c>
       <c r="K15" s="22">
         <f>+I15^$J$3</f>
-        <v>0.91245683854817927</v>
+        <v>0.28529497656828423</v>
       </c>
       <c r="L15" s="22">
-        <f>+K15*J15</f>
-        <v>0.2603193523731735</v>
+        <f>+J15^$K$3</f>
+        <v>0.91566641064654108</v>
       </c>
       <c r="M15" s="22">
-        <f>+L15/SUM(L14:L15)</f>
-        <v>0.30624770322817907</v>
+        <f>+L15*K15</f>
+        <v>0.26123502716976987</v>
       </c>
       <c r="N15" s="22">
-        <f>+$H$3*30*M15</f>
-        <v>9.1874310968453727</v>
-      </c>
-      <c r="O15" s="37">
-        <f>+O12+N15</f>
-        <v>59.409233479356516</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.75">
+        <f>+M15/SUM(M14:M15)</f>
+        <v>0.30913780952326009</v>
+      </c>
+      <c r="O15" s="22">
+        <f>+$I$3*30*N15</f>
+        <v>9.2741342856978033</v>
+      </c>
+      <c r="P15" s="37">
+        <f>+P12+O15</f>
+        <v>59.495936668208948</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B16" s="44">
         <v>150</v>
       </c>
@@ -2544,40 +3910,44 @@
       <c r="G16" s="20">
         <v>2.5E+19</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="21">
+        <f>+((G16/1000000000000000000)*$N$2^220)*1000000000000000000</f>
+        <v>2.0060761671517315E+19</v>
+      </c>
+      <c r="I16" s="22">
         <f>+F16/SUM(F16:F17)</f>
         <v>0.625</v>
       </c>
-      <c r="I16" s="22">
-        <f>+G16/SUM(G16:G17)</f>
+      <c r="J16" s="22">
+        <f>+H16/SUM(H16:H17)</f>
         <v>0.26315789473684209</v>
-      </c>
-      <c r="J16" s="22">
-        <f>+H16^$I$3</f>
-        <v>0.71964118851645298</v>
       </c>
       <c r="K16" s="22">
         <f>+I16^$J$3</f>
+        <v>0.71964118851645298</v>
+      </c>
+      <c r="L16" s="22">
+        <f>+J16^$K$3</f>
         <v>0.66998475538030788</v>
       </c>
-      <c r="L16" s="22">
-        <f>+K16*J16</f>
+      <c r="M16" s="22">
+        <f>+L16*K16</f>
         <v>0.48214862564978977</v>
       </c>
-      <c r="M16" s="22">
-        <f>+L16/SUM(L16:L17)</f>
+      <c r="N16" s="22">
+        <f>+M16/SUM(M16:M17)</f>
         <v>0.51217062333254171</v>
       </c>
-      <c r="N16" s="22">
-        <f>+$H$3*70*M16</f>
+      <c r="O16" s="22">
+        <f>+$I$3*70*N16</f>
         <v>35.851943633277919</v>
       </c>
-      <c r="O16" s="37">
-        <f>+O14+N16</f>
-        <v>126.44271015392141</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="P16" s="37">
+        <f>+P14+O16</f>
+        <v>126.35600696506899</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B17" s="44"/>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
@@ -2590,40 +3960,44 @@
       <c r="G17" s="20">
         <v>7E+19</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="21">
+        <f>+((G17/1000000000000000000)*$N$2^220)*1000000000000000000</f>
+        <v>5.6170132680248484E+19</v>
+      </c>
+      <c r="I17" s="22">
         <f>+F17/SUM(F16:F17)</f>
         <v>0.375</v>
       </c>
-      <c r="I17" s="22">
-        <f>+G17/SUM(G16:G17)</f>
+      <c r="J17" s="22">
+        <f>+H17/SUM(H16:H17)</f>
         <v>0.73684210526315785</v>
-      </c>
-      <c r="J17" s="22">
-        <f>+H17^$I$3</f>
-        <v>0.50329415576044101</v>
       </c>
       <c r="K17" s="22">
         <f>+I17^$J$3</f>
+        <v>0.50329415576044101</v>
+      </c>
+      <c r="L17" s="22">
+        <f>+J17^$K$3</f>
         <v>0.91245683854817927</v>
       </c>
-      <c r="L17" s="22">
-        <f>+K17*J17</f>
+      <c r="M17" s="22">
+        <f>+L17*K17</f>
         <v>0.45923419422494693</v>
       </c>
-      <c r="M17" s="22">
-        <f>+L17/SUM(L16:L17)</f>
+      <c r="N17" s="22">
+        <f>+M17/SUM(M16:M17)</f>
         <v>0.48782937666745824</v>
       </c>
-      <c r="N17" s="22">
-        <f>+$H$3*70*M17</f>
+      <c r="O17" s="22">
+        <f>+$I$3*70*N17</f>
         <v>34.148056366722074</v>
       </c>
-      <c r="O17" s="37">
-        <f>+O15+N17</f>
-        <v>93.557289846078589</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="P17" s="37">
+        <f>+P15+O17</f>
+        <v>93.643993034931015</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B18" s="44">
         <v>220</v>
       </c>
@@ -2634,16 +4008,17 @@
       <c r="E18" s="12"/>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
-      <c r="H18" s="22"/>
+      <c r="H18" s="20"/>
       <c r="I18" s="22"/>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
       <c r="L18" s="22"/>
       <c r="M18" s="22"/>
       <c r="N18" s="22"/>
-      <c r="O18" s="37"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="O18" s="22"/>
+      <c r="P18" s="37"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B19" s="44"/>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
@@ -2656,40 +4031,44 @@
       <c r="G19" s="20">
         <v>2.5E+19</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="21">
+        <f>+((G19/1000000000000000000)*$N$2^250)*1000000000000000000</f>
+        <v>1.9467584352924791E+19</v>
+      </c>
+      <c r="I19" s="22">
         <f>+F19/SUM(F19:F20)</f>
         <v>0.5714285714285714</v>
       </c>
-      <c r="I19" s="22">
-        <f>+G19/SUM(G19:G20)</f>
+      <c r="J19" s="22">
+        <f>+H19/SUM(H19:H20)</f>
         <v>0.26315789473684209</v>
-      </c>
-      <c r="J19" s="22">
-        <f>+H19^$I$3</f>
-        <v>0.67588586797162753</v>
       </c>
       <c r="K19" s="22">
         <f>+I19^$J$3</f>
+        <v>0.67588586797162753</v>
+      </c>
+      <c r="L19" s="22">
+        <f>+J19^$K$3</f>
         <v>0.66998475538030788</v>
       </c>
-      <c r="L19" s="22">
-        <f>+K19*J19</f>
+      <c r="M19" s="22">
+        <f>+L19*K19</f>
         <v>0.45283322791797792</v>
       </c>
-      <c r="M19" s="22">
-        <f>+L19/SUM(L19:L20)</f>
+      <c r="N19" s="22">
+        <f>+M19/SUM(M19:M20)</f>
         <v>0.4731487637387678</v>
       </c>
-      <c r="N19" s="22">
-        <f>+$H$3*30*M19</f>
+      <c r="O19" s="22">
+        <f>+$I$3*30*N19</f>
         <v>14.194462912163035</v>
       </c>
-      <c r="O19" s="37">
-        <f>+O16+N19</f>
-        <v>140.63717306608444</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="P19" s="37">
+        <f>+P16+O19</f>
+        <v>140.55046987723202</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B20" s="44"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
@@ -2702,40 +4081,44 @@
       <c r="G20" s="20">
         <v>7E+19</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="21">
+        <f>+((G20/1000000000000000000)*$N$2^250)*1000000000000000000</f>
+        <v>5.4509236188189409E+19</v>
+      </c>
+      <c r="I20" s="22">
         <f>+F20/SUM(F19:F20)</f>
         <v>0.42857142857142855</v>
       </c>
-      <c r="I20" s="22">
-        <f>+G20/SUM(G19:G20)</f>
+      <c r="J20" s="22">
+        <f>+H20/SUM(H19:H20)</f>
         <v>0.73684210526315785</v>
-      </c>
-      <c r="J20" s="22">
-        <f>+H20^$I$3</f>
-        <v>0.55260683251119402</v>
       </c>
       <c r="K20" s="22">
         <f>+I20^$J$3</f>
+        <v>0.55260683251119402</v>
+      </c>
+      <c r="L20" s="22">
+        <f>+J20^$K$3</f>
         <v>0.91245683854817927</v>
       </c>
-      <c r="L20" s="22">
-        <f>+K20*J20</f>
+      <c r="M20" s="22">
+        <f>+L20*K20</f>
         <v>0.50422988335328733</v>
       </c>
-      <c r="M20" s="22">
-        <f>+L20/SUM(L19:L20)</f>
+      <c r="N20" s="22">
+        <f>+M20/SUM(M19:M20)</f>
         <v>0.5268512362612322</v>
       </c>
-      <c r="N20" s="22">
-        <f>+$H$3*30*M20</f>
+      <c r="O20" s="22">
+        <f>+$I$3*30*N20</f>
         <v>15.805537087836965</v>
       </c>
-      <c r="O20" s="37">
-        <f>+O17+N20</f>
-        <v>109.36282693391556</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="P20" s="37">
+        <f>+P17+O20</f>
+        <v>109.44953012276798</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B21" s="44">
         <v>250</v>
       </c>
@@ -2746,16 +4129,17 @@
       <c r="E21" s="12"/>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
-      <c r="H21" s="22"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="22"/>
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
       <c r="L21" s="22"/>
       <c r="M21" s="22"/>
       <c r="N21" s="22"/>
-      <c r="O21" s="37"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.75">
+      <c r="O21" s="22"/>
+      <c r="P21" s="37"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B22" s="44"/>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
@@ -2768,40 +4152,44 @@
       <c r="G22" s="20">
         <v>1.25E+20</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="21">
+        <f>+((G19/1000000000000000000)*$N$2^300)*1000000000000000000+100000000000000000000</f>
+        <v>1.1851767580390253E+20</v>
+      </c>
+      <c r="I22" s="22">
         <f>+F22/SUM(F22:F23)</f>
         <v>0.5714285714285714</v>
       </c>
-      <c r="I22" s="22">
-        <f>+G22/SUM(G22:G23)</f>
-        <v>0.64102564102564108</v>
-      </c>
       <c r="J22" s="22">
-        <f>+H22^$I$3</f>
-        <v>0.67588586797162753</v>
+        <f>+H22/SUM(H22:H23)</f>
+        <v>0.69566030331477802</v>
       </c>
       <c r="K22" s="22">
         <f>+I22^$J$3</f>
-        <v>0.87510994737242054</v>
+        <v>0.67588586797162753</v>
       </c>
       <c r="L22" s="22">
-        <f>+K22*J22</f>
-        <v>0.5914744463504138</v>
+        <f>+J22^$K$3</f>
+        <v>0.89684866608398484</v>
       </c>
       <c r="M22" s="22">
-        <f>+L22/SUM(L22:L23)</f>
-        <v>0.59274457381575263</v>
+        <f>+L22*K22</f>
+        <v>0.60616733911537046</v>
       </c>
       <c r="N22" s="22">
-        <f>+$H$3*50*M22</f>
-        <v>29.63722869078763</v>
-      </c>
-      <c r="O22" s="37">
-        <f>+O19+N22</f>
-        <v>170.27440175687207</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.75">
+        <f>+M22/SUM(M22:M23)</f>
+        <v>0.61049479562347297</v>
+      </c>
+      <c r="O22" s="22">
+        <f>+$I$3*50*N22</f>
+        <v>30.52473978117365</v>
+      </c>
+      <c r="P22" s="37">
+        <f>+P19+O22</f>
+        <v>171.07520965840567</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.75">
       <c r="B23" s="45">
         <v>300</v>
       </c>
@@ -2818,64 +4206,68 @@
       <c r="G23" s="6">
         <v>7E+19</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="48">
+        <f>+((G23/1000000000000000000)*$N$2^300)*1000000000000000000</f>
+        <v>5.1849492250927088E+19</v>
+      </c>
+      <c r="I23" s="7">
         <f>+F23/SUM(F22:F23)</f>
         <v>0.42857142857142855</v>
       </c>
-      <c r="I23" s="7">
-        <f>+G23/SUM(G22:G23)</f>
-        <v>0.35897435897435898</v>
-      </c>
       <c r="J23" s="7">
-        <f>+H23^$I$3</f>
-        <v>0.55260683251119402</v>
+        <f>+H23/SUM(H22:H23)</f>
+        <v>0.30433969668522198</v>
       </c>
       <c r="K23" s="7">
         <f>+I23^$J$3</f>
-        <v>0.73539221595033788</v>
+        <v>0.55260683251119402</v>
       </c>
       <c r="L23" s="7">
-        <f>+K23*J23</f>
-        <v>0.40638276310970417</v>
+        <f>+J23^$K$3</f>
+        <v>0.69985421253502034</v>
       </c>
       <c r="M23" s="7">
-        <f>+L23/SUM(L22:L23)</f>
-        <v>0.40725542618424743</v>
+        <f>+L23*K23</f>
+        <v>0.38674421960859356</v>
       </c>
       <c r="N23" s="7">
-        <f>+$H$3*50*M23</f>
-        <v>20.36277130921237</v>
-      </c>
-      <c r="O23" s="38">
-        <f>+O20+N23</f>
-        <v>129.72559824312793</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+        <f>+M23/SUM(M22:M23)</f>
+        <v>0.38950520437652697</v>
+      </c>
+      <c r="O23" s="7">
+        <f>+$I$3*50*N23</f>
+        <v>19.47526021882635</v>
+      </c>
+      <c r="P23" s="38">
+        <f>+P20+O23</f>
+        <v>128.92479034159433</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="E25" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="2:15" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+    <row r="26" spans="2:16" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
       <c r="E26" s="12" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="41">
-        <f>+SUM(N8,N11,N14,N16,N19,N22)</f>
-        <v>170.27440175687207</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.75">
+        <f>+SUM(O8,O11,O14,O16,O19,O22)</f>
+        <v>171.07520965840567</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.75">
       <c r="E27" s="13" t="s">
         <v>25</v>
       </c>
       <c r="F27" s="42">
-        <f>+SUM(N9,N12,N15,N17,N20,N23)</f>
-        <v>129.72559824312793</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.75">
+        <f>+SUM(O9,O12,O15,O17,O20,O23)</f>
+        <v>128.92479034159433</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.75">
       <c r="E28" s="14" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
feat: new scripts to deploy and upgrade proxy
</commit_message>
<xml_diff>
--- a/20210921 - Staking Rewards.xlsx
+++ b/20210921 - Staking Rewards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Documents\16slimchance16\token\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3359C63-0188-4F6B-9F87-084DF9F462FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FA64621-B9FE-440B-B8E4-F569C36FAF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="-90" windowWidth="16490" windowHeight="10980" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="-90" windowWidth="16490" windowHeight="10980" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SNX" sheetId="1" state="hidden" r:id="rId1"/>
@@ -18,8 +18,10 @@
     <sheet name="KWENTA" sheetId="5" state="hidden" r:id="rId3"/>
     <sheet name="KWENTA - power" sheetId="6" r:id="rId4"/>
     <sheet name="KWENTA - Decay" sheetId="7" r:id="rId5"/>
+    <sheet name="KWENTA - Final" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="52">
   <si>
     <t>N stake 20</t>
   </si>
@@ -200,7 +202,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000000E+00"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
@@ -208,9 +210,10 @@
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
     <numFmt numFmtId="169" formatCode="0.0%"/>
-    <numFmt numFmtId="172" formatCode="0.000000"/>
-    <numFmt numFmtId="174" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="175" formatCode="0.000E+00"/>
+    <numFmt numFmtId="170" formatCode="0.000000"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="172" formatCode="0.000E+00"/>
+    <numFmt numFmtId="173" formatCode="#,##0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -466,7 +469,6 @@
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -478,9 +480,10 @@
     <xf numFmtId="168" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="175" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2136,8 +2139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486B17B1-BE12-4310-9A3F-24B7422EA458}">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2418,7 +2421,7 @@
         <f>+$H$3*60*M8</f>
         <v>26.892028880393454</v>
       </c>
-      <c r="O8" s="70">
+      <c r="O8" s="84">
         <f>+N8</f>
         <v>26.892028880393454</v>
       </c>
@@ -2476,7 +2479,7 @@
         <f>+$H$3*60*M9</f>
         <v>33.107971119606546</v>
       </c>
-      <c r="O9" s="70">
+      <c r="O9" s="84">
         <f>+N9</f>
         <v>33.107971119606546</v>
       </c>
@@ -2511,7 +2514,7 @@
       <c r="L10" s="68"/>
       <c r="M10" s="68"/>
       <c r="N10" s="68"/>
-      <c r="O10" s="71"/>
+      <c r="O10" s="70"/>
       <c r="P10" s="49"/>
       <c r="Q10" s="49"/>
       <c r="R10" s="49">
@@ -2566,7 +2569,7 @@
         <f>+$H$3*60*M11</f>
         <v>42.886168737095403</v>
       </c>
-      <c r="O11" s="72">
+      <c r="O11" s="71">
         <f>+N11+N8</f>
         <v>69.778197617488857</v>
       </c>
@@ -2618,7 +2621,7 @@
         <f>+$H$3*60*M12</f>
         <v>17.113831262904597</v>
       </c>
-      <c r="O12" s="72">
+      <c r="O12" s="71">
         <f>+N12+N9</f>
         <v>50.221802382511143</v>
       </c>
@@ -2650,7 +2653,7 @@
       <c r="L13" s="68"/>
       <c r="M13" s="68"/>
       <c r="N13" s="68"/>
-      <c r="O13" s="71"/>
+      <c r="O13" s="70"/>
       <c r="P13" s="49"/>
       <c r="Q13" s="49"/>
       <c r="R13" s="49">
@@ -2702,7 +2705,7 @@
         <f>+$H$3*30*M14</f>
         <v>20.812568903154627</v>
       </c>
-      <c r="O14" s="72">
+      <c r="O14" s="71">
         <f>+O11+N14</f>
         <v>90.590766520643484</v>
       </c>
@@ -2754,7 +2757,7 @@
         <f>+$H$3*30*M15</f>
         <v>9.1874310968453727</v>
       </c>
-      <c r="O15" s="72">
+      <c r="O15" s="71">
         <f>+O12+N15</f>
         <v>59.409233479356516</v>
       </c>
@@ -2810,7 +2813,7 @@
         <f>+$H$3*70*M16</f>
         <v>35.851943633277919</v>
       </c>
-      <c r="O16" s="72">
+      <c r="O16" s="71">
         <f>+O14+N16</f>
         <v>126.44271015392141</v>
       </c>
@@ -2862,7 +2865,7 @@
         <f>+$H$3*70*M17</f>
         <v>34.148056366722074</v>
       </c>
-      <c r="O17" s="72">
+      <c r="O17" s="71">
         <f>+O15+N17</f>
         <v>93.557289846078589</v>
       </c>
@@ -2894,7 +2897,7 @@
       <c r="L18" s="68"/>
       <c r="M18" s="68"/>
       <c r="N18" s="68"/>
-      <c r="O18" s="72"/>
+      <c r="O18" s="71"/>
       <c r="P18" s="49"/>
       <c r="Q18" s="49"/>
       <c r="R18" s="49">
@@ -2946,7 +2949,7 @@
         <f>+$H$3*30*M19</f>
         <v>14.194462912163035</v>
       </c>
-      <c r="O19" s="72">
+      <c r="O19" s="71">
         <f>+O16+N19</f>
         <v>140.63717306608444</v>
       </c>
@@ -3001,7 +3004,7 @@
         <f>+$H$3*30*M20</f>
         <v>15.805537087836965</v>
       </c>
-      <c r="O20" s="72">
+      <c r="O20" s="71">
         <f>+O17+N20</f>
         <v>109.36282693391556</v>
       </c>
@@ -3036,13 +3039,13 @@
       <c r="L21" s="68"/>
       <c r="M21" s="68"/>
       <c r="N21" s="68"/>
-      <c r="O21" s="72"/>
+      <c r="O21" s="71"/>
       <c r="P21" s="49"/>
       <c r="Q21" s="49">
         <f>+Q20^(0.3*60)</f>
         <v>0.98215218705145069</v>
       </c>
-      <c r="R21" s="84">
+      <c r="R21" s="83">
         <f>+R20/(Q21*1000000000000000000)</f>
         <v>2.0799973340265288E+18</v>
       </c>
@@ -3091,7 +3094,7 @@
         <f>+$H$3*50*M22</f>
         <v>29.63722869078763</v>
       </c>
-      <c r="O22" s="72">
+      <c r="O22" s="71">
         <f>+O19+N22</f>
         <v>170.27440175687207</v>
       </c>
@@ -3103,14 +3106,14 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.75">
       <c r="A23" s="49"/>
-      <c r="B23" s="73">
+      <c r="B23" s="72">
         <v>300</v>
       </c>
       <c r="C23" s="56" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="56"/>
-      <c r="E23" s="74" t="s">
+      <c r="E23" s="73" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="56">
@@ -3119,35 +3122,35 @@
       <c r="G23" s="56">
         <v>7E+19</v>
       </c>
-      <c r="H23" s="75">
+      <c r="H23" s="74">
         <f>+F23/SUM(F22:F23)</f>
         <v>0.42857142857142855</v>
       </c>
-      <c r="I23" s="75">
+      <c r="I23" s="74">
         <f>+G23/SUM(G22:G23)</f>
         <v>0.35897435897435898</v>
       </c>
-      <c r="J23" s="75">
+      <c r="J23" s="74">
         <f>+H23^$I$3</f>
         <v>0.55260683251119402</v>
       </c>
-      <c r="K23" s="75">
+      <c r="K23" s="74">
         <f>+I23^$J$3</f>
         <v>0.73539221595033788</v>
       </c>
-      <c r="L23" s="75">
+      <c r="L23" s="74">
         <f>+K23*J23</f>
         <v>0.40638276310970417</v>
       </c>
-      <c r="M23" s="75">
+      <c r="M23" s="74">
         <f>+L23/SUM(L22:L23)</f>
         <v>0.40725542618424743</v>
       </c>
-      <c r="N23" s="75">
+      <c r="N23" s="74">
         <f>+$H$3*50*M23</f>
         <v>20.36277130921237</v>
       </c>
-      <c r="O23" s="76">
+      <c r="O23" s="75">
         <f>+O20+N23</f>
         <v>129.72559824312793</v>
       </c>
@@ -3184,10 +3187,10 @@
       <c r="B25" s="49"/>
       <c r="C25" s="49"/>
       <c r="D25" s="49"/>
-      <c r="E25" s="77" t="s">
+      <c r="E25" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="78"/>
+      <c r="F25" s="77"/>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
       <c r="I25" s="49"/>
@@ -3211,7 +3214,7 @@
       <c r="E26" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="79">
+      <c r="F26" s="78">
         <f>+SUM(N8,N11,N14,N16,N19,N22)</f>
         <v>170.27440175687207</v>
       </c>
@@ -3220,7 +3223,7 @@
       <c r="I26" s="49"/>
       <c r="J26" s="49"/>
       <c r="K26" s="50"/>
-      <c r="L26" s="82"/>
+      <c r="L26" s="81"/>
       <c r="M26" s="49"/>
       <c r="N26" s="51"/>
       <c r="O26" s="49"/>
@@ -3235,10 +3238,10 @@
       <c r="B27" s="49"/>
       <c r="C27" s="49"/>
       <c r="D27" s="49"/>
-      <c r="E27" s="74" t="s">
+      <c r="E27" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="80">
+      <c r="F27" s="79">
         <f>+SUM(N9,N12,N15,N17,N20,N23)</f>
         <v>129.72559824312793</v>
       </c>
@@ -3249,7 +3252,7 @@
       <c r="K27" s="50">
         <v>0.999</v>
       </c>
-      <c r="L27" s="83">
+      <c r="L27" s="82">
         <f>+K27*1000000000000000000</f>
         <v>9.99E+17</v>
       </c>
@@ -3267,10 +3270,10 @@
       <c r="B28" s="49"/>
       <c r="C28" s="49"/>
       <c r="D28" s="49"/>
-      <c r="E28" s="73" t="s">
+      <c r="E28" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="81">
+      <c r="F28" s="80">
         <f>+SUM(F26:F27)</f>
         <v>300</v>
       </c>
@@ -4279,4 +4282,1265 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272DD5C9-D190-4388-8820-6AF1434A50B5}">
+  <dimension ref="A1:T32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="2" max="2" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.31640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.76953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.04296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.76953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.6796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+    </row>
+    <row r="2" spans="1:20" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A2" s="49"/>
+      <c r="B2" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="52"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="50"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+    </row>
+    <row r="3" spans="1:20" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="A3" s="49"/>
+      <c r="B3" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="49">
+        <v>25</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49">
+        <v>300</v>
+      </c>
+      <c r="G3" s="49">
+        <v>300</v>
+      </c>
+      <c r="H3" s="49">
+        <v>1</v>
+      </c>
+      <c r="I3" s="49">
+        <v>0.7</v>
+      </c>
+      <c r="J3" s="49">
+        <v>0.3</v>
+      </c>
+      <c r="K3" s="50"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A4" s="49"/>
+      <c r="B4" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="49">
+        <v>50</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A5" s="49"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A6" s="49"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A7" s="49"/>
+      <c r="B7" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="60"/>
+      <c r="E7" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="49"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A8" s="49"/>
+      <c r="B8" s="64">
+        <v>0</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="65"/>
+      <c r="E8" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="65">
+        <v>1E+19</v>
+      </c>
+      <c r="G8" s="67">
+        <v>2.5E+19</v>
+      </c>
+      <c r="H8" s="68">
+        <f>+F8/SUM(F8:F9)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="68">
+        <f>+G8/SUM(G8:G9)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J8" s="68">
+        <f>+H8^$I$3</f>
+        <v>0.61557220667245816</v>
+      </c>
+      <c r="K8" s="68">
+        <f>+I8^$J$3</f>
+        <v>0.71922309332486434</v>
+      </c>
+      <c r="L8" s="68">
+        <f>+K8*J8</f>
+        <v>0.44273374664777804</v>
+      </c>
+      <c r="M8" s="69">
+        <f>+L8/SUM(L8:L9)</f>
+        <v>0.44820048133989088</v>
+      </c>
+      <c r="N8" s="68">
+        <f>+$H$3*60*M8</f>
+        <v>26.892028880393454</v>
+      </c>
+      <c r="O8" s="84">
+        <f>+N8</f>
+        <v>26.892028880393454</v>
+      </c>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49">
+        <f>10^0.7</f>
+        <v>5.0118723362727229</v>
+      </c>
+      <c r="S8" s="49">
+        <f>10^0.7</f>
+        <v>5.0118723362727229</v>
+      </c>
+      <c r="T8" s="49"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A9" s="49"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="65">
+        <v>1E+19</v>
+      </c>
+      <c r="G9" s="67">
+        <v>5E+19</v>
+      </c>
+      <c r="H9" s="68">
+        <f>+F9/SUM(F8:F9)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="68">
+        <f>+G9/SUM(G8:G9)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J9" s="68">
+        <f>+H9^$I$3</f>
+        <v>0.61557220667245816</v>
+      </c>
+      <c r="K9" s="68">
+        <f>+I9^$J$3</f>
+        <v>0.88546749329555607</v>
+      </c>
+      <c r="L9" s="68">
+        <f>+K9*J9</f>
+        <v>0.54506917878467553</v>
+      </c>
+      <c r="M9" s="69">
+        <f>+L9/SUM(L8:L9)</f>
+        <v>0.55179951866010912</v>
+      </c>
+      <c r="N9" s="68">
+        <f>+$H$3*60*M9</f>
+        <v>33.107971119606546</v>
+      </c>
+      <c r="O9" s="84">
+        <f>+N9</f>
+        <v>33.107971119606546</v>
+      </c>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49">
+        <f>25^0.3</f>
+        <v>2.626527804403767</v>
+      </c>
+      <c r="S9" s="49">
+        <f>50^0.3</f>
+        <v>3.2336350328867871</v>
+      </c>
+      <c r="T9" s="49"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A10" s="49"/>
+      <c r="B10" s="64">
+        <v>60</v>
+      </c>
+      <c r="C10" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="65"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="70"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49">
+        <f>+R9*R8</f>
+        <v>13.163822043342373</v>
+      </c>
+      <c r="S10" s="49">
+        <f>+S9*S8</f>
+        <v>16.206565966927624</v>
+      </c>
+      <c r="T10" s="49"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A11" s="49"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="65">
+        <v>5E+19</v>
+      </c>
+      <c r="G11" s="67">
+        <v>2.5E+19</v>
+      </c>
+      <c r="H11" s="68">
+        <f>+F11/SUM(F11:F12)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I11" s="68">
+        <f>+G11/SUM(G11:G12)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J11" s="68">
+        <f>+H11^$I$3</f>
+        <v>0.88018330703271519</v>
+      </c>
+      <c r="K11" s="68">
+        <f>+I11^$J$3</f>
+        <v>0.71922309332486434</v>
+      </c>
+      <c r="L11" s="68">
+        <f>+K11*J11</f>
+        <v>0.63304816077697823</v>
+      </c>
+      <c r="M11" s="68">
+        <f>+L11/SUM(L11:L12)</f>
+        <v>0.71476947895159004</v>
+      </c>
+      <c r="N11" s="68">
+        <f>+$H$3*60*M11</f>
+        <v>42.886168737095403</v>
+      </c>
+      <c r="O11" s="71">
+        <f>+N11+N8</f>
+        <v>69.778197617488857</v>
+      </c>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A12" s="49"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="65">
+        <v>1E+19</v>
+      </c>
+      <c r="G12" s="67">
+        <v>5E+19</v>
+      </c>
+      <c r="H12" s="68">
+        <f>+F12/SUM(F11:F12)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I12" s="68">
+        <f>+G12/SUM(G11:G12)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J12" s="68">
+        <f>+H12^$I$3</f>
+        <v>0.28529497656828423</v>
+      </c>
+      <c r="K12" s="68">
+        <f>+I12^$J$3</f>
+        <v>0.88546749329555607</v>
+      </c>
+      <c r="L12" s="68">
+        <f>+K12*J12</f>
+        <v>0.25261942775173307</v>
+      </c>
+      <c r="M12" s="68">
+        <f>+L12/SUM(L11:L12)</f>
+        <v>0.28523052104840996</v>
+      </c>
+      <c r="N12" s="68">
+        <f>+$H$3*60*M12</f>
+        <v>17.113831262904597</v>
+      </c>
+      <c r="O12" s="71">
+        <f>+N12+N9</f>
+        <v>50.221802382511143</v>
+      </c>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49">
+        <f>+R10+S10</f>
+        <v>29.370388010269998</v>
+      </c>
+      <c r="S12" s="49"/>
+      <c r="T12" s="49"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A13" s="49"/>
+      <c r="B13" s="64">
+        <v>120</v>
+      </c>
+      <c r="C13" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="65"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="70"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49">
+        <f>1/R12/60</f>
+        <v>5.6746498074314853E-4</v>
+      </c>
+      <c r="S13" s="49"/>
+      <c r="T13" s="49"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A14" s="49"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="65">
+        <v>5E+19</v>
+      </c>
+      <c r="G14" s="67">
+        <v>2.5E+19</v>
+      </c>
+      <c r="H14" s="68">
+        <f>+F14/SUM(F14:F15)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I14" s="68">
+        <f>+G14/SUM(G14:G15)</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="J14" s="68">
+        <f>+H14^$I$3</f>
+        <v>0.88018330703271519</v>
+      </c>
+      <c r="K14" s="68">
+        <f>+I14^$J$3</f>
+        <v>0.66998475538030788</v>
+      </c>
+      <c r="L14" s="68">
+        <f>+K14*J14</f>
+        <v>0.58970939765214414</v>
+      </c>
+      <c r="M14" s="68">
+        <f>+L14/SUM(L14:L15)</f>
+        <v>0.69375229677182093</v>
+      </c>
+      <c r="N14" s="68">
+        <f>+$H$3*30*M14</f>
+        <v>20.812568903154627</v>
+      </c>
+      <c r="O14" s="71">
+        <f>+O11+N14</f>
+        <v>90.590766520643484</v>
+      </c>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="49"/>
+      <c r="T14" s="49"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A15" s="49"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="65">
+        <v>1E+19</v>
+      </c>
+      <c r="G15" s="67">
+        <v>7E+19</v>
+      </c>
+      <c r="H15" s="68">
+        <f>+F15/SUM(F14:F15)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I15" s="68">
+        <f>+G15/SUM(G14:G15)</f>
+        <v>0.73684210526315785</v>
+      </c>
+      <c r="J15" s="68">
+        <f>+H15^$I$3</f>
+        <v>0.28529497656828423</v>
+      </c>
+      <c r="K15" s="68">
+        <f>+I15^$J$3</f>
+        <v>0.91245683854817927</v>
+      </c>
+      <c r="L15" s="68">
+        <f>+K15*J15</f>
+        <v>0.2603193523731735</v>
+      </c>
+      <c r="M15" s="68">
+        <f>+L15/SUM(L14:L15)</f>
+        <v>0.30624770322817907</v>
+      </c>
+      <c r="N15" s="68">
+        <f>+$H$3*30*M15</f>
+        <v>9.1874310968453727</v>
+      </c>
+      <c r="O15" s="71">
+        <f>+O12+N15</f>
+        <v>59.409233479356516</v>
+      </c>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="49"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A16" s="49"/>
+      <c r="B16" s="64">
+        <v>150</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="65"/>
+      <c r="E16" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="65">
+        <v>5E+19</v>
+      </c>
+      <c r="G16" s="65">
+        <v>2.5E+19</v>
+      </c>
+      <c r="H16" s="68">
+        <f>+F16/SUM(F16:F17)</f>
+        <v>0.625</v>
+      </c>
+      <c r="I16" s="68">
+        <f>+G16/SUM(G16:G17)</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="J16" s="68">
+        <f>+H16^$I$3</f>
+        <v>0.71964118851645298</v>
+      </c>
+      <c r="K16" s="68">
+        <f>+I16^$J$3</f>
+        <v>0.66998475538030788</v>
+      </c>
+      <c r="L16" s="68">
+        <f>+K16*J16</f>
+        <v>0.48214862564978977</v>
+      </c>
+      <c r="M16" s="68">
+        <f>+L16/SUM(L16:L17)</f>
+        <v>0.51217062333254171</v>
+      </c>
+      <c r="N16" s="68">
+        <f>+$H$3*70*M16</f>
+        <v>35.851943633277919</v>
+      </c>
+      <c r="O16" s="71">
+        <f>+O14+N16</f>
+        <v>126.44271015392141</v>
+      </c>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="49"/>
+      <c r="S16" s="49"/>
+      <c r="T16" s="49"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A17" s="49"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="65">
+        <v>3E+19</v>
+      </c>
+      <c r="G17" s="65">
+        <v>7E+19</v>
+      </c>
+      <c r="H17" s="68">
+        <f>+F17/SUM(F16:F17)</f>
+        <v>0.375</v>
+      </c>
+      <c r="I17" s="68">
+        <f>+G17/SUM(G16:G17)</f>
+        <v>0.73684210526315785</v>
+      </c>
+      <c r="J17" s="68">
+        <f>+H17^$I$3</f>
+        <v>0.50329415576044101</v>
+      </c>
+      <c r="K17" s="68">
+        <f>+I17^$J$3</f>
+        <v>0.91245683854817927</v>
+      </c>
+      <c r="L17" s="68">
+        <f>+K17*J17</f>
+        <v>0.45923419422494693</v>
+      </c>
+      <c r="M17" s="68">
+        <f>+L17/SUM(L16:L17)</f>
+        <v>0.48782937666745824</v>
+      </c>
+      <c r="N17" s="68">
+        <f>+$H$3*70*M17</f>
+        <v>34.148056366722074</v>
+      </c>
+      <c r="O17" s="71">
+        <f>+O15+N17</f>
+        <v>93.557289846078589</v>
+      </c>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49">
+        <f>60*1000000000000000000</f>
+        <v>6E+19</v>
+      </c>
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A18" s="49"/>
+      <c r="B18" s="64">
+        <v>220</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="65"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="68"/>
+      <c r="O18" s="71"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="49">
+        <f>+R17*10000</f>
+        <v>6.0000000000000002E+23</v>
+      </c>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A19" s="49"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="65">
+        <v>4E+19</v>
+      </c>
+      <c r="G19" s="65">
+        <v>2.5E+19</v>
+      </c>
+      <c r="H19" s="68">
+        <f>+F19/SUM(F19:F20)</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="I19" s="68">
+        <f>+G19/SUM(G19:G20)</f>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="J19" s="68">
+        <f>+H19^$I$3</f>
+        <v>0.67588586797162753</v>
+      </c>
+      <c r="K19" s="68">
+        <f>+I19^$J$3</f>
+        <v>0.66998475538030788</v>
+      </c>
+      <c r="L19" s="68">
+        <f>+K19*J19</f>
+        <v>0.45283322791797792</v>
+      </c>
+      <c r="M19" s="68">
+        <f>+L19/SUM(L19:L20)</f>
+        <v>0.4731487637387678</v>
+      </c>
+      <c r="N19" s="68">
+        <f>+$H$3*30*M19</f>
+        <v>14.194462912163035</v>
+      </c>
+      <c r="O19" s="71">
+        <f>+O16+N19</f>
+        <v>140.63717306608444</v>
+      </c>
+      <c r="P19" s="49"/>
+      <c r="Q19" s="49"/>
+      <c r="R19" s="49">
+        <f>+R18*1E+50</f>
+        <v>6.0000000000000002E+73</v>
+      </c>
+      <c r="S19" s="49"/>
+      <c r="T19" s="49"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A20" s="49"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="65">
+        <v>3E+19</v>
+      </c>
+      <c r="G20" s="65">
+        <v>7E+19</v>
+      </c>
+      <c r="H20" s="68">
+        <f>+F20/SUM(F19:F20)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="I20" s="68">
+        <f>+G20/SUM(G19:G20)</f>
+        <v>0.73684210526315785</v>
+      </c>
+      <c r="J20" s="68">
+        <f>+H20^$I$3</f>
+        <v>0.55260683251119402</v>
+      </c>
+      <c r="K20" s="68">
+        <f>+I20^$J$3</f>
+        <v>0.91245683854817927</v>
+      </c>
+      <c r="L20" s="68">
+        <f>+K20*J20</f>
+        <v>0.50422988335328733</v>
+      </c>
+      <c r="M20" s="68">
+        <f>+L20/SUM(L19:L20)</f>
+        <v>0.5268512362612322</v>
+      </c>
+      <c r="N20" s="68">
+        <f>+$H$3*30*M20</f>
+        <v>15.805537087836965</v>
+      </c>
+      <c r="O20" s="71">
+        <f>+O17+N20</f>
+        <v>109.36282693391556</v>
+      </c>
+      <c r="P20" s="49"/>
+      <c r="Q20" s="50">
+        <f>+K27</f>
+        <v>0.999</v>
+      </c>
+      <c r="R20" s="49">
+        <f>+R19/2.93703880102699E+37</f>
+        <v>2.0428739306753418E+36</v>
+      </c>
+      <c r="S20" s="49"/>
+      <c r="T20" s="49"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A21" s="49"/>
+      <c r="B21" s="64">
+        <v>250</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="65"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="68"/>
+      <c r="K21" s="68"/>
+      <c r="L21" s="68"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="68"/>
+      <c r="O21" s="71"/>
+      <c r="P21" s="49"/>
+      <c r="Q21" s="49">
+        <f>+Q20^(0.3*60)</f>
+        <v>0.98215218705145069</v>
+      </c>
+      <c r="R21" s="83">
+        <f>+R20/(Q21*1000000000000000000)</f>
+        <v>2.0799973340265288E+18</v>
+      </c>
+      <c r="S21" s="49"/>
+      <c r="T21" s="49"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A22" s="49"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="65">
+        <v>4E+19</v>
+      </c>
+      <c r="G22" s="65">
+        <v>1.25E+20</v>
+      </c>
+      <c r="H22" s="68">
+        <f>+F22/SUM(F22:F23)</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="I22" s="68">
+        <f>+G22/SUM(G22:G23)</f>
+        <v>0.64102564102564108</v>
+      </c>
+      <c r="J22" s="68">
+        <f>+H22^$I$3</f>
+        <v>0.67588586797162753</v>
+      </c>
+      <c r="K22" s="68">
+        <f>+I22^$J$3</f>
+        <v>0.87510994737242054</v>
+      </c>
+      <c r="L22" s="68">
+        <f>+K22*J22</f>
+        <v>0.5914744463504138</v>
+      </c>
+      <c r="M22" s="68">
+        <f>+L22/SUM(L22:L23)</f>
+        <v>0.59274457381575263</v>
+      </c>
+      <c r="N22" s="68">
+        <f>+$H$3*50*M22</f>
+        <v>29.63722869078763</v>
+      </c>
+      <c r="O22" s="71">
+        <f>+O19+N22</f>
+        <v>170.27440175687207</v>
+      </c>
+      <c r="P22" s="49"/>
+      <c r="Q22" s="49"/>
+      <c r="R22" s="49"/>
+      <c r="S22" s="49"/>
+      <c r="T22" s="49"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A23" s="49"/>
+      <c r="B23" s="72">
+        <v>300</v>
+      </c>
+      <c r="C23" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="56"/>
+      <c r="E23" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="56">
+        <v>3E+19</v>
+      </c>
+      <c r="G23" s="56">
+        <v>7E+19</v>
+      </c>
+      <c r="H23" s="74">
+        <f>+F23/SUM(F22:F23)</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="I23" s="74">
+        <f>+G23/SUM(G22:G23)</f>
+        <v>0.35897435897435898</v>
+      </c>
+      <c r="J23" s="74">
+        <f>+H23^$I$3</f>
+        <v>0.55260683251119402</v>
+      </c>
+      <c r="K23" s="74">
+        <f>+I23^$J$3</f>
+        <v>0.73539221595033788</v>
+      </c>
+      <c r="L23" s="74">
+        <f>+K23*J23</f>
+        <v>0.40638276310970417</v>
+      </c>
+      <c r="M23" s="74">
+        <f>+L23/SUM(L22:L23)</f>
+        <v>0.40725542618424743</v>
+      </c>
+      <c r="N23" s="74">
+        <f>+$H$3*50*M23</f>
+        <v>20.36277130921237</v>
+      </c>
+      <c r="O23" s="75">
+        <f>+O20+N23</f>
+        <v>129.72559824312793</v>
+      </c>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="49"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="49"/>
+      <c r="T23" s="49"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A24" s="49"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="49"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="49"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="49"/>
+      <c r="T24" s="49"/>
+    </row>
+    <row r="25" spans="1:20" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A25" s="49"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="77"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="49"/>
+      <c r="P25" s="49"/>
+      <c r="Q25" s="49"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="49"/>
+      <c r="T25" s="49"/>
+    </row>
+    <row r="26" spans="1:20" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="78">
+        <f>+SUM(N8,N11,N14,N16,N19,N22)</f>
+        <v>170.27440175687207</v>
+      </c>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="81"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="49"/>
+      <c r="P26" s="49"/>
+      <c r="Q26" s="49"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="49"/>
+      <c r="T26" s="49"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A27" s="49"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="79">
+        <f>+SUM(N9,N12,N15,N17,N20,N23)</f>
+        <v>129.72559824312793</v>
+      </c>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="50">
+        <v>0.999</v>
+      </c>
+      <c r="L27" s="82">
+        <f>+K27*1000000000000000000</f>
+        <v>9.99E+17</v>
+      </c>
+      <c r="M27" s="49"/>
+      <c r="N27" s="51"/>
+      <c r="O27" s="49"/>
+      <c r="P27" s="49"/>
+      <c r="Q27" s="49"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="49"/>
+      <c r="T27" s="49"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A28" s="49"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="80">
+        <f>+SUM(F26:F27)</f>
+        <v>300</v>
+      </c>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="50">
+        <f>+K27^(0.3*60)</f>
+        <v>0.98215218705145069</v>
+      </c>
+      <c r="L28" s="49">
+        <f>60*0.3</f>
+        <v>18</v>
+      </c>
+      <c r="M28" s="49"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="49"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A29" s="49"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="51"/>
+      <c r="O29" s="49"/>
+      <c r="P29" s="49"/>
+      <c r="Q29" s="49"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="49"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A30" s="49"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49">
+        <f>2^256-1</f>
+        <v>1.157920892373162E+77</v>
+      </c>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="49"/>
+      <c r="P30" s="49"/>
+      <c r="Q30" s="49"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="49"/>
+      <c r="T30" s="49"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A31" s="49"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49">
+        <f>2^255-1</f>
+        <v>5.7896044618658098E+76</v>
+      </c>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="51"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
+      <c r="T31" s="49"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="A32" s="49"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="50"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="51"/>
+      <c r="O32" s="49"/>
+      <c r="P32" s="49"/>
+      <c r="Q32" s="49"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="49"/>
+      <c r="T32" s="49"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: New reward formula implemented and tested
</commit_message>
<xml_diff>
--- a/20210921 - Staking Rewards.xlsx
+++ b/20210921 - Staking Rewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Documents\16slimchance16\token\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FA64621-B9FE-440B-B8E4-F569C36FAF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA7F215-3C6A-4C38-AF48-131CC86EDF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="-90" windowWidth="16490" windowHeight="10980" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,6 @@
     <sheet name="KWENTA - Final" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="59">
   <si>
     <t>N stake 20</t>
   </si>
@@ -196,6 +195,27 @@
   </si>
   <si>
     <t>decayedFees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">staking % </t>
+  </si>
+  <si>
+    <t xml:space="preserve">trading % </t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>1-alpha</t>
+  </si>
+  <si>
+    <t>staking Reward</t>
+  </si>
+  <si>
+    <t>rewardScore</t>
+  </si>
+  <si>
+    <t>trading Rewards</t>
   </si>
 </sst>
 </file>
@@ -398,7 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -484,6 +504,8 @@
     <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="173" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4286,32 +4308,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272DD5C9-D190-4388-8820-6AF1434A50B5}">
-  <dimension ref="A1:T32"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.58984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.86328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.31640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.76953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.04296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.76953125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11.6796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.40625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.2265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.2265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A1" s="49"/>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -4324,16 +4345,15 @@
       <c r="J1" s="49"/>
       <c r="K1" s="50"/>
       <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="49"/>
       <c r="O1" s="49"/>
       <c r="P1" s="49"/>
       <c r="Q1" s="49"/>
       <c r="R1" s="49"/>
       <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-    </row>
-    <row r="2" spans="1:20" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    </row>
+    <row r="2" spans="1:19" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A2" s="49"/>
       <c r="B2" s="52" t="s">
         <v>12</v>
@@ -4353,23 +4373,26 @@
         <v>2</v>
       </c>
       <c r="I2" s="52" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J2" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="50"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="51"/>
+        <v>53</v>
+      </c>
+      <c r="K2" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="51"/>
+      <c r="N2" s="49"/>
       <c r="O2" s="49"/>
       <c r="P2" s="49"/>
       <c r="Q2" s="49"/>
       <c r="R2" s="49"/>
       <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-    </row>
-    <row r="3" spans="1:20" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+    </row>
+    <row r="3" spans="1:19" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
       <c r="A3" s="49"/>
       <c r="B3" s="53" t="s">
         <v>15</v>
@@ -4388,24 +4411,27 @@
       <c r="H3" s="49">
         <v>1</v>
       </c>
-      <c r="I3" s="49">
+      <c r="I3" s="85">
+        <v>0.8</v>
+      </c>
+      <c r="J3" s="85">
+        <v>0.2</v>
+      </c>
+      <c r="K3" s="49">
         <v>0.7</v>
       </c>
-      <c r="J3" s="49">
+      <c r="L3" s="49">
         <v>0.3</v>
       </c>
-      <c r="K3" s="50"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="49"/>
       <c r="O3" s="49"/>
       <c r="P3" s="49"/>
       <c r="Q3" s="49"/>
       <c r="R3" s="49"/>
       <c r="S3" s="49"/>
-      <c r="T3" s="49"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A4" s="49"/>
       <c r="B4" s="53" t="s">
         <v>16</v>
@@ -4422,16 +4448,15 @@
       <c r="J4" s="49"/>
       <c r="K4" s="50"/>
       <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="50"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="49"/>
       <c r="P4" s="49"/>
       <c r="Q4" s="49"/>
       <c r="R4" s="49"/>
       <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A5" s="49"/>
       <c r="B5" s="55"/>
       <c r="C5" s="56"/>
@@ -4444,16 +4469,15 @@
       <c r="J5" s="56"/>
       <c r="K5" s="57"/>
       <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
+      <c r="M5" s="58"/>
       <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
+      <c r="O5" s="49"/>
       <c r="P5" s="49"/>
       <c r="Q5" s="49"/>
       <c r="R5" s="49"/>
       <c r="S5" s="49"/>
-      <c r="T5" s="49"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A6" s="49"/>
       <c r="B6" s="49"/>
       <c r="C6" s="49"/>
@@ -4466,16 +4490,15 @@
       <c r="J6" s="49"/>
       <c r="K6" s="50"/>
       <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="49"/>
       <c r="O6" s="49"/>
       <c r="P6" s="49"/>
       <c r="Q6" s="49"/>
       <c r="R6" s="49"/>
       <c r="S6" s="49"/>
-      <c r="T6" s="49"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A7" s="49"/>
       <c r="B7" s="59" t="s">
         <v>39</v>
@@ -4497,33 +4520,28 @@
         <v>42</v>
       </c>
       <c r="I7" s="60" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="J7" s="60" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="K7" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="L7" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="M7" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="N7" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="60"/>
+      <c r="M7" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="63" t="s">
+      <c r="N7" s="63" t="s">
         <v>40</v>
       </c>
+      <c r="O7" s="49"/>
       <c r="P7" s="49"/>
       <c r="Q7" s="49"/>
       <c r="R7" s="49"/>
       <c r="S7" s="49"/>
-      <c r="T7" s="49"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A8" s="49"/>
       <c r="B8" s="64">
         <v>0</v>
@@ -4546,46 +4564,39 @@
         <v>0.5</v>
       </c>
       <c r="I8" s="68">
-        <f>+G8/SUM(G8:G9)</f>
-        <v>0.33333333333333331</v>
+        <f>+$I$3*$H$3*H8*60</f>
+        <v>24</v>
       </c>
       <c r="J8" s="68">
-        <f>+H8^$I$3</f>
-        <v>0.61557220667245816</v>
+        <f>+((G8/1000000000000000000)^$K$3)*((F8/1000000000000000000)^$L$3)</f>
+        <v>18.991444823309347</v>
       </c>
       <c r="K8" s="68">
-        <f>+I8^$J$3</f>
-        <v>0.71922309332486434</v>
-      </c>
-      <c r="L8" s="68">
-        <f>+K8*J8</f>
-        <v>0.44273374664777804</v>
-      </c>
-      <c r="M8" s="69">
-        <f>+L8/SUM(L8:L9)</f>
-        <v>0.44820048133989088</v>
-      </c>
-      <c r="N8" s="68">
-        <f>+$H$3*60*M8</f>
-        <v>26.892028880393454</v>
-      </c>
-      <c r="O8" s="84">
-        <f>+N8</f>
-        <v>26.892028880393454</v>
-      </c>
+        <f>+$J$3*$H$3*J8/SUM(J8:J9)*60</f>
+        <v>4.5722911359585643</v>
+      </c>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68">
+        <f>+K8+I8</f>
+        <v>28.572291135958565</v>
+      </c>
+      <c r="N8" s="84">
+        <f>+M8</f>
+        <v>28.572291135958565</v>
+      </c>
+      <c r="O8" s="49"/>
       <c r="P8" s="49"/>
-      <c r="Q8" s="49"/>
+      <c r="Q8" s="49">
+        <f>10^0.7</f>
+        <v>5.0118723362727229</v>
+      </c>
       <c r="R8" s="49">
         <f>10^0.7</f>
         <v>5.0118723362727229</v>
       </c>
-      <c r="S8" s="49">
-        <f>10^0.7</f>
-        <v>5.0118723362727229</v>
-      </c>
-      <c r="T8" s="49"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="S8" s="49"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A9" s="49"/>
       <c r="B9" s="64"/>
       <c r="C9" s="65"/>
@@ -4604,46 +4615,39 @@
         <v>0.5</v>
       </c>
       <c r="I9" s="68">
-        <f>+G9/SUM(G8:G9)</f>
-        <v>0.66666666666666663</v>
+        <f>+$I$3*$H$3*H9*60</f>
+        <v>24</v>
       </c>
       <c r="J9" s="68">
-        <f>+H9^$I$3</f>
-        <v>0.61557220667245816</v>
+        <f>+((G9/1000000000000000000)^$K$3)*((F9/1000000000000000000)^$L$3)</f>
+        <v>30.851693136000481</v>
       </c>
       <c r="K9" s="68">
-        <f>+I9^$J$3</f>
-        <v>0.88546749329555607</v>
-      </c>
-      <c r="L9" s="68">
-        <f>+K9*J9</f>
-        <v>0.54506917878467553</v>
-      </c>
-      <c r="M9" s="69">
-        <f>+L9/SUM(L8:L9)</f>
-        <v>0.55179951866010912</v>
-      </c>
-      <c r="N9" s="68">
-        <f>+$H$3*60*M9</f>
-        <v>33.107971119606546</v>
-      </c>
-      <c r="O9" s="84">
-        <f>+N9</f>
-        <v>33.107971119606546</v>
-      </c>
+        <f>+$J$3*$H$3*J9/SUM(J8:J9)*60</f>
+        <v>7.4277088640414357</v>
+      </c>
+      <c r="L9" s="68"/>
+      <c r="M9" s="68">
+        <f>+K9+I9</f>
+        <v>31.427708864041435</v>
+      </c>
+      <c r="N9" s="84">
+        <f>+M9</f>
+        <v>31.427708864041435</v>
+      </c>
+      <c r="O9" s="49"/>
       <c r="P9" s="49"/>
-      <c r="Q9" s="49"/>
-      <c r="R9" s="49">
+      <c r="Q9" s="49">
         <f>25^0.3</f>
         <v>2.626527804403767</v>
       </c>
-      <c r="S9" s="49">
+      <c r="R9" s="49">
         <f>50^0.3</f>
         <v>3.2336350328867871</v>
       </c>
-      <c r="T9" s="49"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="S9" s="49"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A10" s="49"/>
       <c r="B10" s="64">
         <v>60</v>
@@ -4661,21 +4665,20 @@
       <c r="K10" s="68"/>
       <c r="L10" s="68"/>
       <c r="M10" s="68"/>
-      <c r="N10" s="68"/>
-      <c r="O10" s="70"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="49"/>
       <c r="P10" s="49"/>
-      <c r="Q10" s="49"/>
+      <c r="Q10" s="49">
+        <f>+Q9*Q8</f>
+        <v>13.163822043342373</v>
+      </c>
       <c r="R10" s="49">
         <f>+R9*R8</f>
-        <v>13.163822043342373</v>
-      </c>
-      <c r="S10" s="49">
-        <f>+S9*S8</f>
         <v>16.206565966927624</v>
       </c>
-      <c r="T10" s="49"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.75">
+      <c r="S10" s="49"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A11" s="49"/>
       <c r="B11" s="64"/>
       <c r="C11" s="65"/>
@@ -4694,40 +4697,33 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="I11" s="68">
-        <f>+G11/SUM(G11:G12)</f>
-        <v>0.33333333333333331</v>
+        <f>+$I$3*$H$3*H11*60</f>
+        <v>40.000000000000007</v>
       </c>
       <c r="J11" s="68">
-        <f>+H11^$I$3</f>
-        <v>0.88018330703271519</v>
+        <f>+((G11/1000000000000000000)^$K$3)*((F11/1000000000000000000)^$L$3)</f>
+        <v>30.778610333622904</v>
       </c>
       <c r="K11" s="68">
-        <f>+I11^$J$3</f>
-        <v>0.71922309332486434</v>
-      </c>
-      <c r="L11" s="68">
-        <f>+K11*J11</f>
-        <v>0.63304816077697823</v>
-      </c>
+        <f>+$J$3*$H$3*J11/SUM(J11:J12)*60</f>
+        <v>5.9928850453497837</v>
+      </c>
+      <c r="L11" s="68"/>
       <c r="M11" s="68">
-        <f>+L11/SUM(L11:L12)</f>
-        <v>0.71476947895159004</v>
-      </c>
-      <c r="N11" s="68">
-        <f>+$H$3*60*M11</f>
-        <v>42.886168737095403</v>
-      </c>
-      <c r="O11" s="71">
-        <f>+N11+N8</f>
-        <v>69.778197617488857</v>
-      </c>
+        <f>+K11+I11</f>
+        <v>45.992885045349794</v>
+      </c>
+      <c r="N11" s="84">
+        <f>+M11+N8</f>
+        <v>74.56517618130836</v>
+      </c>
+      <c r="O11" s="49"/>
       <c r="P11" s="49"/>
       <c r="Q11" s="49"/>
       <c r="R11" s="49"/>
       <c r="S11" s="49"/>
-      <c r="T11" s="49"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A12" s="49"/>
       <c r="B12" s="64"/>
       <c r="C12" s="65"/>
@@ -4746,43 +4742,36 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="I12" s="68">
-        <f>+G12/SUM(G11:G12)</f>
-        <v>0.66666666666666663</v>
+        <f>+$I$3*$H$3*H12*60</f>
+        <v>8</v>
       </c>
       <c r="J12" s="68">
-        <f>+H12^$I$3</f>
-        <v>0.28529497656828423</v>
+        <f>+((G12/1000000000000000000)^$K$3)*((F12/1000000000000000000)^$L$3)</f>
+        <v>30.851693136000481</v>
       </c>
       <c r="K12" s="68">
-        <f>+I12^$J$3</f>
-        <v>0.88546749329555607</v>
-      </c>
-      <c r="L12" s="68">
-        <f>+K12*J12</f>
-        <v>0.25261942775173307</v>
-      </c>
+        <f>+$J$3*$H$3*J12/SUM(J11:J12)*60</f>
+        <v>6.0071149546502163</v>
+      </c>
+      <c r="L12" s="68"/>
       <c r="M12" s="68">
-        <f>+L12/SUM(L11:L12)</f>
-        <v>0.28523052104840996</v>
-      </c>
-      <c r="N12" s="68">
-        <f>+$H$3*60*M12</f>
-        <v>17.113831262904597</v>
-      </c>
-      <c r="O12" s="71">
-        <f>+N12+N9</f>
-        <v>50.221802382511143</v>
-      </c>
+        <f>+K12+I12</f>
+        <v>14.007114954650216</v>
+      </c>
+      <c r="N12" s="84">
+        <f>+M12+N9</f>
+        <v>45.434823818691655</v>
+      </c>
+      <c r="O12" s="49"/>
       <c r="P12" s="49"/>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="49">
-        <f>+R10+S10</f>
+      <c r="Q12" s="49">
+        <f>+Q10+R10</f>
         <v>29.370388010269998</v>
       </c>
+      <c r="R12" s="49"/>
       <c r="S12" s="49"/>
-      <c r="T12" s="49"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A13" s="49"/>
       <c r="B13" s="64">
         <v>120</v>
@@ -4800,18 +4789,17 @@
       <c r="K13" s="68"/>
       <c r="L13" s="68"/>
       <c r="M13" s="68"/>
-      <c r="N13" s="68"/>
-      <c r="O13" s="70"/>
+      <c r="N13" s="70"/>
+      <c r="O13" s="49"/>
       <c r="P13" s="49"/>
-      <c r="Q13" s="49"/>
-      <c r="R13" s="49">
-        <f>1/R12/60</f>
+      <c r="Q13" s="49">
+        <f>1/Q12/60</f>
         <v>5.6746498074314853E-4</v>
       </c>
+      <c r="R13" s="49"/>
       <c r="S13" s="49"/>
-      <c r="T13" s="49"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A14" s="49"/>
       <c r="B14" s="64"/>
       <c r="C14" s="65"/>
@@ -4830,40 +4818,33 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="I14" s="68">
-        <f>+G14/SUM(G14:G15)</f>
-        <v>0.26315789473684209</v>
+        <f>+$I$3*$H$3*H14*30</f>
+        <v>20.000000000000004</v>
       </c>
       <c r="J14" s="68">
-        <f>+H14^$I$3</f>
-        <v>0.88018330703271519</v>
+        <f>+((G14/1000000000000000000)^$K$3)*((F14/1000000000000000000)^$L$3)</f>
+        <v>30.778610333622904</v>
       </c>
       <c r="K14" s="68">
-        <f>+I14^$J$3</f>
-        <v>0.66998475538030788</v>
-      </c>
-      <c r="L14" s="68">
-        <f>+K14*J14</f>
-        <v>0.58970939765214414</v>
-      </c>
+        <f>+$J$3*$H$3*J14/SUM(J14:J15)*30</f>
+        <v>2.6448202838006507</v>
+      </c>
+      <c r="L14" s="68"/>
       <c r="M14" s="68">
-        <f>+L14/SUM(L14:L15)</f>
-        <v>0.69375229677182093</v>
-      </c>
-      <c r="N14" s="68">
-        <f>+$H$3*30*M14</f>
-        <v>20.812568903154627</v>
-      </c>
-      <c r="O14" s="71">
-        <f>+O11+N14</f>
-        <v>90.590766520643484</v>
-      </c>
+        <f>+K14+I14</f>
+        <v>22.644820283800655</v>
+      </c>
+      <c r="N14" s="84">
+        <f>+M14+N11</f>
+        <v>97.209996465109015</v>
+      </c>
+      <c r="O14" s="49"/>
       <c r="P14" s="49"/>
       <c r="Q14" s="49"/>
       <c r="R14" s="49"/>
       <c r="S14" s="49"/>
-      <c r="T14" s="49"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A15" s="49"/>
       <c r="B15" s="64"/>
       <c r="C15" s="65"/>
@@ -4882,40 +4863,33 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="I15" s="68">
-        <f>+G15/SUM(G14:G15)</f>
-        <v>0.73684210526315785</v>
+        <f>+$I$3*$H$3*H15*30</f>
+        <v>4</v>
       </c>
       <c r="J15" s="68">
-        <f>+H15^$I$3</f>
-        <v>0.28529497656828423</v>
+        <f>+((G15/1000000000000000000)^$K$3)*((F15/1000000000000000000)^$L$3)</f>
+        <v>39.04528777122723</v>
       </c>
       <c r="K15" s="68">
-        <f>+I15^$J$3</f>
-        <v>0.91245683854817927</v>
-      </c>
-      <c r="L15" s="68">
-        <f>+K15*J15</f>
-        <v>0.2603193523731735</v>
-      </c>
+        <f>+$J$3*$H$3*J15/SUM(J14:J15)*30</f>
+        <v>3.3551797161993497</v>
+      </c>
+      <c r="L15" s="68"/>
       <c r="M15" s="68">
-        <f>+L15/SUM(L14:L15)</f>
-        <v>0.30624770322817907</v>
-      </c>
-      <c r="N15" s="68">
-        <f>+$H$3*30*M15</f>
-        <v>9.1874310968453727</v>
-      </c>
-      <c r="O15" s="71">
-        <f>+O12+N15</f>
-        <v>59.409233479356516</v>
-      </c>
+        <f>+K15+I15</f>
+        <v>7.3551797161993502</v>
+      </c>
+      <c r="N15" s="84">
+        <f>+M15+N12</f>
+        <v>52.790003534891007</v>
+      </c>
+      <c r="O15" s="49"/>
       <c r="P15" s="49"/>
       <c r="Q15" s="49"/>
       <c r="R15" s="49"/>
       <c r="S15" s="49"/>
-      <c r="T15" s="49"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A16" s="49"/>
       <c r="B16" s="64">
         <v>150</v>
@@ -4938,40 +4912,33 @@
         <v>0.625</v>
       </c>
       <c r="I16" s="68">
-        <f>+G16/SUM(G16:G17)</f>
-        <v>0.26315789473684209</v>
+        <f>+$I$3*$H$3*H16*70</f>
+        <v>35</v>
       </c>
       <c r="J16" s="68">
-        <f>+H16^$I$3</f>
-        <v>0.71964118851645298</v>
+        <f>+((G16/1000000000000000000)^$K$3)*((F16/1000000000000000000)^$L$3)</f>
+        <v>30.778610333622904</v>
       </c>
       <c r="K16" s="68">
-        <f>+I16^$J$3</f>
-        <v>0.66998475538030788</v>
-      </c>
-      <c r="L16" s="68">
-        <f>+K16*J16</f>
-        <v>0.48214862564978977</v>
-      </c>
+        <f>+$J$3*$H$3*J16/SUM(J16:J17)*70</f>
+        <v>5.0654399784999322</v>
+      </c>
+      <c r="L16" s="68"/>
       <c r="M16" s="68">
-        <f>+L16/SUM(L16:L17)</f>
-        <v>0.51217062333254171</v>
-      </c>
-      <c r="N16" s="68">
-        <f>+$H$3*70*M16</f>
-        <v>35.851943633277919</v>
-      </c>
-      <c r="O16" s="71">
-        <f>+O14+N16</f>
-        <v>126.44271015392141</v>
-      </c>
+        <f>+K16+I16</f>
+        <v>40.065439978499931</v>
+      </c>
+      <c r="N16" s="84">
+        <f>+M16+N14</f>
+        <v>137.27543644360895</v>
+      </c>
+      <c r="O16" s="49"/>
       <c r="P16" s="49"/>
       <c r="Q16" s="49"/>
       <c r="R16" s="49"/>
       <c r="S16" s="49"/>
-      <c r="T16" s="49"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A17" s="49"/>
       <c r="B17" s="64"/>
       <c r="C17" s="65"/>
@@ -4990,43 +4957,36 @@
         <v>0.375</v>
       </c>
       <c r="I17" s="68">
-        <f>+G17/SUM(G16:G17)</f>
-        <v>0.73684210526315785</v>
+        <f>+$I$3*$H$3*H17*70</f>
+        <v>21.000000000000004</v>
       </c>
       <c r="J17" s="68">
-        <f>+H17^$I$3</f>
-        <v>0.50329415576044101</v>
+        <f>+((G17/1000000000000000000)^$K$3)*((F17/1000000000000000000)^$L$3)</f>
+        <v>54.288145268982554</v>
       </c>
       <c r="K17" s="68">
-        <f>+I17^$J$3</f>
-        <v>0.91245683854817927</v>
-      </c>
-      <c r="L17" s="68">
-        <f>+K17*J17</f>
-        <v>0.45923419422494693</v>
-      </c>
+        <f>+$J$3*$H$3*J17/SUM(J16:J17)*70</f>
+        <v>8.9345600215000704</v>
+      </c>
+      <c r="L17" s="68"/>
       <c r="M17" s="68">
-        <f>+L17/SUM(L16:L17)</f>
-        <v>0.48782937666745824</v>
-      </c>
-      <c r="N17" s="68">
-        <f>+$H$3*70*M17</f>
-        <v>34.148056366722074</v>
-      </c>
-      <c r="O17" s="71">
-        <f>+O15+N17</f>
-        <v>93.557289846078589</v>
-      </c>
+        <f>+K17+I17</f>
+        <v>29.934560021500076</v>
+      </c>
+      <c r="N17" s="84">
+        <f>+M17+N15</f>
+        <v>82.724563556391075</v>
+      </c>
+      <c r="O17" s="49"/>
       <c r="P17" s="49"/>
-      <c r="Q17" s="49"/>
-      <c r="R17" s="49">
+      <c r="Q17" s="49">
         <f>60*1000000000000000000</f>
         <v>6E+19</v>
       </c>
+      <c r="R17" s="49"/>
       <c r="S17" s="49"/>
-      <c r="T17" s="49"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A18" s="49"/>
       <c r="B18" s="64">
         <v>220</v>
@@ -5044,18 +5004,17 @@
       <c r="K18" s="68"/>
       <c r="L18" s="68"/>
       <c r="M18" s="68"/>
-      <c r="N18" s="68"/>
-      <c r="O18" s="71"/>
+      <c r="N18" s="71"/>
+      <c r="O18" s="49"/>
       <c r="P18" s="49"/>
-      <c r="Q18" s="49"/>
-      <c r="R18" s="49">
-        <f>+R17*10000</f>
+      <c r="Q18" s="49">
+        <f>+Q17*10000</f>
         <v>6.0000000000000002E+23</v>
       </c>
+      <c r="R18" s="49"/>
       <c r="S18" s="49"/>
-      <c r="T18" s="49"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A19" s="49"/>
       <c r="B19" s="64"/>
       <c r="C19" s="65"/>
@@ -5074,43 +5033,36 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="I19" s="68">
-        <f>+G19/SUM(G19:G20)</f>
-        <v>0.26315789473684209</v>
+        <f>+$I$3*$H$3*H19*30</f>
+        <v>13.714285714285714</v>
       </c>
       <c r="J19" s="68">
-        <f>+H19^$I$3</f>
-        <v>0.67588586797162753</v>
+        <f>+((G19/1000000000000000000)^$K$3)*((F19/1000000000000000000)^$L$3)</f>
+        <v>28.785647540658108</v>
       </c>
       <c r="K19" s="68">
-        <f>+I19^$J$3</f>
-        <v>0.66998475538030788</v>
-      </c>
-      <c r="L19" s="68">
-        <f>+K19*J19</f>
-        <v>0.45283322791797792</v>
-      </c>
+        <f>+$J$3*$H$3*J19/SUM(J19:J20)*30</f>
+        <v>2.0790417700045754</v>
+      </c>
+      <c r="L19" s="68"/>
       <c r="M19" s="68">
-        <f>+L19/SUM(L19:L20)</f>
-        <v>0.4731487637387678</v>
-      </c>
-      <c r="N19" s="68">
-        <f>+$H$3*30*M19</f>
-        <v>14.194462912163035</v>
-      </c>
-      <c r="O19" s="71">
-        <f>+O16+N19</f>
-        <v>140.63717306608444</v>
-      </c>
+        <f>+K19+I19</f>
+        <v>15.793327484290289</v>
+      </c>
+      <c r="N19" s="84">
+        <f>+M19+N16</f>
+        <v>153.06876392789925</v>
+      </c>
+      <c r="O19" s="49"/>
       <c r="P19" s="49"/>
-      <c r="Q19" s="49"/>
-      <c r="R19" s="49">
-        <f>+R18*1E+50</f>
+      <c r="Q19" s="49">
+        <f>+Q18*1E+50</f>
         <v>6.0000000000000002E+73</v>
       </c>
+      <c r="R19" s="49"/>
       <c r="S19" s="49"/>
-      <c r="T19" s="49"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A20" s="49"/>
       <c r="B20" s="64"/>
       <c r="C20" s="65"/>
@@ -5129,46 +5081,39 @@
         <v>0.42857142857142855</v>
       </c>
       <c r="I20" s="68">
-        <f>+G20/SUM(G19:G20)</f>
-        <v>0.73684210526315785</v>
+        <f>+$I$3*$H$3*H20*30</f>
+        <v>10.285714285714286</v>
       </c>
       <c r="J20" s="68">
-        <f>+H20^$I$3</f>
-        <v>0.55260683251119402</v>
+        <f>+((G20/1000000000000000000)^$K$3)*((F20/1000000000000000000)^$L$3)</f>
+        <v>54.288145268982554</v>
       </c>
       <c r="K20" s="68">
-        <f>+I20^$J$3</f>
-        <v>0.91245683854817927</v>
-      </c>
-      <c r="L20" s="68">
-        <f>+K20*J20</f>
-        <v>0.50422988335328733</v>
-      </c>
+        <f>+$J$3*$H$3*J20/SUM(J19:J20)*30</f>
+        <v>3.9209582299954251</v>
+      </c>
+      <c r="L20" s="68"/>
       <c r="M20" s="68">
-        <f>+L20/SUM(L19:L20)</f>
-        <v>0.5268512362612322</v>
-      </c>
-      <c r="N20" s="68">
-        <f>+$H$3*30*M20</f>
-        <v>15.805537087836965</v>
-      </c>
-      <c r="O20" s="71">
-        <f>+O17+N20</f>
-        <v>109.36282693391556</v>
-      </c>
-      <c r="P20" s="49"/>
-      <c r="Q20" s="50">
+        <f>+K20+I20</f>
+        <v>14.206672515709712</v>
+      </c>
+      <c r="N20" s="84">
+        <f>+M20+N17</f>
+        <v>96.931236072100788</v>
+      </c>
+      <c r="O20" s="49"/>
+      <c r="P20" s="50">
         <f>+K27</f>
         <v>0.999</v>
       </c>
-      <c r="R20" s="49">
-        <f>+R19/2.93703880102699E+37</f>
+      <c r="Q20" s="49">
+        <f>+Q19/2.93703880102699E+37</f>
         <v>2.0428739306753418E+36</v>
       </c>
+      <c r="R20" s="49"/>
       <c r="S20" s="49"/>
-      <c r="T20" s="49"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A21" s="49"/>
       <c r="B21" s="64">
         <v>250</v>
@@ -5186,21 +5131,20 @@
       <c r="K21" s="68"/>
       <c r="L21" s="68"/>
       <c r="M21" s="68"/>
-      <c r="N21" s="68"/>
-      <c r="O21" s="71"/>
-      <c r="P21" s="49"/>
-      <c r="Q21" s="49">
-        <f>+Q20^(0.3*60)</f>
+      <c r="N21" s="71"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="49">
+        <f>+P20^(0.3*60)</f>
         <v>0.98215218705145069</v>
       </c>
-      <c r="R21" s="83">
-        <f>+R20/(Q21*1000000000000000000)</f>
+      <c r="Q21" s="83">
+        <f>+Q20/(P21*1000000000000000000)</f>
         <v>2.0799973340265288E+18</v>
       </c>
+      <c r="R21" s="49"/>
       <c r="S21" s="49"/>
-      <c r="T21" s="49"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A22" s="49"/>
       <c r="B22" s="64"/>
       <c r="C22" s="65"/>
@@ -5219,40 +5163,33 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="I22" s="68">
-        <f>+G22/SUM(G22:G23)</f>
-        <v>0.64102564102564108</v>
+        <f>+$I$3*$H$3*H22*50</f>
+        <v>22.857142857142858</v>
       </c>
       <c r="J22" s="68">
-        <f>+H22^$I$3</f>
-        <v>0.67588586797162753</v>
+        <f>+((G22/1000000000000000000)^$K$3)*((F22/1000000000000000000)^$L$3)</f>
+        <v>88.808596464545104</v>
       </c>
       <c r="K22" s="68">
-        <f>+I22^$J$3</f>
-        <v>0.87510994737242054</v>
-      </c>
-      <c r="L22" s="68">
-        <f>+K22*J22</f>
-        <v>0.5914744463504138</v>
-      </c>
+        <f>+$J$3*$H$3*J22/SUM(J22:J23)*50</f>
+        <v>6.2061927748098533</v>
+      </c>
+      <c r="L22" s="68"/>
       <c r="M22" s="68">
-        <f>+L22/SUM(L22:L23)</f>
-        <v>0.59274457381575263</v>
-      </c>
-      <c r="N22" s="68">
-        <f>+$H$3*50*M22</f>
-        <v>29.63722869078763</v>
-      </c>
-      <c r="O22" s="71">
-        <f>+O19+N22</f>
-        <v>170.27440175687207</v>
-      </c>
+        <f>+K22+I22</f>
+        <v>29.063335631952711</v>
+      </c>
+      <c r="N22" s="84">
+        <f>+M22+N19</f>
+        <v>182.13209955985195</v>
+      </c>
+      <c r="O22" s="49"/>
       <c r="P22" s="49"/>
       <c r="Q22" s="49"/>
       <c r="R22" s="49"/>
       <c r="S22" s="49"/>
-      <c r="T22" s="49"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A23" s="49"/>
       <c r="B23" s="72">
         <v>300</v>
@@ -5275,40 +5212,33 @@
         <v>0.42857142857142855</v>
       </c>
       <c r="I23" s="74">
-        <f>+G23/SUM(G22:G23)</f>
-        <v>0.35897435897435898</v>
+        <f>+$I$3*$H$3*H23*50</f>
+        <v>17.142857142857142</v>
       </c>
       <c r="J23" s="74">
-        <f>+H23^$I$3</f>
-        <v>0.55260683251119402</v>
+        <f>+((G23/1000000000000000000)^$K$3)*((F23/1000000000000000000)^$L$3)</f>
+        <v>54.288145268982554</v>
       </c>
       <c r="K23" s="74">
-        <f>+I23^$J$3</f>
-        <v>0.73539221595033788</v>
-      </c>
-      <c r="L23" s="74">
-        <f>+K23*J23</f>
-        <v>0.40638276310970417</v>
-      </c>
+        <f>+$J$3*$H$3*J23/SUM(J22:J23)*50</f>
+        <v>3.7938072251901462</v>
+      </c>
+      <c r="L23" s="74"/>
       <c r="M23" s="74">
-        <f>+L23/SUM(L22:L23)</f>
-        <v>0.40725542618424743</v>
-      </c>
-      <c r="N23" s="74">
-        <f>+$H$3*50*M23</f>
-        <v>20.36277130921237</v>
-      </c>
-      <c r="O23" s="75">
-        <f>+O20+N23</f>
-        <v>129.72559824312793</v>
-      </c>
+        <f>+K23+I23</f>
+        <v>20.936664368047289</v>
+      </c>
+      <c r="N23" s="86">
+        <f>+M23+N20</f>
+        <v>117.86790044014808</v>
+      </c>
+      <c r="O23" s="49"/>
       <c r="P23" s="49"/>
       <c r="Q23" s="49"/>
       <c r="R23" s="49"/>
       <c r="S23" s="49"/>
-      <c r="T23" s="49"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A24" s="49"/>
       <c r="B24" s="49"/>
       <c r="C24" s="49"/>
@@ -5321,16 +5251,15 @@
       <c r="J24" s="49"/>
       <c r="K24" s="50"/>
       <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="51"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="49"/>
       <c r="O24" s="49"/>
       <c r="P24" s="49"/>
       <c r="Q24" s="49"/>
       <c r="R24" s="49"/>
       <c r="S24" s="49"/>
-      <c r="T24" s="49"/>
-    </row>
-    <row r="25" spans="1:20" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    </row>
+    <row r="25" spans="1:19" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A25" s="49"/>
       <c r="B25" s="49"/>
       <c r="C25" s="49"/>
@@ -5345,16 +5274,15 @@
       <c r="J25" s="49"/>
       <c r="K25" s="50"/>
       <c r="L25" s="49"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="51"/>
+      <c r="M25" s="51"/>
+      <c r="N25" s="49"/>
       <c r="O25" s="49"/>
       <c r="P25" s="49"/>
       <c r="Q25" s="49"/>
       <c r="R25" s="49"/>
       <c r="S25" s="49"/>
-      <c r="T25" s="49"/>
-    </row>
-    <row r="26" spans="1:20" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+    </row>
+    <row r="26" spans="1:19" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
       <c r="A26" s="49"/>
       <c r="B26" s="49"/>
       <c r="C26" s="49"/>
@@ -5363,8 +5291,8 @@
         <v>24</v>
       </c>
       <c r="F26" s="78">
-        <f>+SUM(N8,N11,N14,N16,N19,N22)</f>
-        <v>170.27440175687207</v>
+        <f>+SUM(M8,M11,M14,M16,M19,M22)</f>
+        <v>182.13209955985195</v>
       </c>
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
@@ -5372,16 +5300,15 @@
       <c r="J26" s="49"/>
       <c r="K26" s="50"/>
       <c r="L26" s="81"/>
-      <c r="M26" s="49"/>
-      <c r="N26" s="51"/>
+      <c r="M26" s="51"/>
+      <c r="N26" s="49"/>
       <c r="O26" s="49"/>
       <c r="P26" s="49"/>
       <c r="Q26" s="49"/>
       <c r="R26" s="49"/>
       <c r="S26" s="49"/>
-      <c r="T26" s="49"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A27" s="49"/>
       <c r="B27" s="49"/>
       <c r="C27" s="49"/>
@@ -5390,8 +5317,8 @@
         <v>25</v>
       </c>
       <c r="F27" s="79">
-        <f>+SUM(N9,N12,N15,N17,N20,N23)</f>
-        <v>129.72559824312793</v>
+        <f>+SUM(M9,M12,M15,M17,M20,M23)</f>
+        <v>117.86790044014808</v>
       </c>
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
@@ -5404,16 +5331,15 @@
         <f>+K27*1000000000000000000</f>
         <v>9.99E+17</v>
       </c>
-      <c r="M27" s="49"/>
-      <c r="N27" s="51"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="49"/>
       <c r="O27" s="49"/>
       <c r="P27" s="49"/>
       <c r="Q27" s="49"/>
       <c r="R27" s="49"/>
       <c r="S27" s="49"/>
-      <c r="T27" s="49"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A28" s="49"/>
       <c r="B28" s="49"/>
       <c r="C28" s="49"/>
@@ -5437,16 +5363,15 @@
         <f>60*0.3</f>
         <v>18</v>
       </c>
-      <c r="M28" s="49"/>
-      <c r="N28" s="51"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="49"/>
       <c r="O28" s="49"/>
       <c r="P28" s="49"/>
       <c r="Q28" s="49"/>
       <c r="R28" s="49"/>
       <c r="S28" s="49"/>
-      <c r="T28" s="49"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A29" s="49"/>
       <c r="B29" s="49"/>
       <c r="C29" s="49"/>
@@ -5459,16 +5384,15 @@
       <c r="J29" s="49"/>
       <c r="K29" s="50"/>
       <c r="L29" s="49"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="51"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="49"/>
       <c r="O29" s="49"/>
       <c r="P29" s="49"/>
       <c r="Q29" s="49"/>
       <c r="R29" s="49"/>
       <c r="S29" s="49"/>
-      <c r="T29" s="49"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A30" s="49"/>
       <c r="B30" s="49"/>
       <c r="C30" s="49"/>
@@ -5484,16 +5408,15 @@
       <c r="J30" s="49"/>
       <c r="K30" s="50"/>
       <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="51"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="49"/>
       <c r="O30" s="49"/>
       <c r="P30" s="49"/>
       <c r="Q30" s="49"/>
       <c r="R30" s="49"/>
       <c r="S30" s="49"/>
-      <c r="T30" s="49"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A31" s="49"/>
       <c r="B31" s="49"/>
       <c r="C31" s="49"/>
@@ -5509,16 +5432,15 @@
       <c r="J31" s="49"/>
       <c r="K31" s="50"/>
       <c r="L31" s="49"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="51"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="49"/>
       <c r="O31" s="49"/>
       <c r="P31" s="49"/>
       <c r="Q31" s="49"/>
       <c r="R31" s="49"/>
       <c r="S31" s="49"/>
-      <c r="T31" s="49"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.75">
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A32" s="49"/>
       <c r="B32" s="49"/>
       <c r="C32" s="49"/>
@@ -5531,14 +5453,32 @@
       <c r="J32" s="49"/>
       <c r="K32" s="50"/>
       <c r="L32" s="49"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="51"/>
+      <c r="M32" s="51"/>
+      <c r="N32" s="49"/>
       <c r="O32" s="49"/>
       <c r="P32" s="49"/>
       <c r="Q32" s="49"/>
       <c r="R32" s="49"/>
       <c r="S32" s="49"/>
-      <c r="T32" s="49"/>
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.75">
+      <c r="G39">
+        <v>33</v>
+      </c>
+      <c r="I39">
+        <f>80*G39*10000</f>
+        <v>26400000</v>
+      </c>
+    </row>
+    <row r="40" spans="7:9" x14ac:dyDescent="0.75">
+      <c r="G40">
+        <f>80%*G39</f>
+        <v>26.400000000000002</v>
+      </c>
+      <c r="I40">
+        <f>+I39/10000/100</f>
+        <v>26.4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: changed modifiers to occupy less bytecode
</commit_message>
<xml_diff>
--- a/20210921 - Staking Rewards.xlsx
+++ b/20210921 - Staking Rewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Documents\16slimchance16\token\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA7F215-3C6A-4C38-AF48-131CC86EDF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089AC7A1-7081-42C5-BAFE-4E36110D076D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="-90" windowWidth="16490" windowHeight="10980" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -505,7 +505,7 @@
     <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="173" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4311,7 +4311,7 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -4580,7 +4580,7 @@
         <f>+K8+I8</f>
         <v>28.572291135958565</v>
       </c>
-      <c r="N8" s="84">
+      <c r="N8" s="71">
         <f>+M8</f>
         <v>28.572291135958565</v>
       </c>
@@ -4631,7 +4631,7 @@
         <f>+K9+I9</f>
         <v>31.427708864041435</v>
       </c>
-      <c r="N9" s="84">
+      <c r="N9" s="71">
         <f>+M9</f>
         <v>31.427708864041435</v>
       </c>
@@ -4665,7 +4665,7 @@
       <c r="K10" s="68"/>
       <c r="L10" s="68"/>
       <c r="M10" s="68"/>
-      <c r="N10" s="70"/>
+      <c r="N10" s="71"/>
       <c r="O10" s="49"/>
       <c r="P10" s="49"/>
       <c r="Q10" s="49">
@@ -4713,7 +4713,7 @@
         <f>+K11+I11</f>
         <v>45.992885045349794</v>
       </c>
-      <c r="N11" s="84">
+      <c r="N11" s="71">
         <f>+M11+N8</f>
         <v>74.56517618130836</v>
       </c>
@@ -4758,7 +4758,7 @@
         <f>+K12+I12</f>
         <v>14.007114954650216</v>
       </c>
-      <c r="N12" s="84">
+      <c r="N12" s="71">
         <f>+M12+N9</f>
         <v>45.434823818691655</v>
       </c>
@@ -4789,7 +4789,7 @@
       <c r="K13" s="68"/>
       <c r="L13" s="68"/>
       <c r="M13" s="68"/>
-      <c r="N13" s="70"/>
+      <c r="N13" s="71"/>
       <c r="O13" s="49"/>
       <c r="P13" s="49"/>
       <c r="Q13" s="49">
@@ -4834,7 +4834,7 @@
         <f>+K14+I14</f>
         <v>22.644820283800655</v>
       </c>
-      <c r="N14" s="84">
+      <c r="N14" s="71">
         <f>+M14+N11</f>
         <v>97.209996465109015</v>
       </c>
@@ -4879,7 +4879,7 @@
         <f>+K15+I15</f>
         <v>7.3551797161993502</v>
       </c>
-      <c r="N15" s="84">
+      <c r="N15" s="71">
         <f>+M15+N12</f>
         <v>52.790003534891007</v>
       </c>
@@ -4928,7 +4928,7 @@
         <f>+K16+I16</f>
         <v>40.065439978499931</v>
       </c>
-      <c r="N16" s="84">
+      <c r="N16" s="71">
         <f>+M16+N14</f>
         <v>137.27543644360895</v>
       </c>
@@ -4973,7 +4973,7 @@
         <f>+K17+I17</f>
         <v>29.934560021500076</v>
       </c>
-      <c r="N17" s="84">
+      <c r="N17" s="71">
         <f>+M17+N15</f>
         <v>82.724563556391075</v>
       </c>
@@ -5049,7 +5049,7 @@
         <f>+K19+I19</f>
         <v>15.793327484290289</v>
       </c>
-      <c r="N19" s="84">
+      <c r="N19" s="71">
         <f>+M19+N16</f>
         <v>153.06876392789925</v>
       </c>
@@ -5097,7 +5097,7 @@
         <f>+K20+I20</f>
         <v>14.206672515709712</v>
       </c>
-      <c r="N20" s="84">
+      <c r="N20" s="71">
         <f>+M20+N17</f>
         <v>96.931236072100788</v>
       </c>
@@ -5179,7 +5179,7 @@
         <f>+K22+I22</f>
         <v>29.063335631952711</v>
       </c>
-      <c r="N22" s="84">
+      <c r="N22" s="71">
         <f>+M22+N19</f>
         <v>182.13209955985195</v>
       </c>
@@ -5228,7 +5228,7 @@
         <f>+K23+I23</f>
         <v>20.936664368047289</v>
       </c>
-      <c r="N23" s="86">
+      <c r="N23" s="75">
         <f>+M23+N20</f>
         <v>117.86790044014808</v>
       </c>
@@ -5431,10 +5431,18 @@
       <c r="I31" s="49"/>
       <c r="J31" s="49"/>
       <c r="K31" s="50"/>
-      <c r="L31" s="49"/>
+      <c r="L31" s="49">
+        <v>1.0313746731726601E+20</v>
+      </c>
       <c r="M31" s="51"/>
-      <c r="N31" s="49"/>
-      <c r="O31" s="49"/>
+      <c r="N31" s="49">
+        <f>+L31/1000000000000000000</f>
+        <v>103.137467317266</v>
+      </c>
+      <c r="O31" s="86">
+        <f>+N31-N11</f>
+        <v>28.572291135957641</v>
+      </c>
       <c r="P31" s="49"/>
       <c r="Q31" s="49"/>
       <c r="R31" s="49"/>

</xml_diff>

<commit_message>
fix: included implementation test and Excel file describing a 3-epoch scenario
</commit_message>
<xml_diff>
--- a/20210921 - Staking Rewards.xlsx
+++ b/20210921 - Staking Rewards.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Documents\16slimchance16\token\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089AC7A1-7081-42C5-BAFE-4E36110D076D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3614439B-31E7-4EC0-8DB0-5937F1CDE6EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="-90" windowWidth="16490" windowHeight="10980" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67995" yWindow="-15075" windowWidth="6825" windowHeight="3915" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SNX" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="SNX - Detail" sheetId="4" state="hidden" r:id="rId2"/>
     <sheet name="KWENTA" sheetId="5" state="hidden" r:id="rId3"/>
-    <sheet name="KWENTA - power" sheetId="6" r:id="rId4"/>
-    <sheet name="KWENTA - Decay" sheetId="7" r:id="rId5"/>
-    <sheet name="KWENTA - Final" sheetId="8" r:id="rId6"/>
+    <sheet name="KWENTA - power" sheetId="6" state="hidden" r:id="rId4"/>
+    <sheet name="KWENTA - Decay" sheetId="7" state="hidden" r:id="rId5"/>
+    <sheet name="KWENTA - Final" sheetId="8" state="hidden" r:id="rId6"/>
+    <sheet name="KWENTA - Epochs" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="67">
   <si>
     <t>N stake 20</t>
   </si>
@@ -217,12 +218,36 @@
   <si>
     <t>trading Rewards</t>
   </si>
+  <si>
+    <t>Epoch</t>
+  </si>
+  <si>
+    <t>Both Trade</t>
+  </si>
+  <si>
+    <t>Set reward</t>
+  </si>
+  <si>
+    <t>Staker 1 withdraws half</t>
+  </si>
+  <si>
+    <t>Staker 2 trades</t>
+  </si>
+  <si>
+    <t>Staker 2 withdraws all</t>
+  </si>
+  <si>
+    <t>Staker 2 trades and stakes</t>
+  </si>
+  <si>
+    <t>Staker 1 trades</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="11">
+  <numFmts count="14">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000000E+00"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
@@ -234,6 +259,9 @@
     <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="172" formatCode="0.000E+00"/>
     <numFmt numFmtId="173" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="177" formatCode="#,##0.000000000"/>
+    <numFmt numFmtId="190" formatCode="#,##0.0000000000000000000000"/>
+    <numFmt numFmtId="200" formatCode="0.00000000000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -259,7 +287,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -272,8 +300,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -413,12 +453,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -506,6 +594,32 @@
     <xf numFmtId="173" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="173" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="190" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="200" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="200" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4310,26 +4424,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272DD5C9-D190-4388-8820-6AF1434A50B5}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.58984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.40625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.2265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.2265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.58984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.31640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.40625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.75">
@@ -5491,4 +5606,1022 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3E162D-03F7-4BA4-B1C9-0B1FB7C23E32}">
+  <dimension ref="B1:P34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.31640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.40625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="49"/>
+    </row>
+    <row r="2" spans="2:16" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B2" s="49"/>
+      <c r="C2" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="52"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="51"/>
+      <c r="O2" s="49"/>
+    </row>
+    <row r="3" spans="2:16" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="B3" s="49"/>
+      <c r="C3" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="49">
+        <v>25</v>
+      </c>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49">
+        <v>100</v>
+      </c>
+      <c r="H3" s="49">
+        <f>86400*7</f>
+        <v>604800</v>
+      </c>
+      <c r="I3" s="49">
+        <f>+G3/H3</f>
+        <v>1.6534391534391533E-4</v>
+      </c>
+      <c r="J3" s="85">
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="85">
+        <f>1-J3</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="L3" s="49">
+        <v>0.7</v>
+      </c>
+      <c r="M3" s="49">
+        <v>0.3</v>
+      </c>
+      <c r="N3" s="54"/>
+      <c r="O3" s="49"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B4" s="49"/>
+      <c r="C4" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="49">
+        <v>50</v>
+      </c>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="50"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B5" s="49"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="49"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B7" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="60"/>
+      <c r="F7" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="L7" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" s="60"/>
+      <c r="N7" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="63" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B8" s="93">
+        <v>1</v>
+      </c>
+      <c r="C8" s="94">
+        <v>0</v>
+      </c>
+      <c r="D8" s="95" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="95"/>
+      <c r="F8" s="96" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="95">
+        <v>1E+19</v>
+      </c>
+      <c r="H8" s="97">
+        <v>0</v>
+      </c>
+      <c r="I8" s="98">
+        <f>+G8/SUM(G8:G9)</f>
+        <v>0.5</v>
+      </c>
+      <c r="J8" s="98">
+        <f>+$J$3*$I$3*I8*C10</f>
+        <v>5.7142857142857144</v>
+      </c>
+      <c r="K8" s="98">
+        <f>+((H8/1000000000000000000)^$L$3)*((G8/1000000000000000000)^$M$3)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="98">
+        <v>0</v>
+      </c>
+      <c r="M8" s="98"/>
+      <c r="N8" s="98">
+        <f>+L8+J8</f>
+        <v>5.7142857142857144</v>
+      </c>
+      <c r="O8" s="99">
+        <f>+N8</f>
+        <v>5.7142857142857144</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B9" s="100"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="95">
+        <v>1E+19</v>
+      </c>
+      <c r="H9" s="97">
+        <v>0</v>
+      </c>
+      <c r="I9" s="98">
+        <f>+G9/SUM(G8:G9)</f>
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="98">
+        <f>+$J$3*$I$3*I9*C10</f>
+        <v>5.7142857142857144</v>
+      </c>
+      <c r="K9" s="98">
+        <f>+((H9/1000000000000000000)^$L$3)*((G9/1000000000000000000)^$M$3)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="98">
+        <v>0</v>
+      </c>
+      <c r="M9" s="98"/>
+      <c r="N9" s="98">
+        <f>+L9+J9</f>
+        <v>5.7142857142857144</v>
+      </c>
+      <c r="O9" s="99">
+        <f>+N9</f>
+        <v>5.7142857142857144</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B10" s="100"/>
+      <c r="C10" s="101">
+        <v>86400</v>
+      </c>
+      <c r="D10" s="95" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="95"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="95"/>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="98"/>
+      <c r="L10" s="98"/>
+      <c r="M10" s="98"/>
+      <c r="N10" s="98"/>
+      <c r="O10" s="99"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B11" s="100"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="95"/>
+      <c r="E11" s="95"/>
+      <c r="F11" s="96" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="95">
+        <v>1E+19</v>
+      </c>
+      <c r="H11" s="97">
+        <v>2.5E+19</v>
+      </c>
+      <c r="I11" s="98">
+        <f>+G11/SUM(G11:G12)</f>
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="98">
+        <f>+$J$3*$I$3*I11*(C13-C10)</f>
+        <v>17.142857142857142</v>
+      </c>
+      <c r="K11" s="98">
+        <f>+((H11/1000000000000000000)^$L$3)*((G11/1000000000000000000)^$M$3)</f>
+        <v>18.991444823309347</v>
+      </c>
+      <c r="L11" s="98">
+        <v>0</v>
+      </c>
+      <c r="M11" s="98"/>
+      <c r="N11" s="98">
+        <f>+L11+J11</f>
+        <v>17.142857142857142</v>
+      </c>
+      <c r="O11" s="99">
+        <f>+N11+O8</f>
+        <v>22.857142857142858</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B12" s="100"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="95"/>
+      <c r="F12" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="95">
+        <v>1E+19</v>
+      </c>
+      <c r="H12" s="97">
+        <v>5E+19</v>
+      </c>
+      <c r="I12" s="98">
+        <f>+G12/SUM(G11:G12)</f>
+        <v>0.5</v>
+      </c>
+      <c r="J12" s="98">
+        <f>+$J$3*$I$3*I12*(C13-C10)</f>
+        <v>17.142857142857142</v>
+      </c>
+      <c r="K12" s="98">
+        <f>+((H12/1000000000000000000)^$L$3)*((G12/1000000000000000000)^$M$3)</f>
+        <v>30.851693136000481</v>
+      </c>
+      <c r="L12" s="98">
+        <v>0</v>
+      </c>
+      <c r="M12" s="98"/>
+      <c r="N12" s="98">
+        <f>+L12+J12</f>
+        <v>17.142857142857142</v>
+      </c>
+      <c r="O12" s="99">
+        <f>+N12+O9</f>
+        <v>22.857142857142858</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B13" s="100"/>
+      <c r="C13" s="101">
+        <f>+C10+3*86400</f>
+        <v>345600</v>
+      </c>
+      <c r="D13" s="95" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="95"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="95"/>
+      <c r="H13" s="95"/>
+      <c r="I13" s="98"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="99"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B14" s="100"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="96" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="95">
+        <f>+G11/2</f>
+        <v>5E+18</v>
+      </c>
+      <c r="H14" s="97">
+        <v>2.5E+19</v>
+      </c>
+      <c r="I14" s="98">
+        <f>+G14/SUM(G14:G15)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J14" s="98">
+        <f>+$J$3*$I$3*I14*(C16-C13)</f>
+        <v>11.428571428571429</v>
+      </c>
+      <c r="K14" s="98">
+        <f>+((H14/1000000000000000000)^$L$3)*((G14/1000000000000000000)^$M$3)</f>
+        <v>15.425846568000239</v>
+      </c>
+      <c r="L14" s="108">
+        <f>+K14/SUM(K14:K15)*$G$3*$K$3</f>
+        <v>6.6666666666666643</v>
+      </c>
+      <c r="M14" s="98"/>
+      <c r="N14" s="98">
+        <f>+L14+J14</f>
+        <v>18.095238095238095</v>
+      </c>
+      <c r="O14" s="99">
+        <f>+N14+O11</f>
+        <v>40.952380952380949</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B15" s="100"/>
+      <c r="C15" s="101"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="95">
+        <v>1E+19</v>
+      </c>
+      <c r="H15" s="97">
+        <v>5E+19</v>
+      </c>
+      <c r="I15" s="98">
+        <f>+G15/SUM(G14:G15)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J15" s="98">
+        <f>+$J$3*$I$3*I15*(C16-C13)</f>
+        <v>22.857142857142858</v>
+      </c>
+      <c r="K15" s="98">
+        <f>+((H15/1000000000000000000)^$L$3)*((G15/1000000000000000000)^$M$3)</f>
+        <v>30.851693136000481</v>
+      </c>
+      <c r="L15" s="108">
+        <f>+K15/SUM(K14:K15)*$G$3*$K$3</f>
+        <v>13.333333333333332</v>
+      </c>
+      <c r="M15" s="98"/>
+      <c r="N15" s="98">
+        <f>+L15+J15</f>
+        <v>36.19047619047619</v>
+      </c>
+      <c r="O15" s="99">
+        <f>+N15+O12</f>
+        <v>59.047619047619051</v>
+      </c>
+      <c r="P15" s="92">
+        <f>+SUM(O14:O15)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B16" s="64">
+        <v>2</v>
+      </c>
+      <c r="C16" s="87">
+        <f>7*86400</f>
+        <v>604800</v>
+      </c>
+      <c r="D16" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="65"/>
+      <c r="F16" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="65">
+        <f>+G14</f>
+        <v>5E+18</v>
+      </c>
+      <c r="H16" s="65">
+        <v>0</v>
+      </c>
+      <c r="I16" s="68">
+        <f>+G16/SUM(G16:G17)</f>
+        <v>1</v>
+      </c>
+      <c r="J16" s="68">
+        <f>+$J$3*$I$3*I16*C18</f>
+        <v>11.428571428571429</v>
+      </c>
+      <c r="K16" s="68">
+        <f t="shared" ref="K16:K17" si="0">+((H16/1000000000000000000)^$L$3)*((G16/1000000000000000000)^$M$3)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="68">
+        <v>0</v>
+      </c>
+      <c r="M16" s="68"/>
+      <c r="N16" s="68">
+        <f>+L16+J16</f>
+        <v>11.428571428571429</v>
+      </c>
+      <c r="O16" s="89">
+        <f>+N16+O14</f>
+        <v>52.38095238095238</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B17" s="64"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="65">
+        <v>0</v>
+      </c>
+      <c r="H17" s="67">
+        <v>0</v>
+      </c>
+      <c r="I17" s="68">
+        <f>+G17/SUM(G16:G17)</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="68">
+        <f>+$J$3*$I$3*I17*70</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="68">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="68">
+        <v>0</v>
+      </c>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68">
+        <f>+L17+J17</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="89">
+        <f>+N17+O15</f>
+        <v>59.047619047619051</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B18" s="64"/>
+      <c r="C18" s="87">
+        <f>+C10</f>
+        <v>86400</v>
+      </c>
+      <c r="D18" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="65"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="68"/>
+      <c r="O18" s="89"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B19" s="64"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="65">
+        <f>+G16</f>
+        <v>5E+18</v>
+      </c>
+      <c r="H19" s="65">
+        <v>0</v>
+      </c>
+      <c r="I19" s="68">
+        <f>+G19/SUM(G19:G20)</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="68">
+        <f>+$J$3*$I$3*I19*(C21-C18)</f>
+        <v>68.571428571428569</v>
+      </c>
+      <c r="K19" s="68">
+        <f t="shared" ref="K19:K20" si="1">+((H19/1000000000000000000)^$L$3)*((G19/1000000000000000000)^$M$3)</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="68">
+        <v>0</v>
+      </c>
+      <c r="M19" s="68"/>
+      <c r="N19" s="68">
+        <f>+L19+J19</f>
+        <v>68.571428571428569</v>
+      </c>
+      <c r="O19" s="89">
+        <f>+N19+O16</f>
+        <v>120.95238095238095</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B20" s="64"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="65">
+        <v>0</v>
+      </c>
+      <c r="H20" s="65">
+        <v>7E+19</v>
+      </c>
+      <c r="I20" s="68">
+        <f>+G20/SUM(G19:G20)</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="68">
+        <f>+$J$3*$I$3*I20*30</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="68">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="68">
+        <v>0</v>
+      </c>
+      <c r="M20" s="68"/>
+      <c r="N20" s="68">
+        <f>+L20+J20</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="89">
+        <f>+N20+O17</f>
+        <v>59.047619047619051</v>
+      </c>
+      <c r="P20" s="92">
+        <f>+SUM(O19:O20)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B21" s="102">
+        <v>3</v>
+      </c>
+      <c r="C21" s="103">
+        <f>+C16</f>
+        <v>604800</v>
+      </c>
+      <c r="D21" s="104" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="104"/>
+      <c r="F21" s="105"/>
+      <c r="G21" s="104"/>
+      <c r="H21" s="104"/>
+      <c r="I21" s="106"/>
+      <c r="J21" s="106"/>
+      <c r="K21" s="106"/>
+      <c r="L21" s="106"/>
+      <c r="M21" s="106"/>
+      <c r="N21" s="106"/>
+      <c r="O21" s="107"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B22" s="102"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="104">
+        <f>+G19</f>
+        <v>5E+18</v>
+      </c>
+      <c r="H22" s="104">
+        <f>+H19</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="106">
+        <f>+G22/SUM(G22:G23)</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="J22" s="106">
+        <f>+$J$3*$I$3*I22*(C25)</f>
+        <v>6.5306122448979593</v>
+      </c>
+      <c r="K22" s="106">
+        <f>+((H22/1000000000000000000)^$L$3)*((G22/1000000000000000000)^$M$3)</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="106">
+        <f>+$K$3*$I$3*K22/SUM(K22:K26)*50</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="106"/>
+      <c r="N22" s="106">
+        <f>+L22+J22</f>
+        <v>6.5306122448979593</v>
+      </c>
+      <c r="O22" s="107">
+        <f>+N22+O19</f>
+        <v>127.48299319727892</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B23" s="102"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="104"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="104">
+        <v>3E+19</v>
+      </c>
+      <c r="H23" s="104">
+        <v>9E+19</v>
+      </c>
+      <c r="I23" s="106">
+        <f>+G23/SUM(G22:G23)</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="J23" s="106">
+        <f>+$J$3*$I$3*I23*C25</f>
+        <v>39.183673469387756</v>
+      </c>
+      <c r="K23" s="106">
+        <f>+((H23/1000000000000000000)^$L$3)*((G23/1000000000000000000)^$M$3)</f>
+        <v>64.730078399237783</v>
+      </c>
+      <c r="L23" s="106">
+        <v>0</v>
+      </c>
+      <c r="M23" s="106"/>
+      <c r="N23" s="106">
+        <f>+L23+J23</f>
+        <v>39.183673469387756</v>
+      </c>
+      <c r="O23" s="107">
+        <f>+N23+O20</f>
+        <v>98.231292517006807</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B24" s="102"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="104"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="105"/>
+      <c r="G24" s="104"/>
+      <c r="H24" s="104"/>
+      <c r="I24" s="106"/>
+      <c r="J24" s="106"/>
+      <c r="K24" s="106"/>
+      <c r="L24" s="106"/>
+      <c r="M24" s="106"/>
+      <c r="N24" s="106"/>
+      <c r="O24" s="107"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B25" s="102"/>
+      <c r="C25" s="103">
+        <f>+C13</f>
+        <v>345600</v>
+      </c>
+      <c r="D25" s="104" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="104"/>
+      <c r="F25" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="104">
+        <f>+G22</f>
+        <v>5E+18</v>
+      </c>
+      <c r="H25" s="104">
+        <v>1E+20</v>
+      </c>
+      <c r="I25" s="106">
+        <f>+G25/SUM(G25:G26)</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="J25" s="106">
+        <f>+$J$3*$I$3*I25*(C27-C25)</f>
+        <v>4.8979591836734695</v>
+      </c>
+      <c r="K25" s="109">
+        <f>+((H25/1000000000000000000)^$L$3)*((G25/1000000000000000000)^$M$3)</f>
+        <v>40.709053153690434</v>
+      </c>
+      <c r="L25" s="106">
+        <f>+K25/SUM(K25:K26)*$G$3*$K$3</f>
+        <v>7.7218111632976303</v>
+      </c>
+      <c r="M25" s="106"/>
+      <c r="N25" s="106">
+        <f>+L25+J25</f>
+        <v>12.6197703469711</v>
+      </c>
+      <c r="O25" s="107">
+        <f>+N25+O22</f>
+        <v>140.10276354425002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B26" s="102"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="104"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="105" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="104">
+        <v>3E+19</v>
+      </c>
+      <c r="H26" s="104">
+        <v>9E+19</v>
+      </c>
+      <c r="I26" s="106">
+        <f>+G26/SUM(G25:G26)</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="J26" s="106">
+        <f>+$J$3*$I$3*I26*(C27-C25)</f>
+        <v>29.387755102040817</v>
+      </c>
+      <c r="K26" s="109">
+        <f>+((H26/1000000000000000000)^$L$3)*((G26/1000000000000000000)^$M$3)</f>
+        <v>64.730078399237783</v>
+      </c>
+      <c r="L26" s="106">
+        <f>+K26/SUM(K25:K26)*$G$3*$K$3</f>
+        <v>12.278188836702366</v>
+      </c>
+      <c r="M26" s="106"/>
+      <c r="N26" s="106">
+        <f>+L26+J26</f>
+        <v>41.665943938743183</v>
+      </c>
+      <c r="O26" s="107">
+        <f>+N26+O23</f>
+        <v>139.89723645574998</v>
+      </c>
+      <c r="P26" s="92">
+        <f>+SUM(O25:O26)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B27" s="72"/>
+      <c r="C27" s="88">
+        <f>+C21</f>
+        <v>604800</v>
+      </c>
+      <c r="D27" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="56"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="74"/>
+      <c r="M27" s="74"/>
+      <c r="N27" s="74"/>
+      <c r="O27" s="90"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="49"/>
+    </row>
+    <row r="29" spans="2:16" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="77"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="51"/>
+      <c r="O29" s="49"/>
+    </row>
+    <row r="30" spans="2:16" ht="15.5" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" s="111">
+        <f>+SUM(N8,N11,N14,N16,N19,N22,N25)</f>
+        <v>140.10276354425002</v>
+      </c>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="81"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="49"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="112">
+        <f>+SUM(N9,N12,N15,N17,N20,N23,N26)</f>
+        <v>139.89723645574998</v>
+      </c>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="82"/>
+      <c r="N31" s="51"/>
+      <c r="O31" s="49"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.75">
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="91">
+        <f>+SUM(G30:G31)</f>
+        <v>280</v>
+      </c>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="50"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="51"/>
+      <c r="O32" s="49"/>
+    </row>
+    <row r="34" spans="12:12" x14ac:dyDescent="0.75">
+      <c r="L34" s="110">
+        <f>+K26+K25-K14</f>
+        <v>90.013284984927978</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: added getEpochForDate function for cleaner code and fixed unit tests
</commit_message>
<xml_diff>
--- a/20210921 - Staking Rewards.xlsx
+++ b/20210921 - Staking Rewards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Documents\16slimchance16\token\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3614439B-31E7-4EC0-8DB0-5937F1CDE6EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE26B109-1E8C-461B-A196-BA1B8B2440FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67995" yWindow="-15075" windowWidth="6825" windowHeight="3915" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67485" yWindow="-15210" windowWidth="7500" windowHeight="6000" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SNX" sheetId="1" state="hidden" r:id="rId1"/>
@@ -247,7 +247,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="14">
+  <numFmts count="13">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000000E+00"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
@@ -259,9 +259,8 @@
     <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="172" formatCode="0.000E+00"/>
     <numFmt numFmtId="173" formatCode="#,##0.00000"/>
-    <numFmt numFmtId="177" formatCode="#,##0.000000000"/>
-    <numFmt numFmtId="190" formatCode="#,##0.0000000000000000000000"/>
-    <numFmt numFmtId="200" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="174" formatCode="#,##0.000000000"/>
+    <numFmt numFmtId="176" formatCode="0.00000000000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -506,7 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -615,11 +614,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="190" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="200" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="200" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -5612,7 +5610,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3E162D-03F7-4BA4-B1C9-0B1FB7C23E32}">
   <dimension ref="B1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
@@ -6039,7 +6039,7 @@
         <f>+((H14/1000000000000000000)^$L$3)*((G14/1000000000000000000)^$M$3)</f>
         <v>15.425846568000239</v>
       </c>
-      <c r="L14" s="108">
+      <c r="L14" s="98">
         <f>+K14/SUM(K14:K15)*$G$3*$K$3</f>
         <v>6.6666666666666643</v>
       </c>
@@ -6079,7 +6079,7 @@
         <f>+((H15/1000000000000000000)^$L$3)*((G15/1000000000000000000)^$M$3)</f>
         <v>30.851693136000481</v>
       </c>
-      <c r="L15" s="108">
+      <c r="L15" s="98">
         <f>+K15/SUM(K14:K15)*$G$3*$K$3</f>
         <v>13.333333333333332</v>
       </c>
@@ -6435,7 +6435,7 @@
         <f>+$J$3*$I$3*I25*(C27-C25)</f>
         <v>4.8979591836734695</v>
       </c>
-      <c r="K25" s="109">
+      <c r="K25" s="108">
         <f>+((H25/1000000000000000000)^$L$3)*((G25/1000000000000000000)^$M$3)</f>
         <v>40.709053153690434</v>
       </c>
@@ -6475,7 +6475,7 @@
         <f>+$J$3*$I$3*I26*(C27-C25)</f>
         <v>29.387755102040817</v>
       </c>
-      <c r="K26" s="109">
+      <c r="K26" s="108">
         <f>+((H26/1000000000000000000)^$L$3)*((G26/1000000000000000000)^$M$3)</f>
         <v>64.730078399237783</v>
       </c>
@@ -6560,7 +6560,7 @@
       <c r="F30" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="G30" s="111">
+      <c r="G30" s="110">
         <f>+SUM(N8,N11,N14,N16,N19,N22,N25)</f>
         <v>140.10276354425002</v>
       </c>
@@ -6581,7 +6581,7 @@
       <c r="F31" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="G31" s="112">
+      <c r="G31" s="111">
         <f>+SUM(N9,N12,N15,N17,N20,N23,N26)</f>
         <v>139.89723645574998</v>
       </c>
@@ -6616,7 +6616,7 @@
       <c r="O32" s="49"/>
     </row>
     <row r="34" spans="12:12" x14ac:dyDescent="0.75">
-      <c r="L34" s="110">
+      <c r="L34" s="109">
         <f>+K26+K25-K14</f>
         <v>90.013284984927978</v>
       </c>

</xml_diff>